<commit_message>
kati 1 njesite done
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$132</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$192</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="25">
   <si>
     <t>Nr</t>
   </si>
@@ -112,10 +112,7 @@
     <t>BODRUM</t>
   </si>
   <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>H4</t>
+    <t>KATI1</t>
   </si>
 </sst>
 </file>
@@ -605,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -667,6 +664,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -777,6 +777,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,6 +1186,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>451310</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>16719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>685801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F399456-FFFA-4806-B53B-2B24D3A1E278}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4506239" y="16005112"/>
+          <a:ext cx="859056" cy="669082"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1477,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S135"/>
+  <dimension ref="A1:K195"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:H54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A133" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="E142" sqref="C139:H174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,111 +1566,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -2139,7 +2209,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="21">
@@ -2166,7 +2236,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="14"/>
@@ -2178,7 +2248,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="19" t="s">
@@ -2201,26 +2271,11 @@
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="O35">
-        <v>1</v>
-      </c>
-      <c r="P35">
-        <v>7517924.1610000003</v>
-      </c>
-      <c r="Q35">
-        <v>4692685.9009999996</v>
-      </c>
-      <c r="R35">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="7">
+      <c r="C36" s="9">
         <v>1</v>
       </c>
       <c r="D36" s="8">
@@ -2232,32 +2287,19 @@
       <c r="F36" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="9"/>
+      <c r="H36" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="O36">
-        <v>3</v>
-      </c>
-      <c r="P36">
-        <v>7517926.7680000002</v>
-      </c>
-      <c r="Q36">
-        <v>4692678.1229999997</v>
-      </c>
-      <c r="R36">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="7">
+      <c r="C37" s="9">
         <v>3</v>
       </c>
       <c r="D37" s="8">
@@ -2269,32 +2311,17 @@
       <c r="F37" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="9"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="O37">
-        <v>4</v>
-      </c>
-      <c r="P37">
-        <v>7517929.4824999999</v>
-      </c>
-      <c r="Q37">
-        <v>4692679.0022999998</v>
-      </c>
-      <c r="R37">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="7">
+      <c r="C38" s="9">
         <v>4</v>
       </c>
       <c r="D38" s="8">
@@ -2306,32 +2333,17 @@
       <c r="F38" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H38" s="9"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="O38">
-        <v>12</v>
-      </c>
-      <c r="P38">
-        <v>7517931.1023000004</v>
-      </c>
-      <c r="Q38">
-        <v>4692674.0017999997</v>
-      </c>
-      <c r="R38">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="7">
+      <c r="C39" s="9">
         <v>12</v>
       </c>
       <c r="D39" s="8">
@@ -2343,32 +2355,17 @@
       <c r="F39" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H39" s="9"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="O39">
-        <v>56</v>
-      </c>
-      <c r="P39">
-        <v>7517948.5199999996</v>
-      </c>
-      <c r="Q39">
-        <v>4692694.1529999999</v>
-      </c>
-      <c r="R39">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="7">
+      <c r="C40" s="9">
         <v>56</v>
       </c>
       <c r="D40" s="8">
@@ -2380,32 +2377,17 @@
       <c r="F40" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="9"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="O40">
-        <v>57</v>
-      </c>
-      <c r="P40">
-        <v>7517952.9117999999</v>
-      </c>
-      <c r="Q40">
-        <v>4692681.6829000004</v>
-      </c>
-      <c r="R40">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="7">
+      <c r="C41" s="9">
         <v>57</v>
       </c>
       <c r="D41" s="8">
@@ -2417,32 +2399,17 @@
       <c r="F41" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="9"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="O41">
-        <v>122</v>
-      </c>
-      <c r="P41">
-        <v>7517949.3603999997</v>
-      </c>
-      <c r="Q41">
-        <v>4692691.7666999996</v>
-      </c>
-      <c r="R41">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="7">
+      <c r="C42" s="9">
         <v>122</v>
       </c>
       <c r="D42" s="8">
@@ -2454,32 +2421,17 @@
       <c r="F42" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="9"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="O42">
-        <v>123</v>
-      </c>
-      <c r="P42">
-        <v>7517951.3054</v>
-      </c>
-      <c r="Q42">
-        <v>4692686.2441999996</v>
-      </c>
-      <c r="R42">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="7">
+      <c r="C43" s="9">
         <v>123</v>
       </c>
       <c r="D43" s="8">
@@ -2491,32 +2443,17 @@
       <c r="F43" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="9"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="O43">
-        <v>124</v>
-      </c>
-      <c r="P43">
-        <v>7517950.0350000001</v>
-      </c>
-      <c r="Q43">
-        <v>4692680.6697000004</v>
-      </c>
-      <c r="R43">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="7">
+      <c r="C44" s="9">
         <v>124</v>
       </c>
       <c r="D44" s="8">
@@ -2528,33 +2465,18 @@
       <c r="F44" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H44" s="9"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="O44">
-        <v>125</v>
-      </c>
-      <c r="P44">
-        <v>7517948.4286000002</v>
-      </c>
-      <c r="Q44">
-        <v>4692685.2309999997</v>
-      </c>
-      <c r="R44">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="7">
+      <c r="C45" s="9">
         <v>125</v>
       </c>
       <c r="D45" s="8">
@@ -2566,33 +2488,18 @@
       <c r="F45" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G45" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H45" s="9"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="O45">
-        <v>126</v>
-      </c>
-      <c r="P45">
-        <v>7517946.4715</v>
-      </c>
-      <c r="Q45">
-        <v>4692690.7879999997</v>
-      </c>
-      <c r="R45">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="7">
+      <c r="C46" s="9">
         <v>126</v>
       </c>
       <c r="D46" s="8">
@@ -2604,31 +2511,16 @@
       <c r="F46" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G46" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="9"/>
+      <c r="G46" s="63"/>
+      <c r="H46" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="O46">
-        <v>127</v>
-      </c>
-      <c r="P46">
-        <v>7517941.8687000005</v>
-      </c>
-      <c r="Q46">
-        <v>4692689.2286999999</v>
-      </c>
-      <c r="R46">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C47" s="7">
+    </row>
+    <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C47" s="9">
         <v>127</v>
       </c>
       <c r="D47" s="8">
@@ -2640,29 +2532,14 @@
       <c r="F47" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G47" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="9"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="K47" s="1"/>
-      <c r="O47">
-        <v>128</v>
-      </c>
-      <c r="P47">
-        <v>7517941.0272000004</v>
-      </c>
-      <c r="Q47">
-        <v>4692691.6179</v>
-      </c>
-      <c r="R47">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C48" s="7">
+    </row>
+    <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C48" s="9">
         <v>128</v>
       </c>
       <c r="D48" s="8">
@@ -2674,31 +2551,16 @@
       <c r="F48" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G48" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H48" s="9"/>
+      <c r="G48" s="63"/>
+      <c r="H48" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="K48" s="1"/>
-      <c r="O48">
-        <v>129</v>
-      </c>
-      <c r="P48">
-        <v>7517926.9834000003</v>
-      </c>
-      <c r="Q48">
-        <v>4692686.8570999997</v>
-      </c>
-      <c r="R48">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="7">
+      <c r="C49" s="9">
         <v>129</v>
       </c>
       <c r="D49" s="8">
@@ -2710,33 +2572,18 @@
       <c r="F49" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G49" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H49" s="9"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="O49">
-        <v>130</v>
-      </c>
-      <c r="P49">
-        <v>7517925.7034</v>
-      </c>
-      <c r="Q49">
-        <v>4692686.4281000001</v>
-      </c>
-      <c r="R49">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="7">
+      <c r="C50" s="9">
         <v>130</v>
       </c>
       <c r="D50" s="8">
@@ -2748,33 +2595,18 @@
       <c r="F50" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G50" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H50" s="9"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="O50">
-        <v>131</v>
-      </c>
-      <c r="P50">
-        <v>7517927.4121000003</v>
-      </c>
-      <c r="Q50">
-        <v>4692681.3301999997</v>
-      </c>
-      <c r="R50">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="7">
+      <c r="C51" s="9">
         <v>131</v>
       </c>
       <c r="D51" s="8">
@@ -2786,32 +2618,17 @@
       <c r="F51" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="9"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="O51">
-        <v>132</v>
-      </c>
-      <c r="P51">
-        <v>7517928.6359000001</v>
-      </c>
-      <c r="Q51">
-        <v>4692681.7456999999</v>
-      </c>
-      <c r="R51">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="7">
+      <c r="C52" s="9">
         <v>132</v>
       </c>
       <c r="D52" s="8">
@@ -2823,32 +2640,17 @@
       <c r="F52" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G52" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H52" s="9"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="O52">
-        <v>104</v>
-      </c>
-      <c r="P52">
-        <v>7517945.1684999997</v>
-      </c>
-      <c r="Q52">
-        <v>4692693.0225999998</v>
-      </c>
-      <c r="R52">
-        <v>616.38300000000004</v>
-      </c>
-      <c r="S52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="7">
+      <c r="C53" s="9">
         <v>104</v>
       </c>
       <c r="D53" s="8">
@@ -2860,33 +2662,18 @@
       <c r="F53" s="8">
         <v>616.38300000000004</v>
       </c>
-      <c r="G53" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="9"/>
+      <c r="G53" s="63"/>
+      <c r="H53" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I53" s="11"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="O53">
-        <v>103</v>
-      </c>
-      <c r="P53">
-        <v>7517926.4434000002</v>
-      </c>
-      <c r="Q53">
-        <v>4692686.6742000002</v>
-      </c>
-      <c r="R53">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="7">
+      <c r="C54" s="9">
         <v>103</v>
       </c>
       <c r="D54" s="8">
@@ -2898,15 +2685,15 @@
       <c r="F54" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H54" s="9"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="I54" s="11"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="11"/>
@@ -2919,7 +2706,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="11"/>
@@ -2932,7 +2719,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="11"/>
@@ -2945,7 +2732,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="60" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="11"/>
@@ -2958,146 +2745,146 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
       <c r="I61" s="11"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-    </row>
-    <row r="63" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="42" t="s">
+      <c r="E64" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="43"/>
-      <c r="G64" s="44"/>
-      <c r="H64" s="45" t="s">
+      <c r="F64" s="44"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I64" s="46"/>
-      <c r="J64" s="49"/>
-      <c r="K64" s="50"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="51"/>
     </row>
     <row r="65" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="56" t="s">
+      <c r="A65" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="57"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="59">
+      <c r="B65" s="58"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="60">
         <v>140</v>
       </c>
-      <c r="F65" s="60"/>
-      <c r="G65" s="61"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="52"/>
+      <c r="F65" s="61"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="41"/>
+      <c r="A66" s="42"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
     </row>
     <row r="67" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="41"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="41"/>
+      <c r="A67" s="42"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="42"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="42"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="40" t="s">
+      <c r="A68" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="40"/>
-      <c r="H68" s="40"/>
-      <c r="I68" s="40"/>
-      <c r="J68" s="40"/>
-      <c r="K68" s="40"/>
+      <c r="B68" s="41"/>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="41"/>
+      <c r="G68" s="41"/>
+      <c r="H68" s="41"/>
+      <c r="I68" s="41"/>
+      <c r="J68" s="41"/>
+      <c r="K68" s="41"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="40"/>
-      <c r="B69" s="40"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="40"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
-      <c r="J69" s="40"/>
-      <c r="K69" s="40"/>
+      <c r="A69" s="41"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="41"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="41"/>
+      <c r="K69" s="41"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
-      <c r="B70" s="40"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="40"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
-      <c r="J70" s="40"/>
-      <c r="K70" s="40"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="40"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="40"/>
-      <c r="F71" s="40"/>
-      <c r="G71" s="40"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="40"/>
-      <c r="J71" s="40"/>
-      <c r="K71" s="40"/>
+      <c r="A70" s="41"/>
+      <c r="B70" s="41"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="41"/>
+      <c r="I70" s="41"/>
+      <c r="J70" s="41"/>
+      <c r="K70" s="41"/>
+    </row>
+    <row r="71" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="41"/>
+      <c r="B71" s="41"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="41"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="41"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="41"/>
+      <c r="K71" s="41"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
@@ -3115,22 +2902,22 @@
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="27" t="s">
+      <c r="C73" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D73" s="27" t="s">
+      <c r="D73" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E73" s="27" t="s">
+      <c r="E73" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F73" s="27" t="s">
+      <c r="F73" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="G73" s="27" t="s">
+      <c r="G73" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H73" s="28" t="s">
+      <c r="H73" s="29" t="s">
         <v>3</v>
       </c>
       <c r="I73" s="11"/>
@@ -3143,19 +2930,19 @@
       <c r="C74" s="19">
         <v>101</v>
       </c>
-      <c r="D74" s="29">
+      <c r="D74" s="30">
         <v>7517952.1813000003</v>
       </c>
-      <c r="E74" s="29">
+      <c r="E74" s="30">
         <v>4692679.7653000001</v>
       </c>
-      <c r="F74" s="53">
+      <c r="F74" s="54">
         <v>616.38300000000004</v>
       </c>
-      <c r="G74" s="53" t="s">
+      <c r="G74" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="H74" s="29" t="s">
+      <c r="H74" s="30" t="s">
         <v>21</v>
       </c>
       <c r="I74" s="11"/>
@@ -3168,15 +2955,15 @@
       <c r="C75" s="19">
         <v>2</v>
       </c>
-      <c r="D75" s="29">
+      <c r="D75" s="30">
         <v>7517924.0990000004</v>
       </c>
-      <c r="E75" s="29">
+      <c r="E75" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="29" t="s">
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I75" s="11"/>
@@ -3189,15 +2976,15 @@
       <c r="C76" s="19">
         <v>5</v>
       </c>
-      <c r="D76" s="29">
+      <c r="D76" s="30">
         <v>7517928.4419999998</v>
       </c>
-      <c r="E76" s="29">
+      <c r="E76" s="30">
         <v>4692673.07</v>
       </c>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="29" t="s">
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I76" s="11"/>
@@ -3210,15 +2997,15 @@
       <c r="C77" s="19">
         <v>6</v>
       </c>
-      <c r="D77" s="29">
+      <c r="D77" s="30">
         <v>7517929.8169999998</v>
       </c>
-      <c r="E77" s="29">
+      <c r="E77" s="30">
         <v>4692673.5259999996</v>
       </c>
-      <c r="F77" s="54"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="29" t="s">
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I77" s="11"/>
@@ -3231,15 +3018,15 @@
       <c r="C78" s="19">
         <v>7</v>
       </c>
-      <c r="D78" s="29">
+      <c r="D78" s="30">
         <v>7517929.96</v>
       </c>
-      <c r="E78" s="29">
+      <c r="E78" s="30">
         <v>4692673.2819999997</v>
       </c>
-      <c r="F78" s="54"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="29" t="s">
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I78" s="11"/>
@@ -3252,15 +3039,15 @@
       <c r="C79" s="19">
         <v>8</v>
       </c>
-      <c r="D79" s="29">
+      <c r="D79" s="30">
         <v>7517930.2989999996</v>
       </c>
-      <c r="E79" s="29">
+      <c r="E79" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F79" s="54"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="29" t="s">
+      <c r="F79" s="55"/>
+      <c r="G79" s="55"/>
+      <c r="H79" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I79" s="11"/>
@@ -3273,15 +3060,15 @@
       <c r="C80" s="19">
         <v>9</v>
       </c>
-      <c r="D80" s="29">
+      <c r="D80" s="30">
         <v>7517930.7450000001</v>
       </c>
-      <c r="E80" s="29">
+      <c r="E80" s="30">
         <v>4692672.7690000003</v>
       </c>
-      <c r="F80" s="54"/>
-      <c r="G80" s="54"/>
-      <c r="H80" s="29" t="s">
+      <c r="F80" s="55"/>
+      <c r="G80" s="55"/>
+      <c r="H80" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I80" s="11"/>
@@ -3294,15 +3081,15 @@
       <c r="C81" s="19">
         <v>10</v>
       </c>
-      <c r="D81" s="29">
+      <c r="D81" s="30">
         <v>7517931.2220000001</v>
       </c>
-      <c r="E81" s="29">
+      <c r="E81" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F81" s="54"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="29" t="s">
+      <c r="F81" s="55"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I81" s="11"/>
@@ -3315,15 +3102,15 @@
       <c r="C82" s="19">
         <v>11</v>
       </c>
-      <c r="D82" s="29">
+      <c r="D82" s="30">
         <v>7517931.6050000004</v>
       </c>
-      <c r="E82" s="29">
+      <c r="E82" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F82" s="54"/>
-      <c r="G82" s="54"/>
-      <c r="H82" s="29" t="s">
+      <c r="F82" s="55"/>
+      <c r="G82" s="55"/>
+      <c r="H82" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I82" s="11"/>
@@ -3336,15 +3123,15 @@
       <c r="C83" s="19">
         <v>34</v>
       </c>
-      <c r="D83" s="29">
+      <c r="D83" s="30">
         <v>7517953.7189999996</v>
       </c>
-      <c r="E83" s="29">
+      <c r="E83" s="30">
         <v>4692687.3470000001</v>
       </c>
-      <c r="F83" s="54"/>
-      <c r="G83" s="54"/>
-      <c r="H83" s="29" t="s">
+      <c r="F83" s="55"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I83" s="11"/>
@@ -3357,15 +3144,15 @@
       <c r="C84" s="19">
         <v>35</v>
       </c>
-      <c r="D84" s="29">
+      <c r="D84" s="30">
         <v>7517955.8949999996</v>
       </c>
-      <c r="E84" s="29">
+      <c r="E84" s="30">
         <v>4692681.023</v>
       </c>
-      <c r="F84" s="54"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="29" t="s">
+      <c r="F84" s="55"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I84" s="11"/>
@@ -3378,15 +3165,15 @@
       <c r="C85" s="19">
         <v>58</v>
       </c>
-      <c r="D85" s="29">
+      <c r="D85" s="30">
         <v>7517951.3300000001</v>
       </c>
-      <c r="E85" s="29">
+      <c r="E85" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F85" s="54"/>
-      <c r="G85" s="54"/>
-      <c r="H85" s="29" t="s">
+      <c r="F85" s="55"/>
+      <c r="G85" s="55"/>
+      <c r="H85" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I85" s="11"/>
@@ -3399,15 +3186,15 @@
       <c r="C86" s="19">
         <v>59</v>
       </c>
-      <c r="D86" s="29">
+      <c r="D86" s="30">
         <v>7517951.9790000003</v>
       </c>
-      <c r="E86" s="29">
+      <c r="E86" s="30">
         <v>4692687.1399999997</v>
       </c>
-      <c r="F86" s="54"/>
-      <c r="G86" s="54"/>
-      <c r="H86" s="29" t="s">
+      <c r="F86" s="55"/>
+      <c r="G86" s="55"/>
+      <c r="H86" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I86" s="11"/>
@@ -3420,15 +3207,15 @@
       <c r="C87" s="19">
         <v>60</v>
       </c>
-      <c r="D87" s="29">
+      <c r="D87" s="30">
         <v>7517952.0760000004</v>
       </c>
-      <c r="E87" s="29">
+      <c r="E87" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F87" s="54"/>
-      <c r="G87" s="54"/>
-      <c r="H87" s="29" t="s">
+      <c r="F87" s="55"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I87" s="11"/>
@@ -3441,15 +3228,15 @@
       <c r="C88" s="19">
         <v>61</v>
       </c>
-      <c r="D88" s="29">
+      <c r="D88" s="30">
         <v>7517950.1849999996</v>
       </c>
-      <c r="E88" s="29">
+      <c r="E88" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
-      <c r="H88" s="29" t="s">
+      <c r="F88" s="55"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I88" s="11"/>
@@ -3462,15 +3249,15 @@
       <c r="C89" s="19">
         <v>62</v>
       </c>
-      <c r="D89" s="29">
+      <c r="D89" s="30">
         <v>7517949.5559999999</v>
       </c>
-      <c r="E89" s="29">
+      <c r="E89" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F89" s="54"/>
-      <c r="G89" s="54"/>
-      <c r="H89" s="29" t="s">
+      <c r="F89" s="55"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I89" s="11"/>
@@ -3483,15 +3270,15 @@
       <c r="C90" s="19">
         <v>63</v>
       </c>
-      <c r="D90" s="29">
+      <c r="D90" s="30">
         <v>7517948.5300000003</v>
       </c>
-      <c r="E90" s="29">
+      <c r="E90" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F90" s="54"/>
-      <c r="G90" s="54"/>
-      <c r="H90" s="29" t="s">
+      <c r="F90" s="55"/>
+      <c r="G90" s="55"/>
+      <c r="H90" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I90" s="11"/>
@@ -3504,15 +3291,15 @@
       <c r="C91" s="19">
         <v>105</v>
       </c>
-      <c r="D91" s="29">
+      <c r="D91" s="30">
         <v>7517927.7654999997</v>
       </c>
-      <c r="E91" s="29">
+      <c r="E91" s="30">
         <v>4692687.1445000004</v>
       </c>
-      <c r="F91" s="54"/>
-      <c r="G91" s="54"/>
-      <c r="H91" s="29" t="s">
+      <c r="F91" s="55"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I91" s="11"/>
@@ -3525,15 +3312,15 @@
       <c r="C92" s="19">
         <v>106</v>
       </c>
-      <c r="D92" s="29">
+      <c r="D92" s="30">
         <v>7517928.7182999998</v>
       </c>
-      <c r="E92" s="29">
+      <c r="E92" s="30">
         <v>4692684.3208999997</v>
       </c>
-      <c r="F92" s="54"/>
-      <c r="G92" s="54"/>
-      <c r="H92" s="29" t="s">
+      <c r="F92" s="55"/>
+      <c r="G92" s="55"/>
+      <c r="H92" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I92" s="11"/>
@@ -3546,15 +3333,15 @@
       <c r="C93" s="19">
         <v>107</v>
       </c>
-      <c r="D93" s="29">
+      <c r="D93" s="30">
         <v>7517927.7045</v>
       </c>
-      <c r="E93" s="29">
+      <c r="E93" s="30">
         <v>4692683.9785000002</v>
       </c>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="29" t="s">
+      <c r="F93" s="55"/>
+      <c r="G93" s="55"/>
+      <c r="H93" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I93" s="11"/>
@@ -3567,15 +3354,15 @@
       <c r="C94" s="19">
         <v>108</v>
       </c>
-      <c r="D94" s="29">
+      <c r="D94" s="30">
         <v>7517925.0517999995</v>
       </c>
-      <c r="E94" s="29">
+      <c r="E94" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F94" s="54"/>
-      <c r="G94" s="54"/>
-      <c r="H94" s="29" t="s">
+      <c r="F94" s="55"/>
+      <c r="G94" s="55"/>
+      <c r="H94" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I94" s="11"/>
@@ -3588,15 +3375,15 @@
       <c r="C95" s="19">
         <v>109</v>
       </c>
-      <c r="D95" s="29">
+      <c r="D95" s="30">
         <v>7517926.6694</v>
       </c>
-      <c r="E95" s="29">
+      <c r="E95" s="30">
         <v>4692678.2884999998</v>
       </c>
-      <c r="F95" s="54"/>
-      <c r="G95" s="54"/>
-      <c r="H95" s="29" t="s">
+      <c r="F95" s="55"/>
+      <c r="G95" s="55"/>
+      <c r="H95" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I95" s="11"/>
@@ -3609,15 +3396,15 @@
       <c r="C96" s="19">
         <v>110</v>
       </c>
-      <c r="D96" s="29">
+      <c r="D96" s="30">
         <v>7517928.0525000002</v>
       </c>
-      <c r="E96" s="29">
+      <c r="E96" s="30">
         <v>4692678.7551999995</v>
       </c>
-      <c r="F96" s="54"/>
-      <c r="G96" s="54"/>
-      <c r="H96" s="29" t="s">
+      <c r="F96" s="55"/>
+      <c r="G96" s="55"/>
+      <c r="H96" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I96" s="11"/>
@@ -3630,15 +3417,15 @@
       <c r="C97" s="19">
         <v>111</v>
       </c>
-      <c r="D97" s="29">
+      <c r="D97" s="30">
         <v>7517929.3223999999</v>
       </c>
-      <c r="E97" s="29">
+      <c r="E97" s="30">
         <v>4692679.1836999999</v>
       </c>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="29" t="s">
+      <c r="F97" s="55"/>
+      <c r="G97" s="55"/>
+      <c r="H97" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I97" s="11"/>
@@ -3651,15 +3438,15 @@
       <c r="C98" s="19">
         <v>112</v>
       </c>
-      <c r="D98" s="29">
+      <c r="D98" s="30">
         <v>7517950.6852000002</v>
       </c>
-      <c r="E98" s="29">
+      <c r="E98" s="30">
         <v>4692679.26</v>
       </c>
-      <c r="F98" s="54"/>
-      <c r="G98" s="54"/>
-      <c r="H98" s="29" t="s">
+      <c r="F98" s="55"/>
+      <c r="G98" s="55"/>
+      <c r="H98" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I98" s="11"/>
@@ -3672,15 +3459,15 @@
       <c r="C99" s="19">
         <v>113</v>
       </c>
-      <c r="D99" s="29">
+      <c r="D99" s="30">
         <v>7517953.2906999998</v>
       </c>
-      <c r="E99" s="29">
+      <c r="E99" s="30">
         <v>4692680.1398</v>
       </c>
-      <c r="F99" s="54"/>
-      <c r="G99" s="54"/>
-      <c r="H99" s="29" t="s">
+      <c r="F99" s="55"/>
+      <c r="G99" s="55"/>
+      <c r="H99" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I99" s="11"/>
@@ -3693,15 +3480,15 @@
       <c r="C100" s="19">
         <v>114</v>
       </c>
-      <c r="D100" s="29">
+      <c r="D100" s="30">
         <v>7517948.5182999996</v>
       </c>
-      <c r="E100" s="29">
+      <c r="E100" s="30">
         <v>4692685.5575999999</v>
       </c>
-      <c r="F100" s="54"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="29" t="s">
+      <c r="F100" s="55"/>
+      <c r="G100" s="55"/>
+      <c r="H100" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I100" s="11"/>
@@ -3714,15 +3501,15 @@
       <c r="C101" s="19">
         <v>115</v>
       </c>
-      <c r="D101" s="29">
+      <c r="D101" s="30">
         <v>7517951.1238000002</v>
       </c>
-      <c r="E101" s="29">
+      <c r="E101" s="30">
         <v>4692686.4374000002</v>
       </c>
-      <c r="F101" s="54"/>
-      <c r="G101" s="54"/>
-      <c r="H101" s="29" t="s">
+      <c r="F101" s="55"/>
+      <c r="G101" s="55"/>
+      <c r="H101" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I101" s="11"/>
@@ -3735,15 +3522,15 @@
       <c r="C102" s="19">
         <v>116</v>
       </c>
-      <c r="D102" s="29">
+      <c r="D102" s="30">
         <v>7517946.1694999998</v>
       </c>
-      <c r="E102" s="29">
+      <c r="E102" s="30">
         <v>4692690.9013999999</v>
       </c>
-      <c r="F102" s="54"/>
-      <c r="G102" s="54"/>
-      <c r="H102" s="29" t="s">
+      <c r="F102" s="55"/>
+      <c r="G102" s="55"/>
+      <c r="H102" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I102" s="11"/>
@@ -3756,15 +3543,15 @@
       <c r="C103" s="19">
         <v>117</v>
       </c>
-      <c r="D103" s="29">
+      <c r="D103" s="30">
         <v>7517945.4238999998</v>
       </c>
-      <c r="E103" s="29">
+      <c r="E103" s="30">
         <v>4692693.1089000003</v>
       </c>
-      <c r="F103" s="54"/>
-      <c r="G103" s="54"/>
-      <c r="H103" s="29" t="s">
+      <c r="F103" s="55"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I103" s="11"/>
@@ -3777,15 +3564,15 @@
       <c r="C104" s="19">
         <v>118</v>
       </c>
-      <c r="D104" s="29">
+      <c r="D104" s="30">
         <v>7517941.9455000004</v>
       </c>
-      <c r="E104" s="29">
+      <c r="E104" s="30">
         <v>4692689.4746000003</v>
       </c>
-      <c r="F104" s="54"/>
-      <c r="G104" s="54"/>
-      <c r="H104" s="29" t="s">
+      <c r="F104" s="55"/>
+      <c r="G104" s="55"/>
+      <c r="H104" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I104" s="11"/>
@@ -3798,15 +3585,15 @@
       <c r="C105" s="19">
         <v>119</v>
       </c>
-      <c r="D105" s="29">
+      <c r="D105" s="30">
         <v>7517936.9005000005</v>
       </c>
-      <c r="E105" s="29">
+      <c r="E105" s="30">
         <v>4692687.7706000004</v>
       </c>
-      <c r="F105" s="54"/>
-      <c r="G105" s="54"/>
-      <c r="H105" s="29" t="s">
+      <c r="F105" s="55"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I105" s="11"/>
@@ -3819,15 +3606,15 @@
       <c r="C106" s="19">
         <v>120</v>
       </c>
-      <c r="D106" s="29">
+      <c r="D106" s="30">
         <v>7517936.1549000004</v>
       </c>
-      <c r="E106" s="29">
+      <c r="E106" s="30">
         <v>4692689.9780000001</v>
       </c>
-      <c r="F106" s="54"/>
-      <c r="G106" s="54"/>
-      <c r="H106" s="29" t="s">
+      <c r="F106" s="55"/>
+      <c r="G106" s="55"/>
+      <c r="H106" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I106" s="11"/>
@@ -3840,15 +3627,15 @@
       <c r="C107" s="19">
         <v>14</v>
       </c>
-      <c r="D107" s="29">
+      <c r="D107" s="30">
         <v>7517930.4069999997</v>
       </c>
-      <c r="E107" s="29">
+      <c r="E107" s="30">
         <v>4692671.8150000004</v>
       </c>
-      <c r="F107" s="55"/>
-      <c r="G107" s="55"/>
-      <c r="H107" s="29" t="s">
+      <c r="F107" s="56"/>
+      <c r="G107" s="56"/>
+      <c r="H107" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I107" s="11"/>
@@ -3861,8 +3648,8 @@
       <c r="C108" s="14"/>
       <c r="D108" s="17"/>
       <c r="E108" s="17"/>
-      <c r="F108" s="26"/>
-      <c r="G108" s="26"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
       <c r="H108" s="13"/>
       <c r="I108" s="11"/>
       <c r="J108" s="1"/>
@@ -3871,12 +3658,12 @@
     <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="14"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="26"/>
-      <c r="H109" s="13"/>
+      <c r="C109" s="64"/>
+      <c r="D109" s="64"/>
+      <c r="E109" s="64"/>
+      <c r="F109" s="64"/>
+      <c r="G109" s="64"/>
+      <c r="H109" s="65"/>
       <c r="I109" s="11"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
@@ -3887,8 +3674,8 @@
       <c r="C110" s="14"/>
       <c r="D110" s="17"/>
       <c r="E110" s="17"/>
-      <c r="F110" s="26"/>
-      <c r="G110" s="26"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
       <c r="H110" s="13"/>
       <c r="I110" s="11"/>
       <c r="J110" s="1"/>
@@ -3900,8 +3687,8 @@
       <c r="C111" s="14"/>
       <c r="D111" s="17"/>
       <c r="E111" s="17"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="26"/>
+      <c r="F111" s="27"/>
+      <c r="G111" s="27"/>
       <c r="H111" s="13"/>
       <c r="I111" s="11"/>
       <c r="J111" s="1"/>
@@ -3913,8 +3700,8 @@
       <c r="C112" s="14"/>
       <c r="D112" s="17"/>
       <c r="E112" s="17"/>
-      <c r="F112" s="26"/>
-      <c r="G112" s="26"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="27"/>
       <c r="H112" s="13"/>
       <c r="I112" s="11"/>
       <c r="J112" s="1"/>
@@ -3926,8 +3713,8 @@
       <c r="C113" s="14"/>
       <c r="D113" s="17"/>
       <c r="E113" s="17"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
       <c r="H113" s="13"/>
       <c r="I113" s="11"/>
       <c r="J113" s="1"/>
@@ -3939,8 +3726,8 @@
       <c r="C114" s="14"/>
       <c r="D114" s="17"/>
       <c r="E114" s="17"/>
-      <c r="F114" s="26"/>
-      <c r="G114" s="26"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="27"/>
       <c r="H114" s="13"/>
       <c r="I114" s="11"/>
       <c r="J114" s="1"/>
@@ -3967,7 +3754,7 @@
       <c r="E116" s="18"/>
       <c r="F116" s="18"/>
       <c r="G116" s="18"/>
-      <c r="H116" s="25"/>
+      <c r="H116" s="26"/>
       <c r="I116" s="12"/>
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
@@ -3978,8 +3765,8 @@
       <c r="C117" s="14"/>
       <c r="D117" s="17"/>
       <c r="E117" s="17"/>
-      <c r="F117" s="26"/>
-      <c r="G117" s="26"/>
+      <c r="F117" s="27"/>
+      <c r="G117" s="27"/>
       <c r="H117" s="13"/>
       <c r="I117" s="12"/>
       <c r="J117" s="1"/>
@@ -3991,8 +3778,8 @@
       <c r="C118" s="14"/>
       <c r="D118" s="17"/>
       <c r="E118" s="17"/>
-      <c r="F118" s="26"/>
-      <c r="G118" s="26"/>
+      <c r="F118" s="27"/>
+      <c r="G118" s="27"/>
       <c r="H118" s="13"/>
       <c r="I118" s="12"/>
       <c r="J118" s="1"/>
@@ -4004,8 +3791,8 @@
       <c r="C119" s="14"/>
       <c r="D119" s="17"/>
       <c r="E119" s="17"/>
-      <c r="F119" s="26"/>
-      <c r="G119" s="26"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="27"/>
       <c r="H119" s="13"/>
       <c r="I119" s="12"/>
       <c r="J119" s="1"/>
@@ -4014,26 +3801,28 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="14"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="26"/>
-      <c r="G120" s="26"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="12"/>
+      <c r="C120" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="31"/>
+      <c r="E120" s="31"/>
+      <c r="F120" s="31"/>
+      <c r="G120" s="31"/>
+      <c r="H120" s="31"/>
+      <c r="I120" s="31"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="14"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="26"/>
-      <c r="G121" s="26"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="12"/>
+      <c r="C121" s="31"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="31"/>
+      <c r="F121" s="31"/>
+      <c r="G121" s="31"/>
+      <c r="H121" s="31"/>
+      <c r="I121" s="31"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
@@ -4043,8 +3832,8 @@
       <c r="C122" s="14"/>
       <c r="D122" s="17"/>
       <c r="E122" s="17"/>
-      <c r="F122" s="26"/>
-      <c r="G122" s="26"/>
+      <c r="F122" s="27"/>
+      <c r="G122" s="27"/>
       <c r="H122" s="13"/>
       <c r="I122" s="12"/>
       <c r="J122" s="1"/>
@@ -4056,8 +3845,8 @@
       <c r="C123" s="14"/>
       <c r="D123" s="17"/>
       <c r="E123" s="17"/>
-      <c r="F123" s="26"/>
-      <c r="G123" s="26"/>
+      <c r="F123" s="27"/>
+      <c r="G123" s="27"/>
       <c r="H123" s="13"/>
       <c r="I123" s="12"/>
       <c r="J123" s="1"/>
@@ -4069,10 +3858,10 @@
       <c r="C124" s="14"/>
       <c r="D124" s="17"/>
       <c r="E124" s="17"/>
-      <c r="F124" s="26"/>
-      <c r="G124" s="26"/>
+      <c r="F124" s="27"/>
+      <c r="G124" s="27"/>
       <c r="H124" s="13"/>
-      <c r="I124" s="12"/>
+      <c r="I124" s="25"/>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
     </row>
@@ -4082,110 +3871,1243 @@
       <c r="C125" s="14"/>
       <c r="D125" s="17"/>
       <c r="E125" s="17"/>
-      <c r="F125" s="26"/>
-      <c r="G125" s="26"/>
+      <c r="F125" s="27"/>
+      <c r="G125" s="27"/>
       <c r="H125" s="13"/>
-      <c r="I125" s="12"/>
+      <c r="I125" s="25"/>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
     </row>
     <row r="126" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
-      <c r="B126" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="30"/>
-      <c r="F126" s="30"/>
-      <c r="G126" s="30"/>
-      <c r="H126" s="30"/>
-      <c r="I126" s="12"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="27"/>
+      <c r="G126" s="27"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="25"/>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
     </row>
-    <row r="127" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="1"/>
-      <c r="B127" s="30"/>
-      <c r="C127" s="30"/>
-      <c r="D127" s="30"/>
-      <c r="E127" s="30"/>
-      <c r="F127" s="30"/>
-      <c r="G127" s="30"/>
-      <c r="H127" s="30"/>
-      <c r="I127" s="12"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="27"/>
+      <c r="G127" s="27"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="25"/>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
     </row>
     <row r="128" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="14"/>
-      <c r="D128" s="17"/>
-      <c r="E128" s="17"/>
-      <c r="F128" s="26"/>
-      <c r="G128" s="26"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="11"/>
-      <c r="J128" s="1"/>
-      <c r="K128" s="1"/>
+      <c r="A128" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" s="44"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I128" s="47"/>
+      <c r="J128" s="50"/>
+      <c r="K128" s="51"/>
     </row>
     <row r="129" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K129" s="1"/>
-    </row>
-    <row r="130" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="A129" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B129" s="58"/>
+      <c r="C129" s="58"/>
+      <c r="D129" s="59"/>
+      <c r="E129" s="60">
+        <v>140</v>
+      </c>
+      <c r="F129" s="61"/>
+      <c r="G129" s="62"/>
+      <c r="H129" s="48"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="52"/>
+      <c r="K129" s="53"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A132" s="42"/>
+      <c r="B132" s="42"/>
+      <c r="C132" s="42"/>
+      <c r="D132" s="42"/>
+      <c r="E132" s="42"/>
+      <c r="F132" s="42"/>
+      <c r="G132" s="42"/>
+      <c r="H132" s="42"/>
+      <c r="I132" s="42"/>
+      <c r="J132" s="42"/>
+      <c r="K132" s="42"/>
+    </row>
+    <row r="133" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="42"/>
+      <c r="B133" s="42"/>
+      <c r="C133" s="42"/>
+      <c r="D133" s="42"/>
+      <c r="E133" s="42"/>
+      <c r="F133" s="42"/>
+      <c r="G133" s="42"/>
+      <c r="H133" s="42"/>
+      <c r="I133" s="42"/>
+      <c r="J133" s="42"/>
+      <c r="K133" s="42"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A134" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B134" s="41"/>
+      <c r="C134" s="41"/>
+      <c r="D134" s="41"/>
+      <c r="E134" s="41"/>
+      <c r="F134" s="41"/>
+      <c r="G134" s="41"/>
+      <c r="H134" s="41"/>
+      <c r="I134" s="41"/>
+      <c r="J134" s="41"/>
+      <c r="K134" s="41"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A135" s="41"/>
+      <c r="B135" s="41"/>
+      <c r="C135" s="41"/>
+      <c r="D135" s="41"/>
+      <c r="E135" s="41"/>
+      <c r="F135" s="41"/>
+      <c r="G135" s="41"/>
+      <c r="H135" s="41"/>
+      <c r="I135" s="41"/>
+      <c r="J135" s="41"/>
+      <c r="K135" s="41"/>
+    </row>
+    <row r="136" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="41"/>
+      <c r="B136" s="41"/>
+      <c r="C136" s="41"/>
+      <c r="D136" s="41"/>
+      <c r="E136" s="41"/>
+      <c r="F136" s="41"/>
+      <c r="G136" s="41"/>
+      <c r="H136" s="41"/>
+      <c r="I136" s="41"/>
+      <c r="J136" s="41"/>
+      <c r="K136" s="41"/>
+    </row>
+    <row r="137" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="41"/>
+      <c r="B137" s="41"/>
+      <c r="C137" s="41"/>
+      <c r="D137" s="41"/>
+      <c r="E137" s="41"/>
+      <c r="F137" s="41"/>
+      <c r="G137" s="41"/>
+      <c r="H137" s="41"/>
+      <c r="I137" s="41"/>
+      <c r="J137" s="41"/>
+      <c r="K137" s="41"/>
+    </row>
+    <row r="138" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="25"/>
+      <c r="D138" s="25"/>
+      <c r="E138" s="25"/>
+      <c r="F138" s="25"/>
+      <c r="G138" s="25"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="25"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+    </row>
+    <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D139" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E139" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F139" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G139" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H139" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I139" s="25"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+    </row>
+    <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="19">
+        <v>2</v>
+      </c>
+      <c r="D140" s="30">
+        <v>7517924.0990000004</v>
+      </c>
+      <c r="E140" s="30">
+        <v>4692685.9060000004</v>
+      </c>
+      <c r="F140" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G140" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H140" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I140" s="25"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+    </row>
+    <row r="141" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="19">
+        <v>5</v>
+      </c>
+      <c r="D141" s="30">
+        <v>7517928.4419999998</v>
+      </c>
+      <c r="E141" s="30">
+        <v>4692673.07</v>
+      </c>
+      <c r="F141" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G141" s="55"/>
+      <c r="H141" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I141" s="25"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+    </row>
+    <row r="142" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="19">
+        <v>6</v>
+      </c>
+      <c r="D142" s="30">
+        <v>7517929.8169999998</v>
+      </c>
+      <c r="E142" s="30">
+        <v>4692673.5259999996</v>
+      </c>
+      <c r="F142" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G142" s="55"/>
+      <c r="H142" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I142" s="25"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+    </row>
+    <row r="143" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="19">
+        <v>7</v>
+      </c>
+      <c r="D143" s="30">
+        <v>7517929.96</v>
+      </c>
+      <c r="E143" s="30">
+        <v>4692673.2819999997</v>
+      </c>
+      <c r="F143" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G143" s="55"/>
+      <c r="H143" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I143" s="25"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+    </row>
+    <row r="144" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="19">
+        <v>8</v>
+      </c>
+      <c r="D144" s="30">
+        <v>7517930.2989999996</v>
+      </c>
+      <c r="E144" s="30">
+        <v>4692672.9689999996</v>
+      </c>
+      <c r="F144" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G144" s="55"/>
+      <c r="H144" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I144" s="25"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+    </row>
+    <row r="145" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="19">
+        <v>9</v>
+      </c>
+      <c r="D145" s="30">
+        <v>7517930.7450000001</v>
+      </c>
+      <c r="E145" s="30">
+        <v>4692672.7690000003</v>
+      </c>
+      <c r="F145" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G145" s="55"/>
+      <c r="H145" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I145" s="25"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+    </row>
+    <row r="146" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="19">
+        <v>10</v>
+      </c>
+      <c r="D146" s="30">
+        <v>7517931.2220000001</v>
+      </c>
+      <c r="E146" s="30">
+        <v>4692672.7319999998</v>
+      </c>
+      <c r="F146" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G146" s="55"/>
+      <c r="H146" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I146" s="25"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+    </row>
+    <row r="147" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="19">
+        <v>11</v>
+      </c>
+      <c r="D147" s="30">
+        <v>7517931.6050000004</v>
+      </c>
+      <c r="E147" s="30">
+        <v>4692672.7970000003</v>
+      </c>
+      <c r="F147" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G147" s="55"/>
+      <c r="H147" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I147" s="25"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+    </row>
+    <row r="148" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="19">
+        <v>34</v>
+      </c>
+      <c r="D148" s="30">
+        <v>7517945.9960000003</v>
+      </c>
+      <c r="E148" s="30">
+        <v>4692677.4869999997</v>
+      </c>
+      <c r="F148" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G148" s="55"/>
+      <c r="H148" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I148" s="25"/>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+    </row>
+    <row r="149" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="19">
+        <v>35</v>
+      </c>
+      <c r="D149" s="30">
+        <v>7517945.9700999996</v>
+      </c>
+      <c r="E149" s="30">
+        <v>4692677.5620999997</v>
+      </c>
+      <c r="F149" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G149" s="55"/>
+      <c r="H149" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I149" s="25"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+    </row>
+    <row r="150" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="19">
+        <v>41</v>
+      </c>
+      <c r="D150" s="30">
+        <v>7517950.0548999999</v>
+      </c>
+      <c r="E150" s="30">
+        <v>4692678.9175000004</v>
+      </c>
+      <c r="F150" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G150" s="55"/>
+      <c r="H150" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I150" s="25"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+    </row>
+    <row r="151" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="19">
+        <v>42</v>
+      </c>
+      <c r="D151" s="30">
+        <v>7517950.4249999998</v>
+      </c>
+      <c r="E151" s="30">
+        <v>4692677.8820000002</v>
+      </c>
+      <c r="F151" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G151" s="55"/>
+      <c r="H151" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I151" s="25"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+    </row>
+    <row r="152" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="19">
+        <v>43</v>
+      </c>
+      <c r="D152" s="30">
+        <v>7517953.7850000001</v>
+      </c>
+      <c r="E152" s="30">
+        <v>4692679.0829999996</v>
+      </c>
+      <c r="F152" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G152" s="55"/>
+      <c r="H152" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I152" s="25"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+    </row>
+    <row r="153" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="19">
+        <v>58</v>
+      </c>
+      <c r="D153" s="30">
+        <v>7517951.3300000001</v>
+      </c>
+      <c r="E153" s="30">
+        <v>4692686.5060000001</v>
+      </c>
+      <c r="F153" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G153" s="55"/>
+      <c r="H153" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I153" s="25"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+    </row>
+    <row r="154" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="19">
+        <v>59</v>
+      </c>
+      <c r="D154" s="30">
+        <v>7517951.9790000003</v>
+      </c>
+      <c r="E154" s="30">
+        <v>4692687.1399999997</v>
+      </c>
+      <c r="F154" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G154" s="55"/>
+      <c r="H154" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I154" s="25"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+    </row>
+    <row r="155" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="19">
+        <v>60</v>
+      </c>
+      <c r="D155" s="30">
+        <v>7517952.0760000004</v>
+      </c>
+      <c r="E155" s="30">
+        <v>4692688.1239999998</v>
+      </c>
+      <c r="F155" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G155" s="55"/>
+      <c r="H155" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I155" s="25"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+    </row>
+    <row r="156" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="19">
+        <v>61</v>
+      </c>
+      <c r="D156" s="30">
+        <v>7517950.1849999996</v>
+      </c>
+      <c r="E156" s="30">
+        <v>4692693.4919999996</v>
+      </c>
+      <c r="F156" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G156" s="55"/>
+      <c r="H156" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I156" s="25"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+    </row>
+    <row r="157" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="19">
+        <v>62</v>
+      </c>
+      <c r="D157" s="30">
+        <v>7517949.5559999999</v>
+      </c>
+      <c r="E157" s="30">
+        <v>4692694.1169999996</v>
+      </c>
+      <c r="F157" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G157" s="55"/>
+      <c r="H157" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I157" s="25"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+    </row>
+    <row r="158" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="19">
+        <v>63</v>
+      </c>
+      <c r="D158" s="30">
+        <v>7517948.5300000003</v>
+      </c>
+      <c r="E158" s="30">
+        <v>4692694.1579999998</v>
+      </c>
+      <c r="F158" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G158" s="55"/>
+      <c r="H158" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I158" s="25"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+    </row>
+    <row r="159" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="19">
+        <v>102</v>
+      </c>
+      <c r="D159" s="30">
+        <v>7517936.4840000002</v>
+      </c>
+      <c r="E159" s="30">
+        <v>4692674.3847000003</v>
+      </c>
+      <c r="F159" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G159" s="55"/>
+      <c r="H159" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I159" s="25"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+    </row>
+    <row r="160" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="19">
+        <v>103</v>
+      </c>
+      <c r="D160" s="30">
+        <v>7517936.5029999996</v>
+      </c>
+      <c r="E160" s="30">
+        <v>4692674.3310000002</v>
+      </c>
+      <c r="F160" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G160" s="55"/>
+      <c r="H160" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I160" s="25"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+    </row>
+    <row r="161" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="19">
+        <v>104</v>
+      </c>
+      <c r="D161" s="30">
+        <v>7517941.3384999996</v>
+      </c>
+      <c r="E161" s="30">
+        <v>4692675.6413000003</v>
+      </c>
+      <c r="F161" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G161" s="55"/>
+      <c r="H161" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I161" s="25"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+    </row>
+    <row r="162" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="19">
+        <v>135</v>
+      </c>
+      <c r="D162" s="30">
+        <v>7517926.9230000004</v>
+      </c>
+      <c r="E162" s="30">
+        <v>4692677.5713999998</v>
+      </c>
+      <c r="F162" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G162" s="55"/>
+      <c r="H162" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I162" s="25"/>
+      <c r="J162" s="1"/>
+      <c r="K162" s="1"/>
+    </row>
+    <row r="163" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="19">
+        <v>136</v>
+      </c>
+      <c r="D163" s="30">
+        <v>7517929.3389999997</v>
+      </c>
+      <c r="E163" s="30">
+        <v>4692678.3875000002</v>
+      </c>
+      <c r="F163" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G163" s="55"/>
+      <c r="H163" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I163" s="25"/>
+      <c r="J163" s="1"/>
+      <c r="K163" s="1"/>
+    </row>
+    <row r="164" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="19">
+        <v>137</v>
+      </c>
+      <c r="D164" s="30">
+        <v>7517927.5005999999</v>
+      </c>
+      <c r="E164" s="30">
+        <v>4692683.8356999997</v>
+      </c>
+      <c r="F164" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G164" s="55"/>
+      <c r="H164" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I164" s="25"/>
+      <c r="J164" s="1"/>
+      <c r="K164" s="1"/>
+    </row>
+    <row r="165" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="19">
+        <v>138</v>
+      </c>
+      <c r="D165" s="30">
+        <v>7517928.7559000002</v>
+      </c>
+      <c r="E165" s="30">
+        <v>4692684.2597000003</v>
+      </c>
+      <c r="F165" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G165" s="55"/>
+      <c r="H165" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I165" s="25"/>
+      <c r="J165" s="1"/>
+      <c r="K165" s="1"/>
+    </row>
+    <row r="166" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="19">
+        <v>139</v>
+      </c>
+      <c r="D166" s="30">
+        <v>7517927.7807999998</v>
+      </c>
+      <c r="E166" s="30">
+        <v>4692687.1496000001</v>
+      </c>
+      <c r="F166" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G166" s="55"/>
+      <c r="H166" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I166" s="25"/>
+      <c r="J166" s="1"/>
+      <c r="K166" s="1"/>
+    </row>
+    <row r="167" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="19">
+        <v>140</v>
+      </c>
+      <c r="D167" s="30">
+        <v>7517941.0358999996</v>
+      </c>
+      <c r="E167" s="30">
+        <v>4692691.6266999999</v>
+      </c>
+      <c r="F167" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G167" s="55"/>
+      <c r="H167" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I167" s="25"/>
+      <c r="J167" s="1"/>
+      <c r="K167" s="1"/>
+    </row>
+    <row r="168" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="19">
+        <v>141</v>
+      </c>
+      <c r="D168" s="30">
+        <v>7517941.8782000002</v>
+      </c>
+      <c r="E168" s="30">
+        <v>4692689.2351000002</v>
+      </c>
+      <c r="F168" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G168" s="55"/>
+      <c r="H168" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I168" s="25"/>
+      <c r="J168" s="1"/>
+      <c r="K168" s="1"/>
+    </row>
+    <row r="169" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="19">
+        <v>142</v>
+      </c>
+      <c r="D169" s="30">
+        <v>7517946.1831</v>
+      </c>
+      <c r="E169" s="30">
+        <v>4692690.6902999999</v>
+      </c>
+      <c r="F169" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G169" s="55"/>
+      <c r="H169" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I169" s="25"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
+    </row>
+    <row r="170" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="19">
+        <v>143</v>
+      </c>
+      <c r="D170" s="30">
+        <v>7517945.3410999998</v>
+      </c>
+      <c r="E170" s="30">
+        <v>4692693.0809000004</v>
+      </c>
+      <c r="F170" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G170" s="55"/>
+      <c r="H170" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I170" s="12"/>
+      <c r="J170" s="1"/>
+      <c r="K170" s="1"/>
+    </row>
+    <row r="171" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="19">
+        <v>144</v>
+      </c>
+      <c r="D171" s="30">
+        <v>7517947.9436999997</v>
+      </c>
+      <c r="E171" s="30">
+        <v>4692685.3624999998</v>
+      </c>
+      <c r="F171" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G171" s="55"/>
+      <c r="H171" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I171" s="12"/>
+      <c r="J171" s="1"/>
+      <c r="K171" s="1"/>
+    </row>
+    <row r="172" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A172" s="1"/>
+      <c r="C172" s="19">
+        <v>145</v>
+      </c>
+      <c r="D172" s="30">
+        <v>7517949.3491000002</v>
+      </c>
+      <c r="E172" s="30">
+        <v>4692681.1283999998</v>
+      </c>
+      <c r="F172" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G172" s="55"/>
+      <c r="H172" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I172" s="12"/>
+      <c r="J172" s="1"/>
+      <c r="K172" s="1"/>
+    </row>
+    <row r="173" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A173" s="1"/>
+      <c r="C173" s="19">
+        <v>146</v>
+      </c>
+      <c r="D173" s="30">
+        <v>7517952.7259999998</v>
+      </c>
+      <c r="E173" s="30">
+        <v>4692682.3354000002</v>
+      </c>
+      <c r="F173" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G173" s="55"/>
+      <c r="H173" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I173" s="12"/>
+      <c r="J173" s="1"/>
+      <c r="K173" s="1"/>
+    </row>
+    <row r="174" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="19">
+        <v>101</v>
+      </c>
+      <c r="D174" s="30">
+        <v>7517952.4309</v>
+      </c>
+      <c r="E174" s="30">
+        <v>4692678.5990000004</v>
+      </c>
+      <c r="F174" s="19">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G174" s="56"/>
+      <c r="H174" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I174" s="11"/>
+      <c r="J174" s="1"/>
+      <c r="K174" s="1"/>
+    </row>
+    <row r="175" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="14"/>
+      <c r="D175" s="17"/>
+      <c r="E175" s="17"/>
+      <c r="F175" s="27"/>
+      <c r="G175" s="18"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="25"/>
+      <c r="J175" s="1"/>
+      <c r="K175" s="1"/>
+    </row>
+    <row r="176" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="14"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="17"/>
+      <c r="F176" s="27"/>
+      <c r="G176" s="27"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="25"/>
+      <c r="J176" s="1"/>
+      <c r="K176" s="1"/>
+    </row>
+    <row r="177" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="14"/>
+      <c r="D177" s="17"/>
+      <c r="E177" s="17"/>
+      <c r="F177" s="27"/>
+      <c r="G177" s="27"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="25"/>
+      <c r="J177" s="1"/>
+      <c r="K177" s="1"/>
+    </row>
+    <row r="178" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="14"/>
+      <c r="D178" s="17"/>
+      <c r="E178" s="17"/>
+      <c r="F178" s="27"/>
+      <c r="G178" s="27"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="25"/>
+      <c r="J178" s="1"/>
+      <c r="K178" s="1"/>
+    </row>
+    <row r="179" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="14"/>
+      <c r="D179" s="17"/>
+      <c r="E179" s="17"/>
+      <c r="F179" s="27"/>
+      <c r="G179" s="27"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="25"/>
+      <c r="J179" s="1"/>
+      <c r="K179" s="1"/>
+    </row>
+    <row r="180" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="17"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="27"/>
+      <c r="G180" s="27"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="25"/>
+      <c r="J180" s="1"/>
+      <c r="K180" s="1"/>
+    </row>
+    <row r="181" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="14"/>
+      <c r="D181" s="17"/>
+      <c r="E181" s="17"/>
+      <c r="F181" s="27"/>
+      <c r="G181" s="27"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="25"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+    </row>
+    <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="14"/>
+      <c r="D182" s="17"/>
+      <c r="E182" s="17"/>
+      <c r="F182" s="27"/>
+      <c r="G182" s="27"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="25"/>
+      <c r="J182" s="1"/>
+      <c r="K182" s="1"/>
+    </row>
+    <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="14"/>
+      <c r="D183" s="17"/>
+      <c r="E183" s="17"/>
+      <c r="F183" s="27"/>
+      <c r="G183" s="27"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="25"/>
+      <c r="J183" s="1"/>
+      <c r="K183" s="1"/>
+    </row>
+    <row r="184" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="14"/>
+      <c r="D184" s="17"/>
+      <c r="E184" s="17"/>
+      <c r="F184" s="27"/>
+      <c r="G184" s="27"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="25"/>
+      <c r="J184" s="1"/>
+      <c r="K184" s="1"/>
+    </row>
+    <row r="185" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="14"/>
+      <c r="D185" s="17"/>
+      <c r="E185" s="17"/>
+      <c r="F185" s="27"/>
+      <c r="G185" s="27"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="25"/>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+    </row>
+    <row r="186" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="14"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="27"/>
+      <c r="G186" s="27"/>
+      <c r="H186" s="13"/>
+      <c r="I186" s="25"/>
+      <c r="J186" s="1"/>
+      <c r="K186" s="1"/>
+    </row>
+    <row r="187" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="14"/>
+      <c r="D187" s="17"/>
+      <c r="E187" s="17"/>
+      <c r="F187" s="27"/>
+      <c r="G187" s="27"/>
+      <c r="H187" s="13"/>
+      <c r="I187" s="25"/>
+      <c r="J187" s="1"/>
+      <c r="K187" s="1"/>
+    </row>
+    <row r="188" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="14"/>
+      <c r="D188" s="17"/>
+      <c r="E188" s="17"/>
+      <c r="F188" s="27"/>
+      <c r="G188" s="27"/>
+      <c r="H188" s="13"/>
+      <c r="I188" s="25"/>
+      <c r="J188" s="1"/>
+      <c r="K188" s="1"/>
+    </row>
+    <row r="189" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K189" s="1"/>
+    </row>
+    <row r="190" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="42" t="s">
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="3"/>
+      <c r="E190" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F130" s="43"/>
-      <c r="G130" s="44"/>
-      <c r="H130" s="45" t="s">
+      <c r="F190" s="44"/>
+      <c r="G190" s="45"/>
+      <c r="H190" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I130" s="46"/>
-      <c r="J130" s="49"/>
-      <c r="K130" s="50"/>
-    </row>
-    <row r="131" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="56" t="s">
+      <c r="I190" s="47"/>
+      <c r="J190" s="50"/>
+      <c r="K190" s="51"/>
+    </row>
+    <row r="191" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A191" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B131" s="57"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="58"/>
-      <c r="E131" s="59">
+      <c r="B191" s="58"/>
+      <c r="C191" s="58"/>
+      <c r="D191" s="59"/>
+      <c r="E191" s="60">
         <v>140</v>
       </c>
-      <c r="F131" s="60"/>
-      <c r="G131" s="61"/>
-      <c r="H131" s="47"/>
-      <c r="I131" s="48"/>
-      <c r="J131" s="51"/>
-      <c r="K131" s="52"/>
-    </row>
-    <row r="133" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K133" s="1"/>
-    </row>
-    <row r="134" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K134" s="1"/>
-    </row>
-    <row r="135" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K135" s="1"/>
+      <c r="F191" s="61"/>
+      <c r="G191" s="62"/>
+      <c r="H191" s="48"/>
+      <c r="I191" s="49"/>
+      <c r="J191" s="52"/>
+      <c r="K191" s="53"/>
+    </row>
+    <row r="193" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K193" s="1"/>
+    </row>
+    <row r="194" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K194" s="1"/>
+    </row>
+    <row r="195" spans="11:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K195" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="H130:I131"/>
-    <mergeCell ref="E130:G130"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="E131:G131"/>
-    <mergeCell ref="J130:K131"/>
-    <mergeCell ref="B126:H127"/>
+  <mergeCells count="28">
+    <mergeCell ref="A134:K137"/>
+    <mergeCell ref="G140:G174"/>
+    <mergeCell ref="H128:I129"/>
+    <mergeCell ref="J128:K129"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="E129:G129"/>
+    <mergeCell ref="A132:K133"/>
+    <mergeCell ref="H190:I191"/>
+    <mergeCell ref="E190:G190"/>
+    <mergeCell ref="A191:D191"/>
+    <mergeCell ref="E191:G191"/>
+    <mergeCell ref="J190:K191"/>
+    <mergeCell ref="C120:I121"/>
     <mergeCell ref="C7:I9"/>
     <mergeCell ref="A3:K6"/>
     <mergeCell ref="A1:K2"/>
@@ -4199,6 +5121,8 @@
     <mergeCell ref="E65:G65"/>
     <mergeCell ref="A66:K67"/>
     <mergeCell ref="A68:K71"/>
+    <mergeCell ref="G36:G54"/>
+    <mergeCell ref="E128:G128"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
permirsim i perdheses njesite
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="26">
   <si>
     <t>Nr</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Hyrje</t>
   </si>
   <si>
-    <t>Htrje</t>
-  </si>
-  <si>
     <t>Përdhesa</t>
   </si>
   <si>
@@ -119,12 +116,6 @@
   </si>
   <si>
     <t>KATI3</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>H4</t>
   </si>
 </sst>
 </file>
@@ -645,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -768,6 +759,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,35 +789,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -873,6 +852,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,13 +879,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2808,10 +2802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S317"/>
+  <dimension ref="A1:K317"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="H52" sqref="C35:H55"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A260" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="D84" sqref="C76:H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,110 +2821,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
       <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3470,7 +3464,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="21">
@@ -3497,7 +3491,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="14"/>
@@ -3509,7 +3503,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="44" t="s">
@@ -3533,7 +3527,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="9">
@@ -3548,31 +3542,16 @@
       <c r="F36" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G36" s="85" t="s">
-        <v>23</v>
+      <c r="G36" s="47" t="s">
+        <v>22</v>
       </c>
       <c r="H36" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="O36">
-        <v>1</v>
-      </c>
-      <c r="P36">
-        <v>7517924.1610000003</v>
-      </c>
-      <c r="Q36">
-        <v>4692685.9009999996</v>
-      </c>
-      <c r="R36">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="9">
@@ -3587,29 +3566,14 @@
       <c r="F37" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G37" s="85"/>
+      <c r="G37" s="47"/>
       <c r="H37" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="O37">
-        <v>3</v>
-      </c>
-      <c r="P37">
-        <v>7517926.7680000002</v>
-      </c>
-      <c r="Q37">
-        <v>4692678.1229999997</v>
-      </c>
-      <c r="R37">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="9">
@@ -3624,29 +3588,14 @@
       <c r="F38" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G38" s="85"/>
+      <c r="G38" s="47"/>
       <c r="H38" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="O38">
-        <v>4</v>
-      </c>
-      <c r="P38">
-        <v>7517929.4824999999</v>
-      </c>
-      <c r="Q38">
-        <v>4692679.0022999998</v>
-      </c>
-      <c r="R38">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="9">
@@ -3661,29 +3610,14 @@
       <c r="F39" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G39" s="85"/>
+      <c r="G39" s="47"/>
       <c r="H39" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="O39">
-        <v>12</v>
-      </c>
-      <c r="P39">
-        <v>7517931.1023000004</v>
-      </c>
-      <c r="Q39">
-        <v>4692674.0017999997</v>
-      </c>
-      <c r="R39">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="9">
@@ -3698,29 +3632,14 @@
       <c r="F40" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G40" s="85"/>
+      <c r="G40" s="47"/>
       <c r="H40" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="O40">
-        <v>56</v>
-      </c>
-      <c r="P40">
-        <v>7517948.5199999996</v>
-      </c>
-      <c r="Q40">
-        <v>4692694.1529999999</v>
-      </c>
-      <c r="R40">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="9">
@@ -3735,29 +3654,14 @@
       <c r="F41" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G41" s="85"/>
+      <c r="G41" s="47"/>
       <c r="H41" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="O41">
-        <v>57</v>
-      </c>
-      <c r="P41">
-        <v>7517952.9117999999</v>
-      </c>
-      <c r="Q41">
-        <v>4692681.6829000004</v>
-      </c>
-      <c r="R41">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="9">
@@ -3772,29 +3676,14 @@
       <c r="F42" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G42" s="85"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="O42">
-        <v>122</v>
-      </c>
-      <c r="P42">
-        <v>7517949.3603999997</v>
-      </c>
-      <c r="Q42">
-        <v>4692691.7666999996</v>
-      </c>
-      <c r="R42">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="9">
@@ -3809,29 +3698,14 @@
       <c r="F43" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G43" s="85"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="O43">
-        <v>123</v>
-      </c>
-      <c r="P43">
-        <v>7517951.3173000002</v>
-      </c>
-      <c r="Q43">
-        <v>4692686.2103000004</v>
-      </c>
-      <c r="R43">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="9">
@@ -3846,30 +3720,15 @@
       <c r="F44" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G44" s="85"/>
+      <c r="G44" s="47"/>
       <c r="H44" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="O44">
-        <v>124</v>
-      </c>
-      <c r="P44">
-        <v>7517950.0350000001</v>
-      </c>
-      <c r="Q44">
-        <v>4692680.6697000004</v>
-      </c>
-      <c r="R44">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="9">
@@ -3884,30 +3743,15 @@
       <c r="F45" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G45" s="85"/>
+      <c r="G45" s="47"/>
       <c r="H45" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="O45">
-        <v>125</v>
-      </c>
-      <c r="P45">
-        <v>7517948.4406000003</v>
-      </c>
-      <c r="Q45">
-        <v>4692685.1972000003</v>
-      </c>
-      <c r="R45">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="9">
@@ -3922,30 +3766,15 @@
       <c r="F46" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G46" s="85"/>
+      <c r="G46" s="47"/>
       <c r="H46" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="O46">
-        <v>126</v>
-      </c>
-      <c r="P46">
-        <v>7517946.4715</v>
-      </c>
-      <c r="Q46">
-        <v>4692690.7879999997</v>
-      </c>
-      <c r="R46">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C47" s="9">
         <v>127</v>
       </c>
@@ -3958,28 +3787,13 @@
       <c r="F47" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G47" s="85"/>
+      <c r="G47" s="47"/>
       <c r="H47" s="30" t="s">
         <v>8</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="O47">
-        <v>127</v>
-      </c>
-      <c r="P47">
-        <v>7517942.0581</v>
-      </c>
-      <c r="Q47">
-        <v>4692689.2928999998</v>
-      </c>
-      <c r="R47">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C48" s="9">
         <v>128</v>
       </c>
@@ -3992,28 +3806,13 @@
       <c r="F48" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G48" s="85"/>
+      <c r="G48" s="47"/>
       <c r="H48" s="30" t="s">
         <v>8</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="O48">
-        <v>128</v>
-      </c>
-      <c r="P48">
-        <v>7517941.2176000001</v>
-      </c>
-      <c r="Q48">
-        <v>4692691.6792000001</v>
-      </c>
-      <c r="R48">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="9">
@@ -4028,30 +3827,15 @@
       <c r="F49" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G49" s="85"/>
+      <c r="G49" s="47"/>
       <c r="H49" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="O49">
-        <v>129</v>
-      </c>
-      <c r="P49">
-        <v>7517926.9426999995</v>
-      </c>
-      <c r="Q49">
-        <v>4692686.8432999998</v>
-      </c>
-      <c r="R49">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="9">
@@ -4066,30 +3850,15 @@
       <c r="F50" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G50" s="85"/>
+      <c r="G50" s="47"/>
       <c r="H50" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
-      <c r="O50">
-        <v>130</v>
-      </c>
-      <c r="P50">
-        <v>7517924.6376999998</v>
-      </c>
-      <c r="Q50">
-        <v>4692684.4787999997</v>
-      </c>
-      <c r="R50">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="9">
@@ -4104,29 +3873,14 @@
       <c r="F51" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G51" s="85"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="O51">
-        <v>131</v>
-      </c>
-      <c r="P51">
-        <v>7517927.4254000001</v>
-      </c>
-      <c r="Q51">
-        <v>4692681.2265999997</v>
-      </c>
-      <c r="R51">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="9">
@@ -4141,29 +3895,14 @@
       <c r="F52" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G52" s="85"/>
+      <c r="G52" s="47"/>
       <c r="H52" s="30" t="s">
         <v>8</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="O52">
-        <v>132</v>
-      </c>
-      <c r="P52">
-        <v>7517928.6299000001</v>
-      </c>
-      <c r="Q52">
-        <v>4692681.6346000005</v>
-      </c>
-      <c r="R52">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="9">
@@ -4178,30 +3917,15 @@
       <c r="F53" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G53" s="85"/>
+      <c r="G53" s="47"/>
       <c r="H53" s="30" t="s">
         <v>8</v>
       </c>
       <c r="I53" s="11"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="O53">
-        <v>133</v>
-      </c>
-      <c r="P53">
-        <v>7517945.6312999995</v>
-      </c>
-      <c r="Q53">
-        <v>4692693.1743999999</v>
-      </c>
-      <c r="R53">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S53" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="9">
@@ -4216,30 +3940,15 @@
       <c r="F54" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G54" s="85"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I54" s="11"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="O54">
-        <v>104</v>
-      </c>
-      <c r="P54">
-        <v>7517945.1684999997</v>
-      </c>
-      <c r="Q54">
-        <v>4692693.0225999998</v>
-      </c>
-      <c r="R54">
-        <v>616.38300000000004</v>
-      </c>
-      <c r="S54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="9">
@@ -4254,30 +3963,15 @@
       <c r="F55" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G55" s="85"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="9" t="s">
         <v>20</v>
       </c>
       <c r="I55" s="11"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="O55">
-        <v>103</v>
-      </c>
-      <c r="P55">
-        <v>7517926.4434000002</v>
-      </c>
-      <c r="Q55">
-        <v>4692686.6742000002</v>
-      </c>
-      <c r="R55">
-        <v>611.86699999999996</v>
-      </c>
-      <c r="S55" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="11"/>
@@ -4290,7 +3984,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="11"/>
@@ -4303,7 +3997,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="60" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="11"/>
@@ -4316,179 +4010,179 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="57" t="s">
+      <c r="B61" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="57"/>
-      <c r="H61" s="57"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
       <c r="I61" s="11"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B62" s="57"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-    </row>
-    <row r="63" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="59"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="64" t="s">
+      <c r="E64" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="65"/>
-      <c r="G64" s="66"/>
-      <c r="H64" s="67" t="s">
+      <c r="F64" s="61"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I64" s="68"/>
-      <c r="J64" s="71"/>
-      <c r="K64" s="72"/>
+      <c r="I64" s="64"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="68"/>
     </row>
     <row r="65" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="75" t="s">
+      <c r="A65" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="78">
+      <c r="B65" s="72"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="74">
         <v>140</v>
       </c>
-      <c r="F65" s="79"/>
-      <c r="G65" s="80"/>
-      <c r="H65" s="69"/>
-      <c r="I65" s="70"/>
-      <c r="J65" s="73"/>
-      <c r="K65" s="74"/>
+      <c r="F65" s="75"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="66"/>
+      <c r="J65" s="69"/>
+      <c r="K65" s="70"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="46"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="46"/>
+      <c r="A66" s="48"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="48"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="48"/>
+      <c r="J66" s="48"/>
+      <c r="K66" s="48"/>
     </row>
     <row r="67" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="46"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="46"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
-      <c r="H67" s="46"/>
-      <c r="I67" s="46"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="46"/>
+      <c r="A67" s="48"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="48"/>
+      <c r="K67" s="48"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="47" t="s">
+      <c r="A68" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-      <c r="K68" s="47"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="47"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="47"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="49"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-      <c r="K70" s="47"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="49"/>
     </row>
     <row r="71" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="47"/>
-      <c r="B71" s="47"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="47"/>
+      <c r="A71" s="49"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="49"/>
+      <c r="D71" s="49"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="49"/>
+      <c r="G71" s="49"/>
+      <c r="H71" s="49"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="49"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="49"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="49"/>
-      <c r="H72" s="49"/>
-      <c r="I72" s="50"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="52"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="52"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="55"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
     <row r="74" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="55"/>
+      <c r="C74" s="77"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="78"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="78"/>
       <c r="I74" s="56"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
@@ -4503,22 +4197,22 @@
     <row r="76" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="28" t="s">
+      <c r="C76" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D76" s="28" t="s">
+      <c r="D76" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E76" s="28" t="s">
+      <c r="E76" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F76" s="28" t="s">
+      <c r="F76" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G76" s="28" t="s">
+      <c r="G76" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H76" s="29" t="s">
+      <c r="H76" s="30" t="s">
         <v>3</v>
       </c>
       <c r="I76" s="11"/>
@@ -4528,23 +4222,23 @@
     <row r="77" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="19">
-        <v>101</v>
+      <c r="C77" s="46">
+        <v>14</v>
       </c>
       <c r="D77" s="30">
-        <v>7517952.1813000003</v>
+        <v>7517930.4069999997</v>
       </c>
       <c r="E77" s="30">
-        <v>4692679.7653000001</v>
-      </c>
-      <c r="F77" s="61">
+        <v>4692671.8150000004</v>
+      </c>
+      <c r="F77" s="79">
         <v>616.38300000000004</v>
       </c>
-      <c r="G77" s="61" t="s">
-        <v>22</v>
+      <c r="G77" s="79" t="s">
+        <v>21</v>
       </c>
       <c r="H77" s="30" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="1"/>
@@ -4553,17 +4247,17 @@
     <row r="78" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="19">
-        <v>2</v>
+      <c r="C78" s="46">
+        <v>15</v>
       </c>
       <c r="D78" s="30">
-        <v>7517924.0990000004</v>
+        <v>7517928.9910000004</v>
       </c>
       <c r="E78" s="30">
-        <v>4692685.9060000004</v>
-      </c>
-      <c r="F78" s="62"/>
-      <c r="G78" s="62"/>
+        <v>4692671.3689999999</v>
+      </c>
+      <c r="F78" s="80"/>
+      <c r="G78" s="80"/>
       <c r="H78" s="30" t="s">
         <v>8</v>
       </c>
@@ -4574,17 +4268,17 @@
     <row r="79" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="19">
-        <v>5</v>
+      <c r="C79" s="46">
+        <v>2</v>
       </c>
       <c r="D79" s="30">
-        <v>7517928.4419999998</v>
+        <v>7517924.0990000004</v>
       </c>
       <c r="E79" s="30">
-        <v>4692673.07</v>
-      </c>
-      <c r="F79" s="62"/>
-      <c r="G79" s="62"/>
+        <v>4692685.9060000004</v>
+      </c>
+      <c r="F79" s="80"/>
+      <c r="G79" s="80"/>
       <c r="H79" s="30" t="s">
         <v>8</v>
       </c>
@@ -4595,17 +4289,17 @@
     <row r="80" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="19">
-        <v>6</v>
+      <c r="C80" s="46">
+        <v>5</v>
       </c>
       <c r="D80" s="30">
-        <v>7517929.8169999998</v>
+        <v>7517928.4419999998</v>
       </c>
       <c r="E80" s="30">
-        <v>4692673.5259999996</v>
-      </c>
-      <c r="F80" s="62"/>
-      <c r="G80" s="62"/>
+        <v>4692673.07</v>
+      </c>
+      <c r="F80" s="80"/>
+      <c r="G80" s="80"/>
       <c r="H80" s="30" t="s">
         <v>8</v>
       </c>
@@ -4616,17 +4310,17 @@
     <row r="81" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="19">
-        <v>7</v>
+      <c r="C81" s="46">
+        <v>6</v>
       </c>
       <c r="D81" s="30">
-        <v>7517929.96</v>
+        <v>7517929.8169999998</v>
       </c>
       <c r="E81" s="30">
-        <v>4692673.2819999997</v>
-      </c>
-      <c r="F81" s="62"/>
-      <c r="G81" s="62"/>
+        <v>4692673.5259999996</v>
+      </c>
+      <c r="F81" s="80"/>
+      <c r="G81" s="80"/>
       <c r="H81" s="30" t="s">
         <v>8</v>
       </c>
@@ -4637,17 +4331,17 @@
     <row r="82" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="19">
-        <v>8</v>
+      <c r="C82" s="46">
+        <v>7</v>
       </c>
       <c r="D82" s="30">
-        <v>7517930.2989999996</v>
+        <v>7517929.96</v>
       </c>
       <c r="E82" s="30">
-        <v>4692672.9689999996</v>
-      </c>
-      <c r="F82" s="62"/>
-      <c r="G82" s="62"/>
+        <v>4692673.2819999997</v>
+      </c>
+      <c r="F82" s="80"/>
+      <c r="G82" s="80"/>
       <c r="H82" s="30" t="s">
         <v>8</v>
       </c>
@@ -4658,17 +4352,17 @@
     <row r="83" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="19">
-        <v>9</v>
+      <c r="C83" s="46">
+        <v>8</v>
       </c>
       <c r="D83" s="30">
-        <v>7517930.7450000001</v>
+        <v>7517930.2989999996</v>
       </c>
       <c r="E83" s="30">
-        <v>4692672.7690000003</v>
-      </c>
-      <c r="F83" s="62"/>
-      <c r="G83" s="62"/>
+        <v>4692672.9689999996</v>
+      </c>
+      <c r="F83" s="80"/>
+      <c r="G83" s="80"/>
       <c r="H83" s="30" t="s">
         <v>8</v>
       </c>
@@ -4679,17 +4373,17 @@
     <row r="84" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="19">
-        <v>10</v>
+      <c r="C84" s="46">
+        <v>9</v>
       </c>
       <c r="D84" s="30">
-        <v>7517931.2220000001</v>
+        <v>7517930.7450000001</v>
       </c>
       <c r="E84" s="30">
-        <v>4692672.7319999998</v>
-      </c>
-      <c r="F84" s="62"/>
-      <c r="G84" s="62"/>
+        <v>4692672.7690000003</v>
+      </c>
+      <c r="F84" s="80"/>
+      <c r="G84" s="80"/>
       <c r="H84" s="30" t="s">
         <v>8</v>
       </c>
@@ -4700,17 +4394,17 @@
     <row r="85" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="19">
-        <v>11</v>
+      <c r="C85" s="46">
+        <v>10</v>
       </c>
       <c r="D85" s="30">
-        <v>7517931.6050000004</v>
+        <v>7517931.2220000001</v>
       </c>
       <c r="E85" s="30">
-        <v>4692672.7970000003</v>
-      </c>
-      <c r="F85" s="62"/>
-      <c r="G85" s="62"/>
+        <v>4692672.7319999998</v>
+      </c>
+      <c r="F85" s="80"/>
+      <c r="G85" s="80"/>
       <c r="H85" s="30" t="s">
         <v>8</v>
       </c>
@@ -4721,17 +4415,17 @@
     <row r="86" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="19">
-        <v>34</v>
+      <c r="C86" s="46">
+        <v>11</v>
       </c>
       <c r="D86" s="30">
-        <v>7517953.7189999996</v>
+        <v>7517931.6050000004</v>
       </c>
       <c r="E86" s="30">
-        <v>4692687.3470000001</v>
-      </c>
-      <c r="F86" s="62"/>
-      <c r="G86" s="62"/>
+        <v>4692672.7970000003</v>
+      </c>
+      <c r="F86" s="80"/>
+      <c r="G86" s="80"/>
       <c r="H86" s="30" t="s">
         <v>8</v>
       </c>
@@ -4742,17 +4436,17 @@
     <row r="87" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="19">
-        <v>35</v>
+      <c r="C87" s="46">
+        <v>34</v>
       </c>
       <c r="D87" s="30">
-        <v>7517955.8949999996</v>
+        <v>7517953.7189999996</v>
       </c>
       <c r="E87" s="30">
-        <v>4692681.023</v>
-      </c>
-      <c r="F87" s="62"/>
-      <c r="G87" s="62"/>
+        <v>4692687.3470000001</v>
+      </c>
+      <c r="F87" s="80"/>
+      <c r="G87" s="80"/>
       <c r="H87" s="30" t="s">
         <v>8</v>
       </c>
@@ -4763,17 +4457,17 @@
     <row r="88" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="19">
-        <v>58</v>
+      <c r="C88" s="46">
+        <v>35</v>
       </c>
       <c r="D88" s="30">
-        <v>7517951.3300000001</v>
+        <v>7517955.8949999996</v>
       </c>
       <c r="E88" s="30">
-        <v>4692686.5060000001</v>
-      </c>
-      <c r="F88" s="62"/>
-      <c r="G88" s="62"/>
+        <v>4692681.023</v>
+      </c>
+      <c r="F88" s="80"/>
+      <c r="G88" s="80"/>
       <c r="H88" s="30" t="s">
         <v>8</v>
       </c>
@@ -4784,17 +4478,17 @@
     <row r="89" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="19">
-        <v>59</v>
+      <c r="C89" s="46">
+        <v>58</v>
       </c>
       <c r="D89" s="30">
-        <v>7517951.9790000003</v>
+        <v>7517951.3300000001</v>
       </c>
       <c r="E89" s="30">
-        <v>4692687.1399999997</v>
-      </c>
-      <c r="F89" s="62"/>
-      <c r="G89" s="62"/>
+        <v>4692686.5060000001</v>
+      </c>
+      <c r="F89" s="80"/>
+      <c r="G89" s="80"/>
       <c r="H89" s="30" t="s">
         <v>8</v>
       </c>
@@ -4805,17 +4499,17 @@
     <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="19">
-        <v>60</v>
+      <c r="C90" s="46">
+        <v>59</v>
       </c>
       <c r="D90" s="30">
-        <v>7517952.0760000004</v>
+        <v>7517951.9790000003</v>
       </c>
       <c r="E90" s="30">
-        <v>4692688.1239999998</v>
-      </c>
-      <c r="F90" s="62"/>
-      <c r="G90" s="62"/>
+        <v>4692687.1399999997</v>
+      </c>
+      <c r="F90" s="80"/>
+      <c r="G90" s="80"/>
       <c r="H90" s="30" t="s">
         <v>8</v>
       </c>
@@ -4826,17 +4520,17 @@
     <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="19">
-        <v>61</v>
+      <c r="C91" s="46">
+        <v>60</v>
       </c>
       <c r="D91" s="30">
-        <v>7517950.1849999996</v>
+        <v>7517952.0760000004</v>
       </c>
       <c r="E91" s="30">
-        <v>4692693.4919999996</v>
-      </c>
-      <c r="F91" s="62"/>
-      <c r="G91" s="62"/>
+        <v>4692688.1239999998</v>
+      </c>
+      <c r="F91" s="80"/>
+      <c r="G91" s="80"/>
       <c r="H91" s="30" t="s">
         <v>8</v>
       </c>
@@ -4847,17 +4541,17 @@
     <row r="92" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="19">
-        <v>62</v>
+      <c r="C92" s="46">
+        <v>61</v>
       </c>
       <c r="D92" s="30">
-        <v>7517949.5559999999</v>
+        <v>7517950.1849999996</v>
       </c>
       <c r="E92" s="30">
-        <v>4692694.1169999996</v>
-      </c>
-      <c r="F92" s="62"/>
-      <c r="G92" s="62"/>
+        <v>4692693.4919999996</v>
+      </c>
+      <c r="F92" s="80"/>
+      <c r="G92" s="80"/>
       <c r="H92" s="30" t="s">
         <v>8</v>
       </c>
@@ -4868,17 +4562,17 @@
     <row r="93" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="19">
-        <v>63</v>
+      <c r="C93" s="46">
+        <v>62</v>
       </c>
       <c r="D93" s="30">
-        <v>7517948.5300000003</v>
+        <v>7517949.5559999999</v>
       </c>
       <c r="E93" s="30">
-        <v>4692694.1579999998</v>
-      </c>
-      <c r="F93" s="62"/>
-      <c r="G93" s="62"/>
+        <v>4692694.1169999996</v>
+      </c>
+      <c r="F93" s="80"/>
+      <c r="G93" s="80"/>
       <c r="H93" s="30" t="s">
         <v>8</v>
       </c>
@@ -4889,17 +4583,17 @@
     <row r="94" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="19">
-        <v>105</v>
+      <c r="C94" s="46">
+        <v>63</v>
       </c>
       <c r="D94" s="30">
-        <v>7517927.7654999997</v>
+        <v>7517948.5300000003</v>
       </c>
       <c r="E94" s="30">
-        <v>4692687.1445000004</v>
-      </c>
-      <c r="F94" s="62"/>
-      <c r="G94" s="62"/>
+        <v>4692694.1579999998</v>
+      </c>
+      <c r="F94" s="80"/>
+      <c r="G94" s="80"/>
       <c r="H94" s="30" t="s">
         <v>8</v>
       </c>
@@ -4910,17 +4604,17 @@
     <row r="95" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
-      <c r="C95" s="19">
-        <v>106</v>
+      <c r="C95" s="46">
+        <v>105</v>
       </c>
       <c r="D95" s="30">
-        <v>7517928.7182999998</v>
+        <v>7517927.7654999997</v>
       </c>
       <c r="E95" s="30">
-        <v>4692684.3208999997</v>
-      </c>
-      <c r="F95" s="62"/>
-      <c r="G95" s="62"/>
+        <v>4692687.1445000004</v>
+      </c>
+      <c r="F95" s="80"/>
+      <c r="G95" s="80"/>
       <c r="H95" s="30" t="s">
         <v>8</v>
       </c>
@@ -4931,17 +4625,17 @@
     <row r="96" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="19">
-        <v>107</v>
+      <c r="C96" s="46">
+        <v>106</v>
       </c>
       <c r="D96" s="30">
-        <v>7517927.7045</v>
+        <v>7517928.7182999998</v>
       </c>
       <c r="E96" s="30">
-        <v>4692683.9785000002</v>
-      </c>
-      <c r="F96" s="62"/>
-      <c r="G96" s="62"/>
+        <v>4692684.3208999997</v>
+      </c>
+      <c r="F96" s="80"/>
+      <c r="G96" s="80"/>
       <c r="H96" s="30" t="s">
         <v>8</v>
       </c>
@@ -4952,17 +4646,17 @@
     <row r="97" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
-      <c r="C97" s="19">
-        <v>108</v>
+      <c r="C97" s="46">
+        <v>107</v>
       </c>
       <c r="D97" s="30">
-        <v>7517925.0517999995</v>
+        <v>7517927.7045</v>
       </c>
       <c r="E97" s="30">
-        <v>4692683.0823999997</v>
-      </c>
-      <c r="F97" s="62"/>
-      <c r="G97" s="62"/>
+        <v>4692683.9785000002</v>
+      </c>
+      <c r="F97" s="80"/>
+      <c r="G97" s="80"/>
       <c r="H97" s="30" t="s">
         <v>8</v>
       </c>
@@ -4973,17 +4667,17 @@
     <row r="98" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="19">
-        <v>109</v>
+      <c r="C98" s="46">
+        <v>108</v>
       </c>
       <c r="D98" s="30">
-        <v>7517926.6694</v>
+        <v>7517925.0517999995</v>
       </c>
       <c r="E98" s="30">
-        <v>4692678.2884999998</v>
-      </c>
-      <c r="F98" s="62"/>
-      <c r="G98" s="62"/>
+        <v>4692683.0823999997</v>
+      </c>
+      <c r="F98" s="80"/>
+      <c r="G98" s="80"/>
       <c r="H98" s="30" t="s">
         <v>8</v>
       </c>
@@ -4994,17 +4688,17 @@
     <row r="99" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
-      <c r="C99" s="19">
-        <v>110</v>
+      <c r="C99" s="46">
+        <v>109</v>
       </c>
       <c r="D99" s="30">
-        <v>7517928.0525000002</v>
+        <v>7517926.6694</v>
       </c>
       <c r="E99" s="30">
-        <v>4692678.7551999995</v>
-      </c>
-      <c r="F99" s="62"/>
-      <c r="G99" s="62"/>
+        <v>4692678.2884999998</v>
+      </c>
+      <c r="F99" s="80"/>
+      <c r="G99" s="80"/>
       <c r="H99" s="30" t="s">
         <v>8</v>
       </c>
@@ -5015,17 +4709,17 @@
     <row r="100" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
-      <c r="C100" s="19">
-        <v>111</v>
+      <c r="C100" s="46">
+        <v>110</v>
       </c>
       <c r="D100" s="30">
-        <v>7517929.3223999999</v>
+        <v>7517928.0525000002</v>
       </c>
       <c r="E100" s="30">
-        <v>4692679.1836999999</v>
-      </c>
-      <c r="F100" s="62"/>
-      <c r="G100" s="62"/>
+        <v>4692678.7551999995</v>
+      </c>
+      <c r="F100" s="80"/>
+      <c r="G100" s="80"/>
       <c r="H100" s="30" t="s">
         <v>8</v>
       </c>
@@ -5036,17 +4730,17 @@
     <row r="101" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
-      <c r="C101" s="19">
-        <v>112</v>
+      <c r="C101" s="46">
+        <v>111</v>
       </c>
       <c r="D101" s="30">
-        <v>7517950.6852000002</v>
+        <v>7517929.3223999999</v>
       </c>
       <c r="E101" s="30">
-        <v>4692679.26</v>
-      </c>
-      <c r="F101" s="62"/>
-      <c r="G101" s="62"/>
+        <v>4692679.1836999999</v>
+      </c>
+      <c r="F101" s="80"/>
+      <c r="G101" s="80"/>
       <c r="H101" s="30" t="s">
         <v>8</v>
       </c>
@@ -5057,17 +4751,17 @@
     <row r="102" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="19">
-        <v>113</v>
+      <c r="C102" s="46">
+        <v>112</v>
       </c>
       <c r="D102" s="30">
-        <v>7517953.2906999998</v>
+        <v>7517950.6852000002</v>
       </c>
       <c r="E102" s="30">
-        <v>4692680.1398</v>
-      </c>
-      <c r="F102" s="62"/>
-      <c r="G102" s="62"/>
+        <v>4692679.26</v>
+      </c>
+      <c r="F102" s="80"/>
+      <c r="G102" s="80"/>
       <c r="H102" s="30" t="s">
         <v>8</v>
       </c>
@@ -5078,17 +4772,17 @@
     <row r="103" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
-      <c r="C103" s="19">
-        <v>114</v>
+      <c r="C103" s="46">
+        <v>113</v>
       </c>
       <c r="D103" s="30">
-        <v>7517948.5182999996</v>
+        <v>7517953.2906999998</v>
       </c>
       <c r="E103" s="30">
-        <v>4692685.5575999999</v>
-      </c>
-      <c r="F103" s="62"/>
-      <c r="G103" s="62"/>
+        <v>4692680.1398</v>
+      </c>
+      <c r="F103" s="80"/>
+      <c r="G103" s="80"/>
       <c r="H103" s="30" t="s">
         <v>8</v>
       </c>
@@ -5099,17 +4793,17 @@
     <row r="104" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="19">
-        <v>115</v>
+      <c r="C104" s="46">
+        <v>114</v>
       </c>
       <c r="D104" s="30">
-        <v>7517951.1238000002</v>
+        <v>7517948.5182999996</v>
       </c>
       <c r="E104" s="30">
-        <v>4692686.4374000002</v>
-      </c>
-      <c r="F104" s="62"/>
-      <c r="G104" s="62"/>
+        <v>4692685.5575999999</v>
+      </c>
+      <c r="F104" s="80"/>
+      <c r="G104" s="80"/>
       <c r="H104" s="30" t="s">
         <v>8</v>
       </c>
@@ -5120,17 +4814,17 @@
     <row r="105" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
-      <c r="C105" s="19">
-        <v>116</v>
+      <c r="C105" s="46">
+        <v>115</v>
       </c>
       <c r="D105" s="30">
-        <v>7517946.1694999998</v>
+        <v>7517951.1238000002</v>
       </c>
       <c r="E105" s="30">
-        <v>4692690.9013999999</v>
-      </c>
-      <c r="F105" s="62"/>
-      <c r="G105" s="62"/>
+        <v>4692686.4374000002</v>
+      </c>
+      <c r="F105" s="80"/>
+      <c r="G105" s="80"/>
       <c r="H105" s="30" t="s">
         <v>8</v>
       </c>
@@ -5141,17 +4835,17 @@
     <row r="106" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="19">
-        <v>117</v>
+      <c r="C106" s="46">
+        <v>116</v>
       </c>
       <c r="D106" s="30">
-        <v>7517945.4238999998</v>
+        <v>7517946.1694999998</v>
       </c>
       <c r="E106" s="30">
-        <v>4692693.1089000003</v>
-      </c>
-      <c r="F106" s="62"/>
-      <c r="G106" s="62"/>
+        <v>4692690.9013999999</v>
+      </c>
+      <c r="F106" s="80"/>
+      <c r="G106" s="80"/>
       <c r="H106" s="30" t="s">
         <v>8</v>
       </c>
@@ -5162,17 +4856,17 @@
     <row r="107" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="19">
-        <v>118</v>
+      <c r="C107" s="46">
+        <v>117</v>
       </c>
       <c r="D107" s="30">
-        <v>7517941.9455000004</v>
+        <v>7517945.4238999998</v>
       </c>
       <c r="E107" s="30">
-        <v>4692689.4746000003</v>
-      </c>
-      <c r="F107" s="62"/>
-      <c r="G107" s="62"/>
+        <v>4692693.1089000003</v>
+      </c>
+      <c r="F107" s="80"/>
+      <c r="G107" s="80"/>
       <c r="H107" s="30" t="s">
         <v>8</v>
       </c>
@@ -5183,17 +4877,17 @@
     <row r="108" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
-      <c r="C108" s="19">
-        <v>119</v>
+      <c r="C108" s="46">
+        <v>118</v>
       </c>
       <c r="D108" s="30">
-        <v>7517936.9005000005</v>
+        <v>7517941.8033999996</v>
       </c>
       <c r="E108" s="30">
-        <v>4692687.7706000004</v>
-      </c>
-      <c r="F108" s="62"/>
-      <c r="G108" s="62"/>
+        <v>4692689.4265999999</v>
+      </c>
+      <c r="F108" s="80"/>
+      <c r="G108" s="80"/>
       <c r="H108" s="30" t="s">
         <v>8</v>
       </c>
@@ -5204,17 +4898,17 @@
     <row r="109" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
-      <c r="C109" s="19">
-        <v>120</v>
+      <c r="C109" s="46">
+        <v>119</v>
       </c>
       <c r="D109" s="30">
-        <v>7517936.1549000004</v>
+        <v>7517936.9404999996</v>
       </c>
       <c r="E109" s="30">
-        <v>4692689.9780000001</v>
-      </c>
-      <c r="F109" s="62"/>
-      <c r="G109" s="62"/>
+        <v>4692687.6520999996</v>
+      </c>
+      <c r="F109" s="80"/>
+      <c r="G109" s="80"/>
       <c r="H109" s="30" t="s">
         <v>8</v>
       </c>
@@ -5225,17 +4919,17 @@
     <row r="110" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="19">
-        <v>14</v>
+      <c r="C110" s="46">
+        <v>120</v>
       </c>
       <c r="D110" s="30">
-        <v>7517930.4069999997</v>
+        <v>7517936.1549000004</v>
       </c>
       <c r="E110" s="30">
-        <v>4692671.8150000004</v>
-      </c>
-      <c r="F110" s="63"/>
-      <c r="G110" s="63"/>
+        <v>4692689.9780000001</v>
+      </c>
+      <c r="F110" s="80"/>
+      <c r="G110" s="80"/>
       <c r="H110" s="30" t="s">
         <v>8</v>
       </c>
@@ -5246,12 +4940,20 @@
     <row r="111" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="14"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="13"/>
+      <c r="C111" s="46">
+        <v>121</v>
+      </c>
+      <c r="D111" s="30">
+        <v>7517941.8433999997</v>
+      </c>
+      <c r="E111" s="30">
+        <v>4692689.3081999999</v>
+      </c>
+      <c r="F111" s="80"/>
+      <c r="G111" s="80"/>
+      <c r="H111" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I111" s="11"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -5259,12 +4961,20 @@
     <row r="112" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="14"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="13"/>
+      <c r="C112" s="46">
+        <v>101</v>
+      </c>
+      <c r="D112" s="30">
+        <v>7517952.1813000003</v>
+      </c>
+      <c r="E112" s="30">
+        <v>4692679.7653000001</v>
+      </c>
+      <c r="F112" s="81"/>
+      <c r="G112" s="81"/>
+      <c r="H112" s="30" t="s">
+        <v>20</v>
+      </c>
       <c r="I112" s="11"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -5363,28 +5073,28 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="57" t="s">
+      <c r="C120" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D120" s="57"/>
-      <c r="E120" s="57"/>
-      <c r="F120" s="57"/>
-      <c r="G120" s="57"/>
-      <c r="H120" s="57"/>
-      <c r="I120" s="57"/>
+      <c r="D120" s="59"/>
+      <c r="E120" s="59"/>
+      <c r="F120" s="59"/>
+      <c r="G120" s="59"/>
+      <c r="H120" s="59"/>
+      <c r="I120" s="59"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="57"/>
-      <c r="D121" s="57"/>
-      <c r="E121" s="57"/>
-      <c r="F121" s="57"/>
-      <c r="G121" s="57"/>
-      <c r="H121" s="57"/>
-      <c r="I121" s="57"/>
+      <c r="C121" s="59"/>
+      <c r="D121" s="59"/>
+      <c r="E121" s="59"/>
+      <c r="F121" s="59"/>
+      <c r="G121" s="59"/>
+      <c r="H121" s="59"/>
+      <c r="I121" s="59"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
@@ -5473,114 +5183,114 @@
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
-      <c r="E128" s="64" t="s">
+      <c r="E128" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F128" s="65"/>
-      <c r="G128" s="66"/>
-      <c r="H128" s="67" t="s">
+      <c r="F128" s="61"/>
+      <c r="G128" s="62"/>
+      <c r="H128" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I128" s="68"/>
-      <c r="J128" s="71"/>
-      <c r="K128" s="72"/>
+      <c r="I128" s="64"/>
+      <c r="J128" s="67"/>
+      <c r="K128" s="68"/>
     </row>
     <row r="129" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="75" t="s">
+      <c r="A129" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B129" s="76"/>
-      <c r="C129" s="76"/>
-      <c r="D129" s="77"/>
-      <c r="E129" s="78">
+      <c r="B129" s="72"/>
+      <c r="C129" s="72"/>
+      <c r="D129" s="73"/>
+      <c r="E129" s="74">
         <v>140</v>
       </c>
-      <c r="F129" s="79"/>
-      <c r="G129" s="80"/>
-      <c r="H129" s="69"/>
-      <c r="I129" s="70"/>
-      <c r="J129" s="73"/>
-      <c r="K129" s="74"/>
+      <c r="F129" s="75"/>
+      <c r="G129" s="76"/>
+      <c r="H129" s="65"/>
+      <c r="I129" s="66"/>
+      <c r="J129" s="69"/>
+      <c r="K129" s="70"/>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="46"/>
-      <c r="B132" s="46"/>
-      <c r="C132" s="46"/>
-      <c r="D132" s="46"/>
-      <c r="E132" s="46"/>
-      <c r="F132" s="46"/>
-      <c r="G132" s="46"/>
-      <c r="H132" s="46"/>
-      <c r="I132" s="46"/>
-      <c r="J132" s="46"/>
-      <c r="K132" s="46"/>
+      <c r="A132" s="48"/>
+      <c r="B132" s="48"/>
+      <c r="C132" s="48"/>
+      <c r="D132" s="48"/>
+      <c r="E132" s="48"/>
+      <c r="F132" s="48"/>
+      <c r="G132" s="48"/>
+      <c r="H132" s="48"/>
+      <c r="I132" s="48"/>
+      <c r="J132" s="48"/>
+      <c r="K132" s="48"/>
     </row>
     <row r="133" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="46"/>
-      <c r="B133" s="46"/>
-      <c r="C133" s="46"/>
-      <c r="D133" s="46"/>
-      <c r="E133" s="46"/>
-      <c r="F133" s="46"/>
-      <c r="G133" s="46"/>
-      <c r="H133" s="46"/>
-      <c r="I133" s="46"/>
-      <c r="J133" s="46"/>
-      <c r="K133" s="46"/>
+      <c r="A133" s="48"/>
+      <c r="B133" s="48"/>
+      <c r="C133" s="48"/>
+      <c r="D133" s="48"/>
+      <c r="E133" s="48"/>
+      <c r="F133" s="48"/>
+      <c r="G133" s="48"/>
+      <c r="H133" s="48"/>
+      <c r="I133" s="48"/>
+      <c r="J133" s="48"/>
+      <c r="K133" s="48"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="47" t="s">
+      <c r="A134" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B134" s="47"/>
-      <c r="C134" s="47"/>
-      <c r="D134" s="47"/>
-      <c r="E134" s="47"/>
-      <c r="F134" s="47"/>
-      <c r="G134" s="47"/>
-      <c r="H134" s="47"/>
-      <c r="I134" s="47"/>
-      <c r="J134" s="47"/>
-      <c r="K134" s="47"/>
+      <c r="B134" s="49"/>
+      <c r="C134" s="49"/>
+      <c r="D134" s="49"/>
+      <c r="E134" s="49"/>
+      <c r="F134" s="49"/>
+      <c r="G134" s="49"/>
+      <c r="H134" s="49"/>
+      <c r="I134" s="49"/>
+      <c r="J134" s="49"/>
+      <c r="K134" s="49"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="47"/>
-      <c r="B135" s="47"/>
-      <c r="C135" s="47"/>
-      <c r="D135" s="47"/>
-      <c r="E135" s="47"/>
-      <c r="F135" s="47"/>
-      <c r="G135" s="47"/>
-      <c r="H135" s="47"/>
-      <c r="I135" s="47"/>
-      <c r="J135" s="47"/>
-      <c r="K135" s="47"/>
+      <c r="A135" s="49"/>
+      <c r="B135" s="49"/>
+      <c r="C135" s="49"/>
+      <c r="D135" s="49"/>
+      <c r="E135" s="49"/>
+      <c r="F135" s="49"/>
+      <c r="G135" s="49"/>
+      <c r="H135" s="49"/>
+      <c r="I135" s="49"/>
+      <c r="J135" s="49"/>
+      <c r="K135" s="49"/>
     </row>
     <row r="136" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="47"/>
-      <c r="B136" s="47"/>
-      <c r="C136" s="47"/>
-      <c r="D136" s="47"/>
-      <c r="E136" s="47"/>
-      <c r="F136" s="47"/>
-      <c r="G136" s="47"/>
-      <c r="H136" s="47"/>
-      <c r="I136" s="47"/>
-      <c r="J136" s="47"/>
-      <c r="K136" s="47"/>
+      <c r="A136" s="49"/>
+      <c r="B136" s="49"/>
+      <c r="C136" s="49"/>
+      <c r="D136" s="49"/>
+      <c r="E136" s="49"/>
+      <c r="F136" s="49"/>
+      <c r="G136" s="49"/>
+      <c r="H136" s="49"/>
+      <c r="I136" s="49"/>
+      <c r="J136" s="49"/>
+      <c r="K136" s="49"/>
     </row>
     <row r="137" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="47"/>
-      <c r="B137" s="47"/>
-      <c r="C137" s="47"/>
-      <c r="D137" s="47"/>
-      <c r="E137" s="47"/>
-      <c r="F137" s="47"/>
-      <c r="G137" s="47"/>
-      <c r="H137" s="47"/>
-      <c r="I137" s="47"/>
-      <c r="J137" s="47"/>
-      <c r="K137" s="47"/>
+      <c r="A137" s="49"/>
+      <c r="B137" s="49"/>
+      <c r="C137" s="49"/>
+      <c r="D137" s="49"/>
+      <c r="E137" s="49"/>
+      <c r="F137" s="49"/>
+      <c r="G137" s="49"/>
+      <c r="H137" s="49"/>
+      <c r="I137" s="49"/>
+      <c r="J137" s="49"/>
+      <c r="K137" s="49"/>
     </row>
     <row r="138" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
@@ -5597,36 +5307,36 @@
     </row>
     <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
-      <c r="C139" s="48"/>
-      <c r="D139" s="49"/>
-      <c r="E139" s="49"/>
-      <c r="F139" s="49"/>
-      <c r="G139" s="49"/>
-      <c r="H139" s="49"/>
-      <c r="I139" s="50"/>
+      <c r="C139" s="50"/>
+      <c r="D139" s="51"/>
+      <c r="E139" s="51"/>
+      <c r="F139" s="51"/>
+      <c r="G139" s="51"/>
+      <c r="H139" s="51"/>
+      <c r="I139" s="52"/>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
     </row>
     <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
-      <c r="C140" s="51"/>
-      <c r="D140" s="52"/>
-      <c r="E140" s="52"/>
-      <c r="F140" s="52"/>
-      <c r="G140" s="52"/>
-      <c r="H140" s="52"/>
-      <c r="I140" s="53"/>
+      <c r="C140" s="53"/>
+      <c r="D140" s="54"/>
+      <c r="E140" s="54"/>
+      <c r="F140" s="54"/>
+      <c r="G140" s="54"/>
+      <c r="H140" s="54"/>
+      <c r="I140" s="55"/>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
     </row>
     <row r="141" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
-      <c r="C141" s="54"/>
-      <c r="D141" s="55"/>
-      <c r="E141" s="55"/>
-      <c r="F141" s="55"/>
-      <c r="G141" s="55"/>
-      <c r="H141" s="55"/>
+      <c r="C141" s="77"/>
+      <c r="D141" s="78"/>
+      <c r="E141" s="78"/>
+      <c r="F141" s="78"/>
+      <c r="G141" s="78"/>
+      <c r="H141" s="78"/>
       <c r="I141" s="56"/>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
@@ -5678,8 +5388,8 @@
       <c r="F144" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G144" s="61" t="s">
-        <v>24</v>
+      <c r="G144" s="79" t="s">
+        <v>23</v>
       </c>
       <c r="H144" s="30" t="s">
         <v>8</v>
@@ -5703,7 +5413,7 @@
       <c r="F145" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G145" s="62"/>
+      <c r="G145" s="80"/>
       <c r="H145" s="30" t="s">
         <v>8</v>
       </c>
@@ -5726,7 +5436,7 @@
       <c r="F146" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G146" s="62"/>
+      <c r="G146" s="80"/>
       <c r="H146" s="30" t="s">
         <v>8</v>
       </c>
@@ -5749,7 +5459,7 @@
       <c r="F147" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G147" s="62"/>
+      <c r="G147" s="80"/>
       <c r="H147" s="30" t="s">
         <v>8</v>
       </c>
@@ -5772,7 +5482,7 @@
       <c r="F148" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G148" s="62"/>
+      <c r="G148" s="80"/>
       <c r="H148" s="30" t="s">
         <v>8</v>
       </c>
@@ -5795,7 +5505,7 @@
       <c r="F149" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G149" s="62"/>
+      <c r="G149" s="80"/>
       <c r="H149" s="30" t="s">
         <v>8</v>
       </c>
@@ -5818,7 +5528,7 @@
       <c r="F150" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G150" s="62"/>
+      <c r="G150" s="80"/>
       <c r="H150" s="30" t="s">
         <v>8</v>
       </c>
@@ -5841,7 +5551,7 @@
       <c r="F151" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G151" s="62"/>
+      <c r="G151" s="80"/>
       <c r="H151" s="30" t="s">
         <v>8</v>
       </c>
@@ -5864,7 +5574,7 @@
       <c r="F152" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G152" s="62"/>
+      <c r="G152" s="80"/>
       <c r="H152" s="30" t="s">
         <v>8</v>
       </c>
@@ -5887,7 +5597,7 @@
       <c r="F153" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G153" s="62"/>
+      <c r="G153" s="80"/>
       <c r="H153" s="30" t="s">
         <v>8</v>
       </c>
@@ -5910,7 +5620,7 @@
       <c r="F154" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G154" s="62"/>
+      <c r="G154" s="80"/>
       <c r="H154" s="30" t="s">
         <v>8</v>
       </c>
@@ -5933,7 +5643,7 @@
       <c r="F155" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G155" s="62"/>
+      <c r="G155" s="80"/>
       <c r="H155" s="30" t="s">
         <v>8</v>
       </c>
@@ -5956,7 +5666,7 @@
       <c r="F156" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G156" s="62"/>
+      <c r="G156" s="80"/>
       <c r="H156" s="30" t="s">
         <v>8</v>
       </c>
@@ -5979,7 +5689,7 @@
       <c r="F157" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G157" s="62"/>
+      <c r="G157" s="80"/>
       <c r="H157" s="30" t="s">
         <v>8</v>
       </c>
@@ -6002,7 +5712,7 @@
       <c r="F158" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G158" s="62"/>
+      <c r="G158" s="80"/>
       <c r="H158" s="30" t="s">
         <v>8</v>
       </c>
@@ -6025,7 +5735,7 @@
       <c r="F159" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G159" s="62"/>
+      <c r="G159" s="80"/>
       <c r="H159" s="30" t="s">
         <v>8</v>
       </c>
@@ -6048,7 +5758,7 @@
       <c r="F160" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G160" s="62"/>
+      <c r="G160" s="80"/>
       <c r="H160" s="30" t="s">
         <v>8</v>
       </c>
@@ -6071,7 +5781,7 @@
       <c r="F161" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G161" s="62"/>
+      <c r="G161" s="80"/>
       <c r="H161" s="30" t="s">
         <v>8</v>
       </c>
@@ -6094,7 +5804,7 @@
       <c r="F162" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G162" s="62"/>
+      <c r="G162" s="80"/>
       <c r="H162" s="30" t="s">
         <v>8</v>
       </c>
@@ -6117,7 +5827,7 @@
       <c r="F163" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G163" s="62"/>
+      <c r="G163" s="80"/>
       <c r="H163" s="30" t="s">
         <v>8</v>
       </c>
@@ -6140,7 +5850,7 @@
       <c r="F164" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G164" s="62"/>
+      <c r="G164" s="80"/>
       <c r="H164" s="30" t="s">
         <v>8</v>
       </c>
@@ -6163,7 +5873,7 @@
       <c r="F165" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G165" s="62"/>
+      <c r="G165" s="80"/>
       <c r="H165" s="30" t="s">
         <v>8</v>
       </c>
@@ -6186,7 +5896,7 @@
       <c r="F166" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G166" s="62"/>
+      <c r="G166" s="80"/>
       <c r="H166" s="30" t="s">
         <v>8</v>
       </c>
@@ -6209,7 +5919,7 @@
       <c r="F167" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G167" s="62"/>
+      <c r="G167" s="80"/>
       <c r="H167" s="30" t="s">
         <v>8</v>
       </c>
@@ -6232,7 +5942,7 @@
       <c r="F168" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G168" s="62"/>
+      <c r="G168" s="80"/>
       <c r="H168" s="30" t="s">
         <v>8</v>
       </c>
@@ -6255,7 +5965,7 @@
       <c r="F169" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G169" s="62"/>
+      <c r="G169" s="80"/>
       <c r="H169" s="30" t="s">
         <v>8</v>
       </c>
@@ -6278,7 +5988,7 @@
       <c r="F170" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G170" s="62"/>
+      <c r="G170" s="80"/>
       <c r="H170" s="30" t="s">
         <v>8</v>
       </c>
@@ -6301,7 +6011,7 @@
       <c r="F171" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G171" s="62"/>
+      <c r="G171" s="80"/>
       <c r="H171" s="30" t="s">
         <v>8</v>
       </c>
@@ -6323,7 +6033,7 @@
       <c r="F172" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G172" s="62"/>
+      <c r="G172" s="80"/>
       <c r="H172" s="30" t="s">
         <v>8</v>
       </c>
@@ -6345,7 +6055,7 @@
       <c r="F173" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G173" s="62"/>
+      <c r="G173" s="80"/>
       <c r="H173" s="30" t="s">
         <v>8</v>
       </c>
@@ -6368,7 +6078,7 @@
       <c r="F174" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G174" s="62"/>
+      <c r="G174" s="80"/>
       <c r="H174" s="30" t="s">
         <v>8</v>
       </c>
@@ -6391,7 +6101,7 @@
       <c r="F175" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G175" s="62"/>
+      <c r="G175" s="80"/>
       <c r="H175" s="30" t="s">
         <v>8</v>
       </c>
@@ -6414,7 +6124,7 @@
       <c r="F176" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G176" s="62"/>
+      <c r="G176" s="80"/>
       <c r="H176" s="30" t="s">
         <v>8</v>
       </c>
@@ -6437,7 +6147,7 @@
       <c r="F177" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G177" s="62"/>
+      <c r="G177" s="80"/>
       <c r="H177" s="30" t="s">
         <v>8</v>
       </c>
@@ -6458,9 +6168,9 @@
         <v>4692678.5990000004</v>
       </c>
       <c r="F178" s="19">
-        <v>618.84299999999996</v>
-      </c>
-      <c r="G178" s="63"/>
+        <v>616.38300000000004</v>
+      </c>
+      <c r="G178" s="81"/>
       <c r="H178" s="30" t="s">
         <v>20</v>
       </c>
@@ -6510,28 +6220,28 @@
     <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
-      <c r="C182" s="57" t="s">
+      <c r="C182" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D182" s="57"/>
-      <c r="E182" s="57"/>
-      <c r="F182" s="57"/>
-      <c r="G182" s="57"/>
-      <c r="H182" s="57"/>
-      <c r="I182" s="57"/>
+      <c r="D182" s="59"/>
+      <c r="E182" s="59"/>
+      <c r="F182" s="59"/>
+      <c r="G182" s="59"/>
+      <c r="H182" s="59"/>
+      <c r="I182" s="59"/>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
     </row>
     <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
-      <c r="C183" s="57"/>
-      <c r="D183" s="57"/>
-      <c r="E183" s="57"/>
-      <c r="F183" s="57"/>
-      <c r="G183" s="57"/>
-      <c r="H183" s="57"/>
-      <c r="I183" s="57"/>
+      <c r="C183" s="59"/>
+      <c r="D183" s="59"/>
+      <c r="E183" s="59"/>
+      <c r="F183" s="59"/>
+      <c r="G183" s="59"/>
+      <c r="H183" s="59"/>
+      <c r="I183" s="59"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
     </row>
@@ -6646,147 +6356,147 @@
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
-      <c r="E192" s="64" t="s">
+      <c r="E192" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F192" s="65"/>
-      <c r="G192" s="66"/>
-      <c r="H192" s="67" t="s">
+      <c r="F192" s="61"/>
+      <c r="G192" s="62"/>
+      <c r="H192" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I192" s="68"/>
-      <c r="J192" s="71"/>
-      <c r="K192" s="72"/>
+      <c r="I192" s="64"/>
+      <c r="J192" s="67"/>
+      <c r="K192" s="68"/>
     </row>
     <row r="193" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="75" t="s">
+      <c r="A193" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B193" s="76"/>
-      <c r="C193" s="76"/>
-      <c r="D193" s="77"/>
-      <c r="E193" s="78">
+      <c r="B193" s="72"/>
+      <c r="C193" s="72"/>
+      <c r="D193" s="73"/>
+      <c r="E193" s="74">
         <v>140</v>
       </c>
-      <c r="F193" s="79"/>
-      <c r="G193" s="80"/>
-      <c r="H193" s="69"/>
-      <c r="I193" s="70"/>
-      <c r="J193" s="73"/>
-      <c r="K193" s="74"/>
+      <c r="F193" s="75"/>
+      <c r="G193" s="76"/>
+      <c r="H193" s="65"/>
+      <c r="I193" s="66"/>
+      <c r="J193" s="69"/>
+      <c r="K193" s="70"/>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A194" s="46"/>
-      <c r="B194" s="46"/>
-      <c r="C194" s="46"/>
-      <c r="D194" s="46"/>
-      <c r="E194" s="46"/>
-      <c r="F194" s="46"/>
-      <c r="G194" s="46"/>
-      <c r="H194" s="46"/>
-      <c r="I194" s="46"/>
-      <c r="J194" s="46"/>
-      <c r="K194" s="46"/>
+      <c r="A194" s="48"/>
+      <c r="B194" s="48"/>
+      <c r="C194" s="48"/>
+      <c r="D194" s="48"/>
+      <c r="E194" s="48"/>
+      <c r="F194" s="48"/>
+      <c r="G194" s="48"/>
+      <c r="H194" s="48"/>
+      <c r="I194" s="48"/>
+      <c r="J194" s="48"/>
+      <c r="K194" s="48"/>
     </row>
     <row r="195" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="46"/>
-      <c r="B195" s="46"/>
-      <c r="C195" s="46"/>
-      <c r="D195" s="46"/>
-      <c r="E195" s="46"/>
-      <c r="F195" s="46"/>
-      <c r="G195" s="46"/>
-      <c r="H195" s="46"/>
-      <c r="I195" s="46"/>
-      <c r="J195" s="46"/>
-      <c r="K195" s="46"/>
+      <c r="A195" s="48"/>
+      <c r="B195" s="48"/>
+      <c r="C195" s="48"/>
+      <c r="D195" s="48"/>
+      <c r="E195" s="48"/>
+      <c r="F195" s="48"/>
+      <c r="G195" s="48"/>
+      <c r="H195" s="48"/>
+      <c r="I195" s="48"/>
+      <c r="J195" s="48"/>
+      <c r="K195" s="48"/>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A196" s="47" t="s">
+      <c r="A196" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B196" s="47"/>
-      <c r="C196" s="47"/>
-      <c r="D196" s="47"/>
-      <c r="E196" s="47"/>
-      <c r="F196" s="47"/>
-      <c r="G196" s="47"/>
-      <c r="H196" s="47"/>
-      <c r="I196" s="47"/>
-      <c r="J196" s="47"/>
-      <c r="K196" s="47"/>
+      <c r="B196" s="49"/>
+      <c r="C196" s="49"/>
+      <c r="D196" s="49"/>
+      <c r="E196" s="49"/>
+      <c r="F196" s="49"/>
+      <c r="G196" s="49"/>
+      <c r="H196" s="49"/>
+      <c r="I196" s="49"/>
+      <c r="J196" s="49"/>
+      <c r="K196" s="49"/>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A197" s="47"/>
-      <c r="B197" s="47"/>
-      <c r="C197" s="47"/>
-      <c r="D197" s="47"/>
-      <c r="E197" s="47"/>
-      <c r="F197" s="47"/>
-      <c r="G197" s="47"/>
-      <c r="H197" s="47"/>
-      <c r="I197" s="47"/>
-      <c r="J197" s="47"/>
-      <c r="K197" s="47"/>
+      <c r="A197" s="49"/>
+      <c r="B197" s="49"/>
+      <c r="C197" s="49"/>
+      <c r="D197" s="49"/>
+      <c r="E197" s="49"/>
+      <c r="F197" s="49"/>
+      <c r="G197" s="49"/>
+      <c r="H197" s="49"/>
+      <c r="I197" s="49"/>
+      <c r="J197" s="49"/>
+      <c r="K197" s="49"/>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" s="47"/>
-      <c r="B198" s="47"/>
-      <c r="C198" s="47"/>
-      <c r="D198" s="47"/>
-      <c r="E198" s="47"/>
-      <c r="F198" s="47"/>
-      <c r="G198" s="47"/>
-      <c r="H198" s="47"/>
-      <c r="I198" s="47"/>
-      <c r="J198" s="47"/>
-      <c r="K198" s="47"/>
+      <c r="A198" s="49"/>
+      <c r="B198" s="49"/>
+      <c r="C198" s="49"/>
+      <c r="D198" s="49"/>
+      <c r="E198" s="49"/>
+      <c r="F198" s="49"/>
+      <c r="G198" s="49"/>
+      <c r="H198" s="49"/>
+      <c r="I198" s="49"/>
+      <c r="J198" s="49"/>
+      <c r="K198" s="49"/>
     </row>
     <row r="199" spans="1:11" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="47"/>
-      <c r="B199" s="47"/>
-      <c r="C199" s="47"/>
-      <c r="D199" s="47"/>
-      <c r="E199" s="47"/>
-      <c r="F199" s="47"/>
-      <c r="G199" s="47"/>
-      <c r="H199" s="47"/>
-      <c r="I199" s="47"/>
-      <c r="J199" s="47"/>
-      <c r="K199" s="47"/>
+      <c r="A199" s="49"/>
+      <c r="B199" s="49"/>
+      <c r="C199" s="49"/>
+      <c r="D199" s="49"/>
+      <c r="E199" s="49"/>
+      <c r="F199" s="49"/>
+      <c r="G199" s="49"/>
+      <c r="H199" s="49"/>
+      <c r="I199" s="49"/>
+      <c r="J199" s="49"/>
+      <c r="K199" s="49"/>
     </row>
     <row r="200" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
-      <c r="C200" s="48"/>
-      <c r="D200" s="49"/>
-      <c r="E200" s="49"/>
-      <c r="F200" s="49"/>
-      <c r="G200" s="49"/>
-      <c r="H200" s="49"/>
-      <c r="I200" s="50"/>
+      <c r="C200" s="50"/>
+      <c r="D200" s="51"/>
+      <c r="E200" s="51"/>
+      <c r="F200" s="51"/>
+      <c r="G200" s="51"/>
+      <c r="H200" s="51"/>
+      <c r="I200" s="52"/>
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
     </row>
     <row r="201" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
-      <c r="C201" s="51"/>
-      <c r="D201" s="52"/>
-      <c r="E201" s="52"/>
-      <c r="F201" s="52"/>
-      <c r="G201" s="52"/>
-      <c r="H201" s="52"/>
-      <c r="I201" s="53"/>
+      <c r="C201" s="53"/>
+      <c r="D201" s="54"/>
+      <c r="E201" s="54"/>
+      <c r="F201" s="54"/>
+      <c r="G201" s="54"/>
+      <c r="H201" s="54"/>
+      <c r="I201" s="55"/>
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
     </row>
     <row r="202" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
-      <c r="C202" s="51"/>
-      <c r="D202" s="52"/>
-      <c r="E202" s="52"/>
-      <c r="F202" s="52"/>
-      <c r="G202" s="52"/>
-      <c r="H202" s="52"/>
+      <c r="C202" s="53"/>
+      <c r="D202" s="54"/>
+      <c r="E202" s="54"/>
+      <c r="F202" s="54"/>
+      <c r="G202" s="54"/>
+      <c r="H202" s="54"/>
       <c r="I202" s="56"/>
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
@@ -6828,11 +6538,11 @@
       <c r="E204" s="30">
         <v>4692673.5029999996</v>
       </c>
-      <c r="F204" s="86">
+      <c r="F204" s="57">
         <v>622.86300000000006</v>
       </c>
-      <c r="G204" s="86" t="s">
-        <v>25</v>
+      <c r="G204" s="57" t="s">
+        <v>24</v>
       </c>
       <c r="H204" s="40" t="s">
         <v>8</v>
@@ -6853,8 +6563,8 @@
       <c r="E205" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F205" s="86"/>
-      <c r="G205" s="86"/>
+      <c r="F205" s="57"/>
+      <c r="G205" s="57"/>
       <c r="H205" s="40" t="s">
         <v>8</v>
       </c>
@@ -6874,8 +6584,8 @@
       <c r="E206" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F206" s="86"/>
-      <c r="G206" s="86"/>
+      <c r="F206" s="57"/>
+      <c r="G206" s="57"/>
       <c r="H206" s="40" t="s">
         <v>8</v>
       </c>
@@ -6895,8 +6605,8 @@
       <c r="E207" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F207" s="86"/>
-      <c r="G207" s="86"/>
+      <c r="F207" s="57"/>
+      <c r="G207" s="57"/>
       <c r="H207" s="40" t="s">
         <v>8</v>
       </c>
@@ -6916,8 +6626,8 @@
       <c r="E208" s="30">
         <v>4692674.3839999996</v>
       </c>
-      <c r="F208" s="86"/>
-      <c r="G208" s="86"/>
+      <c r="F208" s="57"/>
+      <c r="G208" s="57"/>
       <c r="H208" s="40" t="s">
         <v>8</v>
       </c>
@@ -6937,8 +6647,8 @@
       <c r="E209" s="30">
         <v>4692677.5640000002</v>
       </c>
-      <c r="F209" s="86"/>
-      <c r="G209" s="86"/>
+      <c r="F209" s="57"/>
+      <c r="G209" s="57"/>
       <c r="H209" s="40" t="s">
         <v>8</v>
       </c>
@@ -6958,8 +6668,8 @@
       <c r="E210" s="30">
         <v>4692679.0279999999</v>
       </c>
-      <c r="F210" s="86"/>
-      <c r="G210" s="86"/>
+      <c r="F210" s="57"/>
+      <c r="G210" s="57"/>
       <c r="H210" s="40" t="s">
         <v>8</v>
       </c>
@@ -6979,8 +6689,8 @@
       <c r="E211" s="30">
         <v>4692680.25</v>
       </c>
-      <c r="F211" s="86"/>
-      <c r="G211" s="86"/>
+      <c r="F211" s="57"/>
+      <c r="G211" s="57"/>
       <c r="H211" s="40" t="s">
         <v>8</v>
       </c>
@@ -7000,8 +6710,8 @@
       <c r="E212" s="30">
         <v>4692673.0663999999</v>
       </c>
-      <c r="F212" s="86"/>
-      <c r="G212" s="86"/>
+      <c r="F212" s="57"/>
+      <c r="G212" s="57"/>
       <c r="H212" s="40" t="s">
         <v>8</v>
       </c>
@@ -7021,8 +6731,8 @@
       <c r="E213" s="30">
         <v>4692675.5999999996</v>
       </c>
-      <c r="F213" s="86"/>
-      <c r="G213" s="86"/>
+      <c r="F213" s="57"/>
+      <c r="G213" s="57"/>
       <c r="H213" s="40" t="s">
         <v>8</v>
       </c>
@@ -7042,8 +6752,8 @@
       <c r="E214" s="30">
         <v>4692674.3310000002</v>
       </c>
-      <c r="F214" s="86"/>
-      <c r="G214" s="86"/>
+      <c r="F214" s="57"/>
+      <c r="G214" s="57"/>
       <c r="H214" s="40" t="s">
         <v>8</v>
       </c>
@@ -7063,8 +6773,8 @@
       <c r="E215" s="30">
         <v>4692675.5310000004</v>
       </c>
-      <c r="F215" s="86"/>
-      <c r="G215" s="86"/>
+      <c r="F215" s="57"/>
+      <c r="G215" s="57"/>
       <c r="H215" s="40" t="s">
         <v>8</v>
       </c>
@@ -7084,8 +6794,8 @@
       <c r="E216" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F216" s="86"/>
-      <c r="G216" s="86"/>
+      <c r="F216" s="57"/>
+      <c r="G216" s="57"/>
       <c r="H216" s="40" t="s">
         <v>8</v>
       </c>
@@ -7105,8 +6815,8 @@
       <c r="E217" s="30">
         <v>4692677.4869999997</v>
       </c>
-      <c r="F217" s="86"/>
-      <c r="G217" s="86"/>
+      <c r="F217" s="57"/>
+      <c r="G217" s="57"/>
       <c r="H217" s="40" t="s">
         <v>8</v>
       </c>
@@ -7126,8 +6836,8 @@
       <c r="E218" s="30">
         <v>4692678.7819999997</v>
       </c>
-      <c r="F218" s="86"/>
-      <c r="G218" s="86"/>
+      <c r="F218" s="57"/>
+      <c r="G218" s="57"/>
       <c r="H218" s="40" t="s">
         <v>8</v>
       </c>
@@ -7147,8 +6857,8 @@
       <c r="E219" s="30">
         <v>4692681.2970000003</v>
       </c>
-      <c r="F219" s="86"/>
-      <c r="G219" s="86"/>
+      <c r="F219" s="57"/>
+      <c r="G219" s="57"/>
       <c r="H219" s="40" t="s">
         <v>8</v>
       </c>
@@ -7168,8 +6878,8 @@
       <c r="E220" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F220" s="86"/>
-      <c r="G220" s="86"/>
+      <c r="F220" s="57"/>
+      <c r="G220" s="57"/>
       <c r="H220" s="40" t="s">
         <v>8</v>
       </c>
@@ -7189,8 +6899,8 @@
       <c r="E221" s="30">
         <v>4692687.1791000003</v>
       </c>
-      <c r="F221" s="86"/>
-      <c r="G221" s="86"/>
+      <c r="F221" s="57"/>
+      <c r="G221" s="57"/>
       <c r="H221" s="40" t="s">
         <v>8</v>
       </c>
@@ -7210,8 +6920,8 @@
       <c r="E222" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F222" s="86"/>
-      <c r="G222" s="86"/>
+      <c r="F222" s="57"/>
+      <c r="G222" s="57"/>
       <c r="H222" s="40" t="s">
         <v>8</v>
       </c>
@@ -7231,8 +6941,8 @@
       <c r="E223" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F223" s="86"/>
-      <c r="G223" s="86"/>
+      <c r="F223" s="57"/>
+      <c r="G223" s="57"/>
       <c r="H223" s="40" t="s">
         <v>8</v>
       </c>
@@ -7252,8 +6962,8 @@
       <c r="E224" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F224" s="86"/>
-      <c r="G224" s="86"/>
+      <c r="F224" s="57"/>
+      <c r="G224" s="57"/>
       <c r="H224" s="40" t="s">
         <v>8</v>
       </c>
@@ -7273,8 +6983,8 @@
       <c r="E225" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F225" s="86"/>
-      <c r="G225" s="86"/>
+      <c r="F225" s="57"/>
+      <c r="G225" s="57"/>
       <c r="H225" s="40" t="s">
         <v>8</v>
       </c>
@@ -7294,8 +7004,8 @@
       <c r="E226" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F226" s="86"/>
-      <c r="G226" s="86"/>
+      <c r="F226" s="57"/>
+      <c r="G226" s="57"/>
       <c r="H226" s="40" t="s">
         <v>8</v>
       </c>
@@ -7315,8 +7025,8 @@
       <c r="E227" s="30">
         <v>4692683.9784000004</v>
       </c>
-      <c r="F227" s="86"/>
-      <c r="G227" s="86"/>
+      <c r="F227" s="57"/>
+      <c r="G227" s="57"/>
       <c r="H227" s="40" t="s">
         <v>8</v>
       </c>
@@ -7336,8 +7046,8 @@
       <c r="E228" s="30">
         <v>4692680.5674000001</v>
       </c>
-      <c r="F228" s="86"/>
-      <c r="G228" s="86"/>
+      <c r="F228" s="57"/>
+      <c r="G228" s="57"/>
       <c r="H228" s="40" t="s">
         <v>8</v>
       </c>
@@ -7357,8 +7067,8 @@
       <c r="E229" s="30">
         <v>4692679.6714000003</v>
       </c>
-      <c r="F229" s="86"/>
-      <c r="G229" s="86"/>
+      <c r="F229" s="57"/>
+      <c r="G229" s="57"/>
       <c r="H229" s="40" t="s">
         <v>8</v>
       </c>
@@ -7378,8 +7088,8 @@
       <c r="E230" s="30">
         <v>4692687.4755999995</v>
       </c>
-      <c r="F230" s="86"/>
-      <c r="G230" s="86"/>
+      <c r="F230" s="57"/>
+      <c r="G230" s="57"/>
       <c r="H230" s="40" t="s">
         <v>8</v>
       </c>
@@ -7399,8 +7109,8 @@
       <c r="E231" s="30">
         <v>4692681.2410000004</v>
       </c>
-      <c r="F231" s="86"/>
-      <c r="G231" s="86"/>
+      <c r="F231" s="57"/>
+      <c r="G231" s="57"/>
       <c r="H231" s="40" t="s">
         <v>8</v>
       </c>
@@ -7420,8 +7130,8 @@
       <c r="E232" s="30">
         <v>4692682.2426000005</v>
       </c>
-      <c r="F232" s="86"/>
-      <c r="G232" s="86"/>
+      <c r="F232" s="57"/>
+      <c r="G232" s="57"/>
       <c r="H232" s="40" t="s">
         <v>8</v>
       </c>
@@ -7441,8 +7151,8 @@
       <c r="E233" s="30">
         <v>4692688.4773000004</v>
       </c>
-      <c r="F233" s="86"/>
-      <c r="G233" s="86"/>
+      <c r="F233" s="57"/>
+      <c r="G233" s="57"/>
       <c r="H233" s="40" t="s">
         <v>8</v>
       </c>
@@ -7462,8 +7172,8 @@
       <c r="E234" s="30">
         <v>4692689.9908999996</v>
       </c>
-      <c r="F234" s="86"/>
-      <c r="G234" s="86"/>
+      <c r="F234" s="57"/>
+      <c r="G234" s="57"/>
       <c r="H234" s="40" t="s">
         <v>8</v>
       </c>
@@ -7483,8 +7193,8 @@
       <c r="E235" s="30">
         <v>4692683.7561999997</v>
       </c>
-      <c r="F235" s="86"/>
-      <c r="G235" s="86"/>
+      <c r="F235" s="57"/>
+      <c r="G235" s="57"/>
       <c r="H235" s="40" t="s">
         <v>8</v>
       </c>
@@ -7504,8 +7214,8 @@
       <c r="E236" s="30">
         <v>4692685.3595000003</v>
       </c>
-      <c r="F236" s="86"/>
-      <c r="G236" s="86"/>
+      <c r="F236" s="57"/>
+      <c r="G236" s="57"/>
       <c r="H236" s="40" t="s">
         <v>8</v>
       </c>
@@ -7525,8 +7235,8 @@
       <c r="E237" s="30">
         <v>4692691.5941000003</v>
       </c>
-      <c r="F237" s="86"/>
-      <c r="G237" s="86"/>
+      <c r="F237" s="57"/>
+      <c r="G237" s="57"/>
       <c r="H237" s="40" t="s">
         <v>8</v>
       </c>
@@ -7546,8 +7256,8 @@
       <c r="E238" s="30">
         <v>4692693.0789000001</v>
       </c>
-      <c r="F238" s="86"/>
-      <c r="G238" s="86"/>
+      <c r="F238" s="57"/>
+      <c r="G238" s="57"/>
       <c r="H238" s="40" t="s">
         <v>8</v>
       </c>
@@ -7567,8 +7277,8 @@
       <c r="E239" s="30">
         <v>4692686.8443</v>
       </c>
-      <c r="F239" s="86"/>
-      <c r="G239" s="86"/>
+      <c r="F239" s="57"/>
+      <c r="G239" s="57"/>
       <c r="H239" s="40" t="s">
         <v>8</v>
       </c>
@@ -7588,8 +7298,8 @@
       <c r="E240" s="30">
         <v>4692689.7762000002</v>
       </c>
-      <c r="F240" s="86"/>
-      <c r="G240" s="86"/>
+      <c r="F240" s="57"/>
+      <c r="G240" s="57"/>
       <c r="H240" s="40" t="s">
         <v>8</v>
       </c>
@@ -7609,8 +7319,8 @@
       <c r="E241" s="30">
         <v>4692687.6679999996</v>
       </c>
-      <c r="F241" s="86"/>
-      <c r="G241" s="86"/>
+      <c r="F241" s="57"/>
+      <c r="G241" s="57"/>
       <c r="H241" s="40" t="s">
         <v>8</v>
       </c>
@@ -7630,8 +7340,8 @@
       <c r="E242" s="30">
         <v>4692690.4787999997</v>
       </c>
-      <c r="F242" s="86"/>
-      <c r="G242" s="86"/>
+      <c r="F242" s="57"/>
+      <c r="G242" s="57"/>
       <c r="H242" s="40" t="s">
         <v>8</v>
       </c>
@@ -7651,8 +7361,8 @@
       <c r="E243" s="30">
         <v>4692688.38</v>
       </c>
-      <c r="F243" s="86"/>
-      <c r="G243" s="86"/>
+      <c r="F243" s="57"/>
+      <c r="G243" s="57"/>
       <c r="H243" s="40" t="s">
         <v>8</v>
       </c>
@@ -7672,8 +7382,8 @@
       <c r="E244" s="30">
         <v>4692685.5033</v>
       </c>
-      <c r="F244" s="86"/>
-      <c r="G244" s="86"/>
+      <c r="F244" s="57"/>
+      <c r="G244" s="57"/>
       <c r="H244" s="40" t="s">
         <v>8</v>
       </c>
@@ -7693,8 +7403,8 @@
       <c r="E245" s="30">
         <v>4692686.4769000001</v>
       </c>
-      <c r="F245" s="86"/>
-      <c r="G245" s="86"/>
+      <c r="F245" s="57"/>
+      <c r="G245" s="57"/>
       <c r="H245" s="40" t="s">
         <v>8</v>
       </c>
@@ -7714,8 +7424,8 @@
       <c r="E246" s="30">
         <v>4692680.3293000003</v>
       </c>
-      <c r="F246" s="86"/>
-      <c r="G246" s="86"/>
+      <c r="F246" s="57"/>
+      <c r="G246" s="57"/>
       <c r="H246" s="40" t="s">
         <v>8</v>
       </c>
@@ -7735,8 +7445,8 @@
       <c r="E247" s="30">
         <v>4692685.9365999997</v>
       </c>
-      <c r="F247" s="86"/>
-      <c r="G247" s="86"/>
+      <c r="F247" s="57"/>
+      <c r="G247" s="57"/>
       <c r="H247" s="40" t="s">
         <v>8</v>
       </c>
@@ -7756,8 +7466,8 @@
       <c r="E248" s="30">
         <v>4692684.2878</v>
       </c>
-      <c r="F248" s="86"/>
-      <c r="G248" s="86"/>
+      <c r="F248" s="57"/>
+      <c r="G248" s="57"/>
       <c r="H248" s="40" t="s">
         <v>8</v>
       </c>
@@ -7777,8 +7487,8 @@
       <c r="E249" s="30">
         <v>4692677.3678000001</v>
       </c>
-      <c r="F249" s="86"/>
-      <c r="G249" s="86"/>
+      <c r="F249" s="57"/>
+      <c r="G249" s="57"/>
       <c r="H249" s="40" t="s">
         <v>8</v>
       </c>
@@ -7798,8 +7508,8 @@
       <c r="E250" s="30">
         <v>4692675.551</v>
       </c>
-      <c r="F250" s="86"/>
-      <c r="G250" s="86"/>
+      <c r="F250" s="57"/>
+      <c r="G250" s="57"/>
       <c r="H250" s="40" t="s">
         <v>8</v>
       </c>
@@ -7819,8 +7529,8 @@
       <c r="E251" s="30">
         <v>4692682.6838999996</v>
       </c>
-      <c r="F251" s="86"/>
-      <c r="G251" s="86"/>
+      <c r="F251" s="57"/>
+      <c r="G251" s="57"/>
       <c r="H251" s="40" t="s">
         <v>8</v>
       </c>
@@ -7840,8 +7550,8 @@
       <c r="E252" s="30">
         <v>4692681.1698000003</v>
       </c>
-      <c r="F252" s="86"/>
-      <c r="G252" s="86"/>
+      <c r="F252" s="57"/>
+      <c r="G252" s="57"/>
       <c r="H252" s="40" t="s">
         <v>8</v>
       </c>
@@ -7859,8 +7569,8 @@
       <c r="E253" s="30">
         <v>4692679.5367999999</v>
       </c>
-      <c r="F253" s="86"/>
-      <c r="G253" s="86"/>
+      <c r="F253" s="57"/>
+      <c r="G253" s="57"/>
       <c r="H253" s="40" t="s">
         <v>8</v>
       </c>
@@ -7875,8 +7585,8 @@
       <c r="E254" s="30">
         <v>4692678.6008000001</v>
       </c>
-      <c r="F254" s="86"/>
-      <c r="G254" s="86"/>
+      <c r="F254" s="57"/>
+      <c r="G254" s="57"/>
       <c r="H254" s="40" t="s">
         <v>8</v>
       </c>
@@ -7893,8 +7603,8 @@
       <c r="E255" s="30">
         <v>4692673.9884000001</v>
       </c>
-      <c r="F255" s="86"/>
-      <c r="G255" s="86"/>
+      <c r="F255" s="57"/>
+      <c r="G255" s="57"/>
       <c r="H255" s="40" t="s">
         <v>8</v>
       </c>
@@ -7914,8 +7624,8 @@
       <c r="E256" s="42">
         <v>4692673.2940999996</v>
       </c>
-      <c r="F256" s="87"/>
-      <c r="G256" s="87"/>
+      <c r="F256" s="58"/>
+      <c r="G256" s="58"/>
       <c r="H256" s="43" t="s">
         <v>20</v>
       </c>
@@ -7930,34 +7640,34 @@
       <c r="B257" s="3"/>
       <c r="C257" s="35"/>
       <c r="D257" s="35"/>
-      <c r="E257" s="82" t="s">
+      <c r="E257" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="F257" s="83"/>
-      <c r="G257" s="84"/>
-      <c r="H257" s="81" t="s">
+      <c r="F257" s="84"/>
+      <c r="G257" s="85"/>
+      <c r="H257" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="I257" s="68"/>
-      <c r="J257" s="71"/>
-      <c r="K257" s="72"/>
+      <c r="I257" s="64"/>
+      <c r="J257" s="67"/>
+      <c r="K257" s="68"/>
     </row>
     <row r="258" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="75" t="s">
+      <c r="A258" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B258" s="76"/>
-      <c r="C258" s="76"/>
-      <c r="D258" s="77"/>
-      <c r="E258" s="78">
+      <c r="B258" s="72"/>
+      <c r="C258" s="72"/>
+      <c r="D258" s="73"/>
+      <c r="E258" s="74">
         <v>140</v>
       </c>
-      <c r="F258" s="79"/>
-      <c r="G258" s="80"/>
-      <c r="H258" s="69"/>
-      <c r="I258" s="70"/>
-      <c r="J258" s="73"/>
-      <c r="K258" s="74"/>
+      <c r="F258" s="75"/>
+      <c r="G258" s="76"/>
+      <c r="H258" s="65"/>
+      <c r="I258" s="66"/>
+      <c r="J258" s="69"/>
+      <c r="K258" s="70"/>
     </row>
     <row r="259" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A259" s="1"/>
@@ -7973,117 +7683,117 @@
       <c r="K259" s="1"/>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A260" s="46"/>
-      <c r="B260" s="46"/>
-      <c r="C260" s="46"/>
-      <c r="D260" s="46"/>
-      <c r="E260" s="46"/>
-      <c r="F260" s="46"/>
-      <c r="G260" s="46"/>
-      <c r="H260" s="46"/>
-      <c r="I260" s="46"/>
-      <c r="J260" s="46"/>
-      <c r="K260" s="46"/>
+      <c r="A260" s="48"/>
+      <c r="B260" s="48"/>
+      <c r="C260" s="48"/>
+      <c r="D260" s="48"/>
+      <c r="E260" s="48"/>
+      <c r="F260" s="48"/>
+      <c r="G260" s="48"/>
+      <c r="H260" s="48"/>
+      <c r="I260" s="48"/>
+      <c r="J260" s="48"/>
+      <c r="K260" s="48"/>
     </row>
     <row r="261" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="46"/>
-      <c r="B261" s="46"/>
-      <c r="C261" s="46"/>
-      <c r="D261" s="46"/>
-      <c r="E261" s="46"/>
-      <c r="F261" s="46"/>
-      <c r="G261" s="46"/>
-      <c r="H261" s="46"/>
-      <c r="I261" s="46"/>
-      <c r="J261" s="46"/>
-      <c r="K261" s="46"/>
+      <c r="A261" s="48"/>
+      <c r="B261" s="48"/>
+      <c r="C261" s="48"/>
+      <c r="D261" s="48"/>
+      <c r="E261" s="48"/>
+      <c r="F261" s="48"/>
+      <c r="G261" s="48"/>
+      <c r="H261" s="48"/>
+      <c r="I261" s="48"/>
+      <c r="J261" s="48"/>
+      <c r="K261" s="48"/>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A262" s="47" t="s">
+      <c r="A262" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B262" s="47"/>
-      <c r="C262" s="47"/>
-      <c r="D262" s="47"/>
-      <c r="E262" s="47"/>
-      <c r="F262" s="47"/>
-      <c r="G262" s="47"/>
-      <c r="H262" s="47"/>
-      <c r="I262" s="47"/>
-      <c r="J262" s="47"/>
-      <c r="K262" s="47"/>
+      <c r="B262" s="49"/>
+      <c r="C262" s="49"/>
+      <c r="D262" s="49"/>
+      <c r="E262" s="49"/>
+      <c r="F262" s="49"/>
+      <c r="G262" s="49"/>
+      <c r="H262" s="49"/>
+      <c r="I262" s="49"/>
+      <c r="J262" s="49"/>
+      <c r="K262" s="49"/>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A263" s="47"/>
-      <c r="B263" s="47"/>
-      <c r="C263" s="47"/>
-      <c r="D263" s="47"/>
-      <c r="E263" s="47"/>
-      <c r="F263" s="47"/>
-      <c r="G263" s="47"/>
-      <c r="H263" s="47"/>
-      <c r="I263" s="47"/>
-      <c r="J263" s="47"/>
-      <c r="K263" s="47"/>
+      <c r="A263" s="49"/>
+      <c r="B263" s="49"/>
+      <c r="C263" s="49"/>
+      <c r="D263" s="49"/>
+      <c r="E263" s="49"/>
+      <c r="F263" s="49"/>
+      <c r="G263" s="49"/>
+      <c r="H263" s="49"/>
+      <c r="I263" s="49"/>
+      <c r="J263" s="49"/>
+      <c r="K263" s="49"/>
     </row>
     <row r="264" spans="1:11" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="47"/>
-      <c r="B264" s="47"/>
-      <c r="C264" s="47"/>
-      <c r="D264" s="47"/>
-      <c r="E264" s="47"/>
-      <c r="F264" s="47"/>
-      <c r="G264" s="47"/>
-      <c r="H264" s="47"/>
-      <c r="I264" s="47"/>
-      <c r="J264" s="47"/>
-      <c r="K264" s="47"/>
+      <c r="A264" s="49"/>
+      <c r="B264" s="49"/>
+      <c r="C264" s="49"/>
+      <c r="D264" s="49"/>
+      <c r="E264" s="49"/>
+      <c r="F264" s="49"/>
+      <c r="G264" s="49"/>
+      <c r="H264" s="49"/>
+      <c r="I264" s="49"/>
+      <c r="J264" s="49"/>
+      <c r="K264" s="49"/>
     </row>
     <row r="265" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="47"/>
-      <c r="B265" s="47"/>
-      <c r="C265" s="47"/>
-      <c r="D265" s="47"/>
-      <c r="E265" s="47"/>
-      <c r="F265" s="47"/>
-      <c r="G265" s="47"/>
-      <c r="H265" s="47"/>
-      <c r="I265" s="47"/>
-      <c r="J265" s="47"/>
-      <c r="K265" s="47"/>
+      <c r="A265" s="49"/>
+      <c r="B265" s="49"/>
+      <c r="C265" s="49"/>
+      <c r="D265" s="49"/>
+      <c r="E265" s="49"/>
+      <c r="F265" s="49"/>
+      <c r="G265" s="49"/>
+      <c r="H265" s="49"/>
+      <c r="I265" s="49"/>
+      <c r="J265" s="49"/>
+      <c r="K265" s="49"/>
     </row>
     <row r="266" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A266" s="1"/>
-      <c r="C266" s="48"/>
-      <c r="D266" s="49"/>
-      <c r="E266" s="49"/>
-      <c r="F266" s="49"/>
-      <c r="G266" s="49"/>
-      <c r="H266" s="49"/>
-      <c r="I266" s="50"/>
+      <c r="C266" s="50"/>
+      <c r="D266" s="51"/>
+      <c r="E266" s="51"/>
+      <c r="F266" s="51"/>
+      <c r="G266" s="51"/>
+      <c r="H266" s="51"/>
+      <c r="I266" s="52"/>
       <c r="J266" s="1"/>
       <c r="K266" s="1"/>
     </row>
     <row r="267" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A267" s="1"/>
-      <c r="C267" s="51"/>
-      <c r="D267" s="52"/>
-      <c r="E267" s="52"/>
-      <c r="F267" s="52"/>
-      <c r="G267" s="52"/>
-      <c r="H267" s="52"/>
-      <c r="I267" s="53"/>
+      <c r="C267" s="53"/>
+      <c r="D267" s="54"/>
+      <c r="E267" s="54"/>
+      <c r="F267" s="54"/>
+      <c r="G267" s="54"/>
+      <c r="H267" s="54"/>
+      <c r="I267" s="55"/>
       <c r="J267" s="1"/>
       <c r="K267" s="1"/>
     </row>
     <row r="268" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A268" s="1"/>
-      <c r="C268" s="54"/>
-      <c r="D268" s="55"/>
-      <c r="E268" s="55"/>
-      <c r="F268" s="55"/>
-      <c r="G268" s="55"/>
-      <c r="H268" s="55"/>
+      <c r="C268" s="77"/>
+      <c r="D268" s="78"/>
+      <c r="E268" s="78"/>
+      <c r="F268" s="78"/>
+      <c r="G268" s="78"/>
+      <c r="H268" s="78"/>
       <c r="I268" s="56"/>
       <c r="J268" s="1"/>
       <c r="K268" s="1"/>
@@ -8138,11 +7848,11 @@
       <c r="E271" s="30">
         <v>4692673.5029999996</v>
       </c>
-      <c r="F271" s="61">
+      <c r="F271" s="79">
         <v>625.72</v>
       </c>
-      <c r="G271" s="58" t="s">
-        <v>26</v>
+      <c r="G271" s="86" t="s">
+        <v>25</v>
       </c>
       <c r="H271" s="45" t="s">
         <v>8</v>
@@ -8163,8 +7873,8 @@
       <c r="E272" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F272" s="62"/>
-      <c r="G272" s="59"/>
+      <c r="F272" s="80"/>
+      <c r="G272" s="87"/>
       <c r="H272" s="45" t="s">
         <v>8</v>
       </c>
@@ -8184,8 +7894,8 @@
       <c r="E273" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F273" s="62"/>
-      <c r="G273" s="59"/>
+      <c r="F273" s="80"/>
+      <c r="G273" s="87"/>
       <c r="H273" s="45" t="s">
         <v>8</v>
       </c>
@@ -8205,8 +7915,8 @@
       <c r="E274" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F274" s="62"/>
-      <c r="G274" s="59"/>
+      <c r="F274" s="80"/>
+      <c r="G274" s="87"/>
       <c r="H274" s="45" t="s">
         <v>8</v>
       </c>
@@ -8226,8 +7936,8 @@
       <c r="E275" s="30">
         <v>4692674.3839999996</v>
       </c>
-      <c r="F275" s="62"/>
-      <c r="G275" s="59"/>
+      <c r="F275" s="80"/>
+      <c r="G275" s="87"/>
       <c r="H275" s="45" t="s">
         <v>8</v>
       </c>
@@ -8247,8 +7957,8 @@
       <c r="E276" s="30">
         <v>4692677.5640000002</v>
       </c>
-      <c r="F276" s="62"/>
-      <c r="G276" s="59"/>
+      <c r="F276" s="80"/>
+      <c r="G276" s="87"/>
       <c r="H276" s="45" t="s">
         <v>8</v>
       </c>
@@ -8268,8 +7978,8 @@
       <c r="E277" s="30">
         <v>4692679.0279999999</v>
       </c>
-      <c r="F277" s="62"/>
-      <c r="G277" s="59"/>
+      <c r="F277" s="80"/>
+      <c r="G277" s="87"/>
       <c r="H277" s="45" t="s">
         <v>8</v>
       </c>
@@ -8289,8 +7999,8 @@
       <c r="E278" s="30">
         <v>4692680.25</v>
       </c>
-      <c r="F278" s="62"/>
-      <c r="G278" s="59"/>
+      <c r="F278" s="80"/>
+      <c r="G278" s="87"/>
       <c r="H278" s="45" t="s">
         <v>8</v>
       </c>
@@ -8310,8 +8020,8 @@
       <c r="E279" s="30">
         <v>4692673.0663999999</v>
       </c>
-      <c r="F279" s="62"/>
-      <c r="G279" s="59"/>
+      <c r="F279" s="80"/>
+      <c r="G279" s="87"/>
       <c r="H279" s="45" t="s">
         <v>8</v>
       </c>
@@ -8331,8 +8041,8 @@
       <c r="E280" s="30">
         <v>4692675.5999999996</v>
       </c>
-      <c r="F280" s="62"/>
-      <c r="G280" s="59"/>
+      <c r="F280" s="80"/>
+      <c r="G280" s="87"/>
       <c r="H280" s="45" t="s">
         <v>8</v>
       </c>
@@ -8352,8 +8062,8 @@
       <c r="E281" s="30">
         <v>4692674.3310000002</v>
       </c>
-      <c r="F281" s="62"/>
-      <c r="G281" s="59"/>
+      <c r="F281" s="80"/>
+      <c r="G281" s="87"/>
       <c r="H281" s="45" t="s">
         <v>8</v>
       </c>
@@ -8373,8 +8083,8 @@
       <c r="E282" s="30">
         <v>4692675.5310000004</v>
       </c>
-      <c r="F282" s="62"/>
-      <c r="G282" s="59"/>
+      <c r="F282" s="80"/>
+      <c r="G282" s="87"/>
       <c r="H282" s="45" t="s">
         <v>8</v>
       </c>
@@ -8394,8 +8104,8 @@
       <c r="E283" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F283" s="62"/>
-      <c r="G283" s="59"/>
+      <c r="F283" s="80"/>
+      <c r="G283" s="87"/>
       <c r="H283" s="45" t="s">
         <v>8</v>
       </c>
@@ -8415,8 +8125,8 @@
       <c r="E284" s="30">
         <v>4692677.4869999997</v>
       </c>
-      <c r="F284" s="62"/>
-      <c r="G284" s="59"/>
+      <c r="F284" s="80"/>
+      <c r="G284" s="87"/>
       <c r="H284" s="45" t="s">
         <v>8</v>
       </c>
@@ -8436,8 +8146,8 @@
       <c r="E285" s="30">
         <v>4692678.7819999997</v>
       </c>
-      <c r="F285" s="62"/>
-      <c r="G285" s="59"/>
+      <c r="F285" s="80"/>
+      <c r="G285" s="87"/>
       <c r="H285" s="45" t="s">
         <v>8</v>
       </c>
@@ -8457,8 +8167,8 @@
       <c r="E286" s="30">
         <v>4692681.2970000003</v>
       </c>
-      <c r="F286" s="62"/>
-      <c r="G286" s="59"/>
+      <c r="F286" s="80"/>
+      <c r="G286" s="87"/>
       <c r="H286" s="45" t="s">
         <v>8</v>
       </c>
@@ -8478,8 +8188,8 @@
       <c r="E287" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F287" s="62"/>
-      <c r="G287" s="59"/>
+      <c r="F287" s="80"/>
+      <c r="G287" s="87"/>
       <c r="H287" s="45" t="s">
         <v>8</v>
       </c>
@@ -8499,8 +8209,8 @@
       <c r="E288" s="30">
         <v>4692687.1791000003</v>
       </c>
-      <c r="F288" s="62"/>
-      <c r="G288" s="59"/>
+      <c r="F288" s="80"/>
+      <c r="G288" s="87"/>
       <c r="H288" s="45" t="s">
         <v>8</v>
       </c>
@@ -8520,8 +8230,8 @@
       <c r="E289" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F289" s="62"/>
-      <c r="G289" s="59"/>
+      <c r="F289" s="80"/>
+      <c r="G289" s="87"/>
       <c r="H289" s="45" t="s">
         <v>8</v>
       </c>
@@ -8541,8 +8251,8 @@
       <c r="E290" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F290" s="62"/>
-      <c r="G290" s="59"/>
+      <c r="F290" s="80"/>
+      <c r="G290" s="87"/>
       <c r="H290" s="45" t="s">
         <v>8</v>
       </c>
@@ -8562,8 +8272,8 @@
       <c r="E291" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F291" s="62"/>
-      <c r="G291" s="59"/>
+      <c r="F291" s="80"/>
+      <c r="G291" s="87"/>
       <c r="H291" s="45" t="s">
         <v>8</v>
       </c>
@@ -8583,8 +8293,8 @@
       <c r="E292" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F292" s="62"/>
-      <c r="G292" s="59"/>
+      <c r="F292" s="80"/>
+      <c r="G292" s="87"/>
       <c r="H292" s="45" t="s">
         <v>8</v>
       </c>
@@ -8604,8 +8314,8 @@
       <c r="E293" s="30">
         <v>4692689.9910000004</v>
       </c>
-      <c r="F293" s="62"/>
-      <c r="G293" s="59"/>
+      <c r="F293" s="80"/>
+      <c r="G293" s="87"/>
       <c r="H293" s="45" t="s">
         <v>8</v>
       </c>
@@ -8625,8 +8335,8 @@
       <c r="E294" s="30">
         <v>4692691.5941000003</v>
       </c>
-      <c r="F294" s="62"/>
-      <c r="G294" s="59"/>
+      <c r="F294" s="80"/>
+      <c r="G294" s="87"/>
       <c r="H294" s="45" t="s">
         <v>8</v>
       </c>
@@ -8646,8 +8356,8 @@
       <c r="E295" s="30">
         <v>4692685.3595000003</v>
       </c>
-      <c r="F295" s="62"/>
-      <c r="G295" s="59"/>
+      <c r="F295" s="80"/>
+      <c r="G295" s="87"/>
       <c r="H295" s="45" t="s">
         <v>8</v>
       </c>
@@ -8667,8 +8377,8 @@
       <c r="E296" s="30">
         <v>4692683.7562999995</v>
       </c>
-      <c r="F296" s="62"/>
-      <c r="G296" s="59"/>
+      <c r="F296" s="80"/>
+      <c r="G296" s="87"/>
       <c r="H296" s="45" t="s">
         <v>8</v>
       </c>
@@ -8688,8 +8398,8 @@
       <c r="E297" s="30">
         <v>4692680.5674000001</v>
       </c>
-      <c r="F297" s="62"/>
-      <c r="G297" s="59"/>
+      <c r="F297" s="80"/>
+      <c r="G297" s="87"/>
       <c r="H297" s="45" t="s">
         <v>8</v>
       </c>
@@ -8709,8 +8419,8 @@
       <c r="E298" s="30">
         <v>4692683.9784000004</v>
       </c>
-      <c r="F298" s="62"/>
-      <c r="G298" s="59"/>
+      <c r="F298" s="80"/>
+      <c r="G298" s="87"/>
       <c r="H298" s="45" t="s">
         <v>8</v>
       </c>
@@ -8730,8 +8440,8 @@
       <c r="E299" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F299" s="62"/>
-      <c r="G299" s="59"/>
+      <c r="F299" s="80"/>
+      <c r="G299" s="87"/>
       <c r="H299" s="45" t="s">
         <v>8</v>
       </c>
@@ -8751,8 +8461,8 @@
       <c r="E300" s="30">
         <v>4692679.6714000003</v>
       </c>
-      <c r="F300" s="62"/>
-      <c r="G300" s="59"/>
+      <c r="F300" s="80"/>
+      <c r="G300" s="87"/>
       <c r="H300" s="45" t="s">
         <v>8</v>
       </c>
@@ -8772,8 +8482,8 @@
       <c r="E301" s="30">
         <v>4692678.2399000004</v>
       </c>
-      <c r="F301" s="62"/>
-      <c r="G301" s="59"/>
+      <c r="F301" s="80"/>
+      <c r="G301" s="87"/>
       <c r="H301" s="45" t="s">
         <v>8</v>
       </c>
@@ -8793,8 +8503,8 @@
       <c r="E302" s="30">
         <v>4692682.3244000003</v>
       </c>
-      <c r="F302" s="62"/>
-      <c r="G302" s="59"/>
+      <c r="F302" s="80"/>
+      <c r="G302" s="87"/>
       <c r="H302" s="45" t="s">
         <v>8</v>
       </c>
@@ -8814,8 +8524,8 @@
       <c r="E303" s="30">
         <v>4692683.8091000002</v>
       </c>
-      <c r="F303" s="62"/>
-      <c r="G303" s="59"/>
+      <c r="F303" s="80"/>
+      <c r="G303" s="87"/>
       <c r="H303" s="45" t="s">
         <v>8</v>
       </c>
@@ -8835,8 +8545,8 @@
       <c r="E304" s="30">
         <v>4692683.9275000002</v>
       </c>
-      <c r="F304" s="62"/>
-      <c r="G304" s="59"/>
+      <c r="F304" s="80"/>
+      <c r="G304" s="87"/>
       <c r="H304" s="45" t="s">
         <v>8</v>
       </c>
@@ -8856,8 +8566,8 @@
       <c r="E305" s="30">
         <v>4692686.4386999998</v>
       </c>
-      <c r="F305" s="62"/>
-      <c r="G305" s="59"/>
+      <c r="F305" s="80"/>
+      <c r="G305" s="87"/>
       <c r="H305" s="45" t="s">
         <v>8</v>
       </c>
@@ -8877,8 +8587,8 @@
       <c r="E306" s="30">
         <v>4692675.5519000003</v>
       </c>
-      <c r="F306" s="63"/>
-      <c r="G306" s="59"/>
+      <c r="F306" s="81"/>
+      <c r="G306" s="87"/>
       <c r="H306" s="45" t="s">
         <v>8</v>
       </c>
@@ -8901,7 +8611,7 @@
       <c r="F307" s="34">
         <v>616.38300000000004</v>
       </c>
-      <c r="G307" s="60"/>
+      <c r="G307" s="88"/>
       <c r="H307" s="45" t="s">
         <v>20</v>
       </c>
@@ -8925,28 +8635,28 @@
     <row r="309" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
-      <c r="C309" s="57" t="s">
+      <c r="C309" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="D309" s="57"/>
-      <c r="E309" s="57"/>
-      <c r="F309" s="57"/>
-      <c r="G309" s="57"/>
-      <c r="H309" s="57"/>
-      <c r="I309" s="57"/>
+      <c r="D309" s="59"/>
+      <c r="E309" s="59"/>
+      <c r="F309" s="59"/>
+      <c r="G309" s="59"/>
+      <c r="H309" s="59"/>
+      <c r="I309" s="59"/>
       <c r="J309" s="1"/>
       <c r="K309" s="1"/>
     </row>
     <row r="310" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
-      <c r="C310" s="57"/>
-      <c r="D310" s="57"/>
-      <c r="E310" s="57"/>
-      <c r="F310" s="57"/>
-      <c r="G310" s="57"/>
-      <c r="H310" s="57"/>
-      <c r="I310" s="57"/>
+      <c r="C310" s="59"/>
+      <c r="D310" s="59"/>
+      <c r="E310" s="59"/>
+      <c r="F310" s="59"/>
+      <c r="G310" s="59"/>
+      <c r="H310" s="59"/>
+      <c r="I310" s="59"/>
       <c r="J310" s="1"/>
       <c r="K310" s="1"/>
     </row>
@@ -9022,62 +8732,50 @@
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
-      <c r="E316" s="64" t="s">
+      <c r="E316" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F316" s="65"/>
-      <c r="G316" s="66"/>
-      <c r="H316" s="67" t="s">
+      <c r="F316" s="61"/>
+      <c r="G316" s="62"/>
+      <c r="H316" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I316" s="68"/>
-      <c r="J316" s="71"/>
-      <c r="K316" s="72"/>
+      <c r="I316" s="64"/>
+      <c r="J316" s="67"/>
+      <c r="K316" s="68"/>
     </row>
     <row r="317" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A317" s="75" t="s">
+      <c r="A317" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B317" s="76"/>
-      <c r="C317" s="76"/>
-      <c r="D317" s="77"/>
-      <c r="E317" s="78">
+      <c r="B317" s="72"/>
+      <c r="C317" s="72"/>
+      <c r="D317" s="73"/>
+      <c r="E317" s="74">
         <v>140</v>
       </c>
-      <c r="F317" s="79"/>
-      <c r="G317" s="80"/>
-      <c r="H317" s="69"/>
-      <c r="I317" s="70"/>
-      <c r="J317" s="73"/>
-      <c r="K317" s="74"/>
+      <c r="F317" s="75"/>
+      <c r="G317" s="76"/>
+      <c r="H317" s="65"/>
+      <c r="I317" s="66"/>
+      <c r="J317" s="69"/>
+      <c r="K317" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G36:G55"/>
-    <mergeCell ref="A194:K195"/>
-    <mergeCell ref="A196:K199"/>
-    <mergeCell ref="C200:I202"/>
-    <mergeCell ref="G204:G256"/>
-    <mergeCell ref="F204:F256"/>
-    <mergeCell ref="C182:I183"/>
-    <mergeCell ref="E192:G192"/>
-    <mergeCell ref="H192:I193"/>
-    <mergeCell ref="J192:K193"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="E193:G193"/>
-    <mergeCell ref="C120:I121"/>
-    <mergeCell ref="C7:I9"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="B61:H62"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:I65"/>
-    <mergeCell ref="J64:K65"/>
-    <mergeCell ref="F77:F110"/>
-    <mergeCell ref="G77:G110"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="A66:K67"/>
+    <mergeCell ref="G77:G112"/>
+    <mergeCell ref="F77:F112"/>
+    <mergeCell ref="A260:K261"/>
+    <mergeCell ref="A262:K265"/>
+    <mergeCell ref="C266:I268"/>
+    <mergeCell ref="C309:I310"/>
+    <mergeCell ref="G271:G307"/>
+    <mergeCell ref="F271:F306"/>
+    <mergeCell ref="E316:G316"/>
+    <mergeCell ref="H316:I317"/>
+    <mergeCell ref="J316:K317"/>
+    <mergeCell ref="A317:D317"/>
+    <mergeCell ref="E317:G317"/>
     <mergeCell ref="A68:K71"/>
     <mergeCell ref="C72:I74"/>
     <mergeCell ref="H257:I258"/>
@@ -9094,17 +8792,29 @@
     <mergeCell ref="A132:K133"/>
     <mergeCell ref="E128:G128"/>
     <mergeCell ref="C139:I141"/>
-    <mergeCell ref="E316:G316"/>
-    <mergeCell ref="H316:I317"/>
-    <mergeCell ref="J316:K317"/>
-    <mergeCell ref="A317:D317"/>
-    <mergeCell ref="E317:G317"/>
-    <mergeCell ref="A260:K261"/>
-    <mergeCell ref="A262:K265"/>
-    <mergeCell ref="C266:I268"/>
-    <mergeCell ref="C309:I310"/>
-    <mergeCell ref="G271:G307"/>
-    <mergeCell ref="F271:F306"/>
+    <mergeCell ref="C7:I9"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="B61:H62"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:I65"/>
+    <mergeCell ref="J64:K65"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="G36:G55"/>
+    <mergeCell ref="A194:K195"/>
+    <mergeCell ref="A196:K199"/>
+    <mergeCell ref="C200:I202"/>
+    <mergeCell ref="G204:G256"/>
+    <mergeCell ref="F204:F256"/>
+    <mergeCell ref="C182:I183"/>
+    <mergeCell ref="E192:G192"/>
+    <mergeCell ref="H192:I193"/>
+    <mergeCell ref="J192:K193"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="E193:G193"/>
+    <mergeCell ref="C120:I121"/>
+    <mergeCell ref="A66:K67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
kati 1 njesite permirsim i njesive
</commit_message>
<xml_diff>
--- a/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
+++ b/5-Njësite-banesore/regjistri/22-Koordinatat-për-pjesë-të-ndertesës.xlsx-Dior.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="26">
   <si>
     <t>Nr</t>
   </si>
@@ -636,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -762,7 +762,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -789,17 +798,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -852,21 +870,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -879,13 +882,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2804,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K317"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A260" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="D84" sqref="C76:H112"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A130" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="D145" sqref="C143:H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,111 +2824,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="53"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="77"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="56"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="61"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3542,7 +3545,7 @@
       <c r="F36" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G36" s="47" t="s">
+      <c r="G36" s="87" t="s">
         <v>22</v>
       </c>
       <c r="H36" s="30" t="s">
@@ -3566,7 +3569,7 @@
       <c r="F37" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G37" s="47"/>
+      <c r="G37" s="87"/>
       <c r="H37" s="30" t="s">
         <v>8</v>
       </c>
@@ -3588,7 +3591,7 @@
       <c r="F38" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G38" s="47"/>
+      <c r="G38" s="87"/>
       <c r="H38" s="30" t="s">
         <v>8</v>
       </c>
@@ -3610,7 +3613,7 @@
       <c r="F39" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G39" s="47"/>
+      <c r="G39" s="87"/>
       <c r="H39" s="30" t="s">
         <v>8</v>
       </c>
@@ -3632,7 +3635,7 @@
       <c r="F40" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G40" s="47"/>
+      <c r="G40" s="87"/>
       <c r="H40" s="30" t="s">
         <v>8</v>
       </c>
@@ -3654,7 +3657,7 @@
       <c r="F41" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G41" s="47"/>
+      <c r="G41" s="87"/>
       <c r="H41" s="30" t="s">
         <v>8</v>
       </c>
@@ -3676,7 +3679,7 @@
       <c r="F42" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G42" s="47"/>
+      <c r="G42" s="87"/>
       <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
@@ -3698,7 +3701,7 @@
       <c r="F43" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G43" s="47"/>
+      <c r="G43" s="87"/>
       <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
@@ -3720,7 +3723,7 @@
       <c r="F44" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G44" s="47"/>
+      <c r="G44" s="87"/>
       <c r="H44" s="30" t="s">
         <v>8</v>
       </c>
@@ -3743,7 +3746,7 @@
       <c r="F45" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G45" s="47"/>
+      <c r="G45" s="87"/>
       <c r="H45" s="30" t="s">
         <v>8</v>
       </c>
@@ -3766,7 +3769,7 @@
       <c r="F46" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G46" s="47"/>
+      <c r="G46" s="87"/>
       <c r="H46" s="30" t="s">
         <v>8</v>
       </c>
@@ -3787,7 +3790,7 @@
       <c r="F47" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G47" s="47"/>
+      <c r="G47" s="87"/>
       <c r="H47" s="30" t="s">
         <v>8</v>
       </c>
@@ -3806,7 +3809,7 @@
       <c r="F48" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G48" s="47"/>
+      <c r="G48" s="87"/>
       <c r="H48" s="30" t="s">
         <v>8</v>
       </c>
@@ -3827,7 +3830,7 @@
       <c r="F49" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G49" s="47"/>
+      <c r="G49" s="87"/>
       <c r="H49" s="30" t="s">
         <v>8</v>
       </c>
@@ -3850,7 +3853,7 @@
       <c r="F50" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G50" s="47"/>
+      <c r="G50" s="87"/>
       <c r="H50" s="30" t="s">
         <v>8</v>
       </c>
@@ -3873,7 +3876,7 @@
       <c r="F51" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G51" s="47"/>
+      <c r="G51" s="87"/>
       <c r="H51" s="30" t="s">
         <v>8</v>
       </c>
@@ -3895,7 +3898,7 @@
       <c r="F52" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G52" s="47"/>
+      <c r="G52" s="87"/>
       <c r="H52" s="30" t="s">
         <v>8</v>
       </c>
@@ -3917,7 +3920,7 @@
       <c r="F53" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G53" s="47"/>
+      <c r="G53" s="87"/>
       <c r="H53" s="30" t="s">
         <v>8</v>
       </c>
@@ -3940,7 +3943,7 @@
       <c r="F54" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G54" s="47"/>
+      <c r="G54" s="87"/>
       <c r="H54" s="9" t="s">
         <v>20</v>
       </c>
@@ -3963,7 +3966,7 @@
       <c r="F55" s="8">
         <v>611.86699999999996</v>
       </c>
-      <c r="G55" s="47"/>
+      <c r="G55" s="87"/>
       <c r="H55" s="9" t="s">
         <v>20</v>
       </c>
@@ -4012,27 +4015,27 @@
     </row>
     <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="59" t="s">
+      <c r="B61" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
       <c r="I61" s="11"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="59"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="62"/>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62"/>
     </row>
     <row r="63" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -4042,148 +4045,148 @@
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="60" t="s">
+      <c r="E64" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="61"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="63" t="s">
+      <c r="F64" s="67"/>
+      <c r="G64" s="68"/>
+      <c r="H64" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="I64" s="64"/>
-      <c r="J64" s="67"/>
-      <c r="K64" s="68"/>
+      <c r="I64" s="70"/>
+      <c r="J64" s="73"/>
+      <c r="K64" s="74"/>
     </row>
     <row r="65" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="71" t="s">
+      <c r="A65" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="74">
+      <c r="B65" s="78"/>
+      <c r="C65" s="78"/>
+      <c r="D65" s="79"/>
+      <c r="E65" s="80">
         <v>140</v>
       </c>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
-      <c r="H65" s="65"/>
-      <c r="I65" s="66"/>
-      <c r="J65" s="69"/>
-      <c r="K65" s="70"/>
+      <c r="F65" s="81"/>
+      <c r="G65" s="82"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="72"/>
+      <c r="J65" s="75"/>
+      <c r="K65" s="76"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="48"/>
-      <c r="B66" s="48"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="48"/>
-      <c r="K66" s="48"/>
+      <c r="A66" s="51"/>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="51"/>
     </row>
     <row r="67" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="48"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
-      <c r="J67" s="48"/>
-      <c r="K67" s="48"/>
+      <c r="A67" s="51"/>
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="49" t="s">
+      <c r="A68" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="49"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="49"/>
-      <c r="I68" s="49"/>
-      <c r="J68" s="49"/>
-      <c r="K68" s="49"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52"/>
+      <c r="F68" s="52"/>
+      <c r="G68" s="52"/>
+      <c r="H68" s="52"/>
+      <c r="I68" s="52"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="52"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="49"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="49"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="49"/>
-      <c r="I69" s="49"/>
-      <c r="J69" s="49"/>
-      <c r="K69" s="49"/>
+      <c r="A69" s="52"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="52"/>
+      <c r="F69" s="52"/>
+      <c r="G69" s="52"/>
+      <c r="H69" s="52"/>
+      <c r="I69" s="52"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="52"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="49"/>
-      <c r="B70" s="49"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="49"/>
-      <c r="I70" s="49"/>
-      <c r="J70" s="49"/>
-      <c r="K70" s="49"/>
+      <c r="A70" s="52"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="52"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="52"/>
     </row>
     <row r="71" spans="1:11" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="49"/>
-      <c r="B71" s="49"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="49"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="49"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="49"/>
-      <c r="I71" s="49"/>
-      <c r="J71" s="49"/>
-      <c r="K71" s="49"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="52"/>
+      <c r="C71" s="52"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="52"/>
+      <c r="F71" s="52"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="52"/>
     </row>
     <row r="72" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="51"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
-      <c r="I72" s="52"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="55"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
     <row r="73" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="55"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="57"/>
+      <c r="F73" s="57"/>
+      <c r="G73" s="57"/>
+      <c r="H73" s="57"/>
+      <c r="I73" s="58"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
     <row r="74" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
-      <c r="C74" s="77"/>
-      <c r="D74" s="78"/>
-      <c r="E74" s="78"/>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="56"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="60"/>
+      <c r="F74" s="60"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="60"/>
+      <c r="I74" s="61"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
@@ -4231,10 +4234,10 @@
       <c r="E77" s="30">
         <v>4692671.8150000004</v>
       </c>
-      <c r="F77" s="79">
+      <c r="F77" s="48">
         <v>616.38300000000004</v>
       </c>
-      <c r="G77" s="79" t="s">
+      <c r="G77" s="48" t="s">
         <v>21</v>
       </c>
       <c r="H77" s="30" t="s">
@@ -4256,8 +4259,8 @@
       <c r="E78" s="30">
         <v>4692671.3689999999</v>
       </c>
-      <c r="F78" s="80"/>
-      <c r="G78" s="80"/>
+      <c r="F78" s="49"/>
+      <c r="G78" s="49"/>
       <c r="H78" s="30" t="s">
         <v>8</v>
       </c>
@@ -4277,8 +4280,8 @@
       <c r="E79" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F79" s="80"/>
-      <c r="G79" s="80"/>
+      <c r="F79" s="49"/>
+      <c r="G79" s="49"/>
       <c r="H79" s="30" t="s">
         <v>8</v>
       </c>
@@ -4298,8 +4301,8 @@
       <c r="E80" s="30">
         <v>4692673.07</v>
       </c>
-      <c r="F80" s="80"/>
-      <c r="G80" s="80"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="49"/>
       <c r="H80" s="30" t="s">
         <v>8</v>
       </c>
@@ -4319,8 +4322,8 @@
       <c r="E81" s="30">
         <v>4692673.5259999996</v>
       </c>
-      <c r="F81" s="80"/>
-      <c r="G81" s="80"/>
+      <c r="F81" s="49"/>
+      <c r="G81" s="49"/>
       <c r="H81" s="30" t="s">
         <v>8</v>
       </c>
@@ -4340,8 +4343,8 @@
       <c r="E82" s="30">
         <v>4692673.2819999997</v>
       </c>
-      <c r="F82" s="80"/>
-      <c r="G82" s="80"/>
+      <c r="F82" s="49"/>
+      <c r="G82" s="49"/>
       <c r="H82" s="30" t="s">
         <v>8</v>
       </c>
@@ -4361,8 +4364,8 @@
       <c r="E83" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F83" s="80"/>
-      <c r="G83" s="80"/>
+      <c r="F83" s="49"/>
+      <c r="G83" s="49"/>
       <c r="H83" s="30" t="s">
         <v>8</v>
       </c>
@@ -4382,8 +4385,8 @@
       <c r="E84" s="30">
         <v>4692672.7690000003</v>
       </c>
-      <c r="F84" s="80"/>
-      <c r="G84" s="80"/>
+      <c r="F84" s="49"/>
+      <c r="G84" s="49"/>
       <c r="H84" s="30" t="s">
         <v>8</v>
       </c>
@@ -4403,8 +4406,8 @@
       <c r="E85" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F85" s="80"/>
-      <c r="G85" s="80"/>
+      <c r="F85" s="49"/>
+      <c r="G85" s="49"/>
       <c r="H85" s="30" t="s">
         <v>8</v>
       </c>
@@ -4424,8 +4427,8 @@
       <c r="E86" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F86" s="80"/>
-      <c r="G86" s="80"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49"/>
       <c r="H86" s="30" t="s">
         <v>8</v>
       </c>
@@ -4445,8 +4448,8 @@
       <c r="E87" s="30">
         <v>4692687.3470000001</v>
       </c>
-      <c r="F87" s="80"/>
-      <c r="G87" s="80"/>
+      <c r="F87" s="49"/>
+      <c r="G87" s="49"/>
       <c r="H87" s="30" t="s">
         <v>8</v>
       </c>
@@ -4466,8 +4469,8 @@
       <c r="E88" s="30">
         <v>4692681.023</v>
       </c>
-      <c r="F88" s="80"/>
-      <c r="G88" s="80"/>
+      <c r="F88" s="49"/>
+      <c r="G88" s="49"/>
       <c r="H88" s="30" t="s">
         <v>8</v>
       </c>
@@ -4487,8 +4490,8 @@
       <c r="E89" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F89" s="80"/>
-      <c r="G89" s="80"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
       <c r="H89" s="30" t="s">
         <v>8</v>
       </c>
@@ -4508,8 +4511,8 @@
       <c r="E90" s="30">
         <v>4692687.1399999997</v>
       </c>
-      <c r="F90" s="80"/>
-      <c r="G90" s="80"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="49"/>
       <c r="H90" s="30" t="s">
         <v>8</v>
       </c>
@@ -4529,8 +4532,8 @@
       <c r="E91" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F91" s="80"/>
-      <c r="G91" s="80"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="49"/>
       <c r="H91" s="30" t="s">
         <v>8</v>
       </c>
@@ -4550,8 +4553,8 @@
       <c r="E92" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F92" s="80"/>
-      <c r="G92" s="80"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="49"/>
       <c r="H92" s="30" t="s">
         <v>8</v>
       </c>
@@ -4571,8 +4574,8 @@
       <c r="E93" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F93" s="80"/>
-      <c r="G93" s="80"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="49"/>
       <c r="H93" s="30" t="s">
         <v>8</v>
       </c>
@@ -4592,8 +4595,8 @@
       <c r="E94" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F94" s="80"/>
-      <c r="G94" s="80"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="49"/>
       <c r="H94" s="30" t="s">
         <v>8</v>
       </c>
@@ -4613,8 +4616,8 @@
       <c r="E95" s="30">
         <v>4692687.1445000004</v>
       </c>
-      <c r="F95" s="80"/>
-      <c r="G95" s="80"/>
+      <c r="F95" s="49"/>
+      <c r="G95" s="49"/>
       <c r="H95" s="30" t="s">
         <v>8</v>
       </c>
@@ -4634,8 +4637,8 @@
       <c r="E96" s="30">
         <v>4692684.3208999997</v>
       </c>
-      <c r="F96" s="80"/>
-      <c r="G96" s="80"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
       <c r="H96" s="30" t="s">
         <v>8</v>
       </c>
@@ -4655,8 +4658,8 @@
       <c r="E97" s="30">
         <v>4692683.9785000002</v>
       </c>
-      <c r="F97" s="80"/>
-      <c r="G97" s="80"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="49"/>
       <c r="H97" s="30" t="s">
         <v>8</v>
       </c>
@@ -4676,8 +4679,8 @@
       <c r="E98" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F98" s="80"/>
-      <c r="G98" s="80"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="49"/>
       <c r="H98" s="30" t="s">
         <v>8</v>
       </c>
@@ -4697,8 +4700,8 @@
       <c r="E99" s="30">
         <v>4692678.2884999998</v>
       </c>
-      <c r="F99" s="80"/>
-      <c r="G99" s="80"/>
+      <c r="F99" s="49"/>
+      <c r="G99" s="49"/>
       <c r="H99" s="30" t="s">
         <v>8</v>
       </c>
@@ -4718,8 +4721,8 @@
       <c r="E100" s="30">
         <v>4692678.7551999995</v>
       </c>
-      <c r="F100" s="80"/>
-      <c r="G100" s="80"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="49"/>
       <c r="H100" s="30" t="s">
         <v>8</v>
       </c>
@@ -4739,8 +4742,8 @@
       <c r="E101" s="30">
         <v>4692679.1836999999</v>
       </c>
-      <c r="F101" s="80"/>
-      <c r="G101" s="80"/>
+      <c r="F101" s="49"/>
+      <c r="G101" s="49"/>
       <c r="H101" s="30" t="s">
         <v>8</v>
       </c>
@@ -4760,8 +4763,8 @@
       <c r="E102" s="30">
         <v>4692679.26</v>
       </c>
-      <c r="F102" s="80"/>
-      <c r="G102" s="80"/>
+      <c r="F102" s="49"/>
+      <c r="G102" s="49"/>
       <c r="H102" s="30" t="s">
         <v>8</v>
       </c>
@@ -4781,8 +4784,8 @@
       <c r="E103" s="30">
         <v>4692680.1398</v>
       </c>
-      <c r="F103" s="80"/>
-      <c r="G103" s="80"/>
+      <c r="F103" s="49"/>
+      <c r="G103" s="49"/>
       <c r="H103" s="30" t="s">
         <v>8</v>
       </c>
@@ -4802,8 +4805,8 @@
       <c r="E104" s="30">
         <v>4692685.5575999999</v>
       </c>
-      <c r="F104" s="80"/>
-      <c r="G104" s="80"/>
+      <c r="F104" s="49"/>
+      <c r="G104" s="49"/>
       <c r="H104" s="30" t="s">
         <v>8</v>
       </c>
@@ -4823,8 +4826,8 @@
       <c r="E105" s="30">
         <v>4692686.4374000002</v>
       </c>
-      <c r="F105" s="80"/>
-      <c r="G105" s="80"/>
+      <c r="F105" s="49"/>
+      <c r="G105" s="49"/>
       <c r="H105" s="30" t="s">
         <v>8</v>
       </c>
@@ -4844,8 +4847,8 @@
       <c r="E106" s="30">
         <v>4692690.9013999999</v>
       </c>
-      <c r="F106" s="80"/>
-      <c r="G106" s="80"/>
+      <c r="F106" s="49"/>
+      <c r="G106" s="49"/>
       <c r="H106" s="30" t="s">
         <v>8</v>
       </c>
@@ -4865,8 +4868,8 @@
       <c r="E107" s="30">
         <v>4692693.1089000003</v>
       </c>
-      <c r="F107" s="80"/>
-      <c r="G107" s="80"/>
+      <c r="F107" s="49"/>
+      <c r="G107" s="49"/>
       <c r="H107" s="30" t="s">
         <v>8</v>
       </c>
@@ -4886,8 +4889,8 @@
       <c r="E108" s="30">
         <v>4692689.4265999999</v>
       </c>
-      <c r="F108" s="80"/>
-      <c r="G108" s="80"/>
+      <c r="F108" s="49"/>
+      <c r="G108" s="49"/>
       <c r="H108" s="30" t="s">
         <v>8</v>
       </c>
@@ -4907,8 +4910,8 @@
       <c r="E109" s="30">
         <v>4692687.6520999996</v>
       </c>
-      <c r="F109" s="80"/>
-      <c r="G109" s="80"/>
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
       <c r="H109" s="30" t="s">
         <v>8</v>
       </c>
@@ -4928,8 +4931,8 @@
       <c r="E110" s="30">
         <v>4692689.9780000001</v>
       </c>
-      <c r="F110" s="80"/>
-      <c r="G110" s="80"/>
+      <c r="F110" s="49"/>
+      <c r="G110" s="49"/>
       <c r="H110" s="30" t="s">
         <v>8</v>
       </c>
@@ -4949,8 +4952,8 @@
       <c r="E111" s="30">
         <v>4692689.3081999999</v>
       </c>
-      <c r="F111" s="80"/>
-      <c r="G111" s="80"/>
+      <c r="F111" s="49"/>
+      <c r="G111" s="49"/>
       <c r="H111" s="30" t="s">
         <v>8</v>
       </c>
@@ -4970,8 +4973,8 @@
       <c r="E112" s="30">
         <v>4692679.7653000001</v>
       </c>
-      <c r="F112" s="81"/>
-      <c r="G112" s="81"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="50"/>
       <c r="H112" s="30" t="s">
         <v>20</v>
       </c>
@@ -5073,28 +5076,28 @@
     <row r="120" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
-      <c r="C120" s="59" t="s">
+      <c r="C120" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D120" s="59"/>
-      <c r="E120" s="59"/>
-      <c r="F120" s="59"/>
-      <c r="G120" s="59"/>
-      <c r="H120" s="59"/>
-      <c r="I120" s="59"/>
+      <c r="D120" s="62"/>
+      <c r="E120" s="62"/>
+      <c r="F120" s="62"/>
+      <c r="G120" s="62"/>
+      <c r="H120" s="62"/>
+      <c r="I120" s="62"/>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
     <row r="121" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
-      <c r="C121" s="59"/>
-      <c r="D121" s="59"/>
-      <c r="E121" s="59"/>
-      <c r="F121" s="59"/>
-      <c r="G121" s="59"/>
-      <c r="H121" s="59"/>
-      <c r="I121" s="59"/>
+      <c r="C121" s="62"/>
+      <c r="D121" s="62"/>
+      <c r="E121" s="62"/>
+      <c r="F121" s="62"/>
+      <c r="G121" s="62"/>
+      <c r="H121" s="62"/>
+      <c r="I121" s="62"/>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
@@ -5183,114 +5186,114 @@
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
-      <c r="E128" s="60" t="s">
+      <c r="E128" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="F128" s="61"/>
-      <c r="G128" s="62"/>
-      <c r="H128" s="63" t="s">
+      <c r="F128" s="67"/>
+      <c r="G128" s="68"/>
+      <c r="H128" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="I128" s="64"/>
-      <c r="J128" s="67"/>
-      <c r="K128" s="68"/>
+      <c r="I128" s="70"/>
+      <c r="J128" s="73"/>
+      <c r="K128" s="74"/>
     </row>
     <row r="129" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="71" t="s">
+      <c r="A129" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B129" s="72"/>
-      <c r="C129" s="72"/>
-      <c r="D129" s="73"/>
-      <c r="E129" s="74">
+      <c r="B129" s="78"/>
+      <c r="C129" s="78"/>
+      <c r="D129" s="79"/>
+      <c r="E129" s="80">
         <v>140</v>
       </c>
-      <c r="F129" s="75"/>
-      <c r="G129" s="76"/>
-      <c r="H129" s="65"/>
-      <c r="I129" s="66"/>
-      <c r="J129" s="69"/>
-      <c r="K129" s="70"/>
+      <c r="F129" s="81"/>
+      <c r="G129" s="82"/>
+      <c r="H129" s="71"/>
+      <c r="I129" s="72"/>
+      <c r="J129" s="75"/>
+      <c r="K129" s="76"/>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A132" s="48"/>
-      <c r="B132" s="48"/>
-      <c r="C132" s="48"/>
-      <c r="D132" s="48"/>
-      <c r="E132" s="48"/>
-      <c r="F132" s="48"/>
-      <c r="G132" s="48"/>
-      <c r="H132" s="48"/>
-      <c r="I132" s="48"/>
-      <c r="J132" s="48"/>
-      <c r="K132" s="48"/>
+      <c r="A132" s="51"/>
+      <c r="B132" s="51"/>
+      <c r="C132" s="51"/>
+      <c r="D132" s="51"/>
+      <c r="E132" s="51"/>
+      <c r="F132" s="51"/>
+      <c r="G132" s="51"/>
+      <c r="H132" s="51"/>
+      <c r="I132" s="51"/>
+      <c r="J132" s="51"/>
+      <c r="K132" s="51"/>
     </row>
     <row r="133" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="48"/>
-      <c r="B133" s="48"/>
-      <c r="C133" s="48"/>
-      <c r="D133" s="48"/>
-      <c r="E133" s="48"/>
-      <c r="F133" s="48"/>
-      <c r="G133" s="48"/>
-      <c r="H133" s="48"/>
-      <c r="I133" s="48"/>
-      <c r="J133" s="48"/>
-      <c r="K133" s="48"/>
+      <c r="A133" s="51"/>
+      <c r="B133" s="51"/>
+      <c r="C133" s="51"/>
+      <c r="D133" s="51"/>
+      <c r="E133" s="51"/>
+      <c r="F133" s="51"/>
+      <c r="G133" s="51"/>
+      <c r="H133" s="51"/>
+      <c r="I133" s="51"/>
+      <c r="J133" s="51"/>
+      <c r="K133" s="51"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="49" t="s">
+      <c r="A134" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B134" s="49"/>
-      <c r="C134" s="49"/>
-      <c r="D134" s="49"/>
-      <c r="E134" s="49"/>
-      <c r="F134" s="49"/>
-      <c r="G134" s="49"/>
-      <c r="H134" s="49"/>
-      <c r="I134" s="49"/>
-      <c r="J134" s="49"/>
-      <c r="K134" s="49"/>
+      <c r="B134" s="52"/>
+      <c r="C134" s="52"/>
+      <c r="D134" s="52"/>
+      <c r="E134" s="52"/>
+      <c r="F134" s="52"/>
+      <c r="G134" s="52"/>
+      <c r="H134" s="52"/>
+      <c r="I134" s="52"/>
+      <c r="J134" s="52"/>
+      <c r="K134" s="52"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="49"/>
-      <c r="B135" s="49"/>
-      <c r="C135" s="49"/>
-      <c r="D135" s="49"/>
-      <c r="E135" s="49"/>
-      <c r="F135" s="49"/>
-      <c r="G135" s="49"/>
-      <c r="H135" s="49"/>
-      <c r="I135" s="49"/>
-      <c r="J135" s="49"/>
-      <c r="K135" s="49"/>
+      <c r="A135" s="52"/>
+      <c r="B135" s="52"/>
+      <c r="C135" s="52"/>
+      <c r="D135" s="52"/>
+      <c r="E135" s="52"/>
+      <c r="F135" s="52"/>
+      <c r="G135" s="52"/>
+      <c r="H135" s="52"/>
+      <c r="I135" s="52"/>
+      <c r="J135" s="52"/>
+      <c r="K135" s="52"/>
     </row>
     <row r="136" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="49"/>
-      <c r="B136" s="49"/>
-      <c r="C136" s="49"/>
-      <c r="D136" s="49"/>
-      <c r="E136" s="49"/>
-      <c r="F136" s="49"/>
-      <c r="G136" s="49"/>
-      <c r="H136" s="49"/>
-      <c r="I136" s="49"/>
-      <c r="J136" s="49"/>
-      <c r="K136" s="49"/>
+      <c r="A136" s="52"/>
+      <c r="B136" s="52"/>
+      <c r="C136" s="52"/>
+      <c r="D136" s="52"/>
+      <c r="E136" s="52"/>
+      <c r="F136" s="52"/>
+      <c r="G136" s="52"/>
+      <c r="H136" s="52"/>
+      <c r="I136" s="52"/>
+      <c r="J136" s="52"/>
+      <c r="K136" s="52"/>
     </row>
     <row r="137" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="49"/>
-      <c r="B137" s="49"/>
-      <c r="C137" s="49"/>
-      <c r="D137" s="49"/>
-      <c r="E137" s="49"/>
-      <c r="F137" s="49"/>
-      <c r="G137" s="49"/>
-      <c r="H137" s="49"/>
-      <c r="I137" s="49"/>
-      <c r="J137" s="49"/>
-      <c r="K137" s="49"/>
+      <c r="A137" s="52"/>
+      <c r="B137" s="52"/>
+      <c r="C137" s="52"/>
+      <c r="D137" s="52"/>
+      <c r="E137" s="52"/>
+      <c r="F137" s="52"/>
+      <c r="G137" s="52"/>
+      <c r="H137" s="52"/>
+      <c r="I137" s="52"/>
+      <c r="J137" s="52"/>
+      <c r="K137" s="52"/>
     </row>
     <row r="138" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="1"/>
@@ -5307,37 +5310,37 @@
     </row>
     <row r="139" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A139" s="1"/>
-      <c r="C139" s="50"/>
-      <c r="D139" s="51"/>
-      <c r="E139" s="51"/>
-      <c r="F139" s="51"/>
-      <c r="G139" s="51"/>
-      <c r="H139" s="51"/>
-      <c r="I139" s="52"/>
+      <c r="C139" s="53"/>
+      <c r="D139" s="54"/>
+      <c r="E139" s="54"/>
+      <c r="F139" s="54"/>
+      <c r="G139" s="54"/>
+      <c r="H139" s="54"/>
+      <c r="I139" s="55"/>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
     </row>
     <row r="140" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
-      <c r="C140" s="53"/>
-      <c r="D140" s="54"/>
-      <c r="E140" s="54"/>
-      <c r="F140" s="54"/>
-      <c r="G140" s="54"/>
-      <c r="H140" s="54"/>
-      <c r="I140" s="55"/>
+      <c r="C140" s="56"/>
+      <c r="D140" s="57"/>
+      <c r="E140" s="57"/>
+      <c r="F140" s="57"/>
+      <c r="G140" s="57"/>
+      <c r="H140" s="57"/>
+      <c r="I140" s="58"/>
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
     </row>
     <row r="141" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1"/>
-      <c r="C141" s="77"/>
-      <c r="D141" s="78"/>
-      <c r="E141" s="78"/>
-      <c r="F141" s="78"/>
-      <c r="G141" s="78"/>
-      <c r="H141" s="78"/>
-      <c r="I141" s="56"/>
+      <c r="C141" s="59"/>
+      <c r="D141" s="60"/>
+      <c r="E141" s="60"/>
+      <c r="F141" s="60"/>
+      <c r="G141" s="60"/>
+      <c r="H141" s="60"/>
+      <c r="I141" s="61"/>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
     </row>
@@ -5388,7 +5391,7 @@
       <c r="F144" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G144" s="79" t="s">
+      <c r="G144" s="88" t="s">
         <v>23</v>
       </c>
       <c r="H144" s="30" t="s">
@@ -5413,7 +5416,7 @@
       <c r="F145" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G145" s="80"/>
+      <c r="G145" s="88"/>
       <c r="H145" s="30" t="s">
         <v>8</v>
       </c>
@@ -5436,7 +5439,7 @@
       <c r="F146" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G146" s="80"/>
+      <c r="G146" s="88"/>
       <c r="H146" s="30" t="s">
         <v>8</v>
       </c>
@@ -5459,7 +5462,7 @@
       <c r="F147" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G147" s="80"/>
+      <c r="G147" s="88"/>
       <c r="H147" s="30" t="s">
         <v>8</v>
       </c>
@@ -5482,7 +5485,7 @@
       <c r="F148" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G148" s="80"/>
+      <c r="G148" s="88"/>
       <c r="H148" s="30" t="s">
         <v>8</v>
       </c>
@@ -5505,7 +5508,7 @@
       <c r="F149" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G149" s="80"/>
+      <c r="G149" s="88"/>
       <c r="H149" s="30" t="s">
         <v>8</v>
       </c>
@@ -5528,7 +5531,7 @@
       <c r="F150" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G150" s="80"/>
+      <c r="G150" s="88"/>
       <c r="H150" s="30" t="s">
         <v>8</v>
       </c>
@@ -5551,7 +5554,7 @@
       <c r="F151" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G151" s="80"/>
+      <c r="G151" s="88"/>
       <c r="H151" s="30" t="s">
         <v>8</v>
       </c>
@@ -5574,7 +5577,7 @@
       <c r="F152" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G152" s="80"/>
+      <c r="G152" s="88"/>
       <c r="H152" s="30" t="s">
         <v>8</v>
       </c>
@@ -5597,7 +5600,7 @@
       <c r="F153" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G153" s="80"/>
+      <c r="G153" s="88"/>
       <c r="H153" s="30" t="s">
         <v>8</v>
       </c>
@@ -5620,7 +5623,7 @@
       <c r="F154" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G154" s="80"/>
+      <c r="G154" s="88"/>
       <c r="H154" s="30" t="s">
         <v>8</v>
       </c>
@@ -5643,7 +5646,7 @@
       <c r="F155" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G155" s="80"/>
+      <c r="G155" s="88"/>
       <c r="H155" s="30" t="s">
         <v>8</v>
       </c>
@@ -5666,7 +5669,7 @@
       <c r="F156" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G156" s="80"/>
+      <c r="G156" s="88"/>
       <c r="H156" s="30" t="s">
         <v>8</v>
       </c>
@@ -5689,7 +5692,7 @@
       <c r="F157" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G157" s="80"/>
+      <c r="G157" s="88"/>
       <c r="H157" s="30" t="s">
         <v>8</v>
       </c>
@@ -5712,7 +5715,7 @@
       <c r="F158" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G158" s="80"/>
+      <c r="G158" s="88"/>
       <c r="H158" s="30" t="s">
         <v>8</v>
       </c>
@@ -5735,7 +5738,7 @@
       <c r="F159" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G159" s="80"/>
+      <c r="G159" s="88"/>
       <c r="H159" s="30" t="s">
         <v>8</v>
       </c>
@@ -5758,7 +5761,7 @@
       <c r="F160" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G160" s="80"/>
+      <c r="G160" s="88"/>
       <c r="H160" s="30" t="s">
         <v>8</v>
       </c>
@@ -5781,7 +5784,7 @@
       <c r="F161" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G161" s="80"/>
+      <c r="G161" s="88"/>
       <c r="H161" s="30" t="s">
         <v>8</v>
       </c>
@@ -5804,7 +5807,7 @@
       <c r="F162" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G162" s="80"/>
+      <c r="G162" s="88"/>
       <c r="H162" s="30" t="s">
         <v>8</v>
       </c>
@@ -5827,7 +5830,7 @@
       <c r="F163" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G163" s="80"/>
+      <c r="G163" s="88"/>
       <c r="H163" s="30" t="s">
         <v>8</v>
       </c>
@@ -5850,7 +5853,7 @@
       <c r="F164" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G164" s="80"/>
+      <c r="G164" s="88"/>
       <c r="H164" s="30" t="s">
         <v>8</v>
       </c>
@@ -5873,7 +5876,7 @@
       <c r="F165" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G165" s="80"/>
+      <c r="G165" s="88"/>
       <c r="H165" s="30" t="s">
         <v>8</v>
       </c>
@@ -5888,15 +5891,15 @@
         <v>135</v>
       </c>
       <c r="D166" s="30">
-        <v>7517926.9230000004</v>
+        <v>7517926.9447999997</v>
       </c>
       <c r="E166" s="30">
-        <v>4692677.5713999998</v>
+        <v>4692677.4724000003</v>
       </c>
       <c r="F166" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G166" s="80"/>
+      <c r="G166" s="88"/>
       <c r="H166" s="30" t="s">
         <v>8</v>
       </c>
@@ -5911,15 +5914,15 @@
         <v>136</v>
       </c>
       <c r="D167" s="30">
-        <v>7517929.3389999997</v>
+        <v>7517929.5975000001</v>
       </c>
       <c r="E167" s="30">
-        <v>4692678.3875000002</v>
+        <v>4692678.3684</v>
       </c>
       <c r="F167" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G167" s="80"/>
+      <c r="G167" s="88"/>
       <c r="H167" s="30" t="s">
         <v>8</v>
       </c>
@@ -5934,15 +5937,15 @@
         <v>137</v>
       </c>
       <c r="D168" s="30">
-        <v>7517927.5005999999</v>
+        <v>7517927.6245999997</v>
       </c>
       <c r="E168" s="30">
-        <v>4692683.8356999997</v>
+        <v>4692684.2153000003</v>
       </c>
       <c r="F168" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G168" s="80"/>
+      <c r="G168" s="88"/>
       <c r="H168" s="30" t="s">
         <v>8</v>
       </c>
@@ -5957,15 +5960,15 @@
         <v>138</v>
       </c>
       <c r="D169" s="30">
-        <v>7517928.7559000002</v>
+        <v>7517928.6431</v>
       </c>
       <c r="E169" s="30">
-        <v>4692684.2597000003</v>
+        <v>4692684.5592999998</v>
       </c>
       <c r="F169" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G169" s="80"/>
+      <c r="G169" s="88"/>
       <c r="H169" s="30" t="s">
         <v>8</v>
       </c>
@@ -5988,7 +5991,7 @@
       <c r="F170" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G170" s="80"/>
+      <c r="G170" s="88"/>
       <c r="H170" s="30" t="s">
         <v>8</v>
       </c>
@@ -6003,15 +6006,15 @@
         <v>140</v>
       </c>
       <c r="D171" s="30">
-        <v>7517941.0358999996</v>
+        <v>7517940.9913999997</v>
       </c>
       <c r="E171" s="30">
-        <v>4692691.6266999999</v>
+        <v>4692691.6117000002</v>
       </c>
       <c r="F171" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G171" s="80"/>
+      <c r="G171" s="88"/>
       <c r="H171" s="30" t="s">
         <v>8</v>
       </c>
@@ -6025,15 +6028,15 @@
         <v>141</v>
       </c>
       <c r="D172" s="30">
-        <v>7517941.8782000002</v>
+        <v>7517941.8485000003</v>
       </c>
       <c r="E172" s="30">
-        <v>4692689.2351000002</v>
+        <v>4692689.1782</v>
       </c>
       <c r="F172" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G172" s="80"/>
+      <c r="G172" s="88"/>
       <c r="H172" s="30" t="s">
         <v>8</v>
       </c>
@@ -6047,15 +6050,15 @@
         <v>142</v>
       </c>
       <c r="D173" s="30">
-        <v>7517946.1831</v>
+        <v>7517946.4798999997</v>
       </c>
       <c r="E173" s="30">
-        <v>4692690.6902999999</v>
+        <v>4692690.7472000001</v>
       </c>
       <c r="F173" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G173" s="80"/>
+      <c r="G173" s="88"/>
       <c r="H173" s="30" t="s">
         <v>8</v>
       </c>
@@ -6070,15 +6073,15 @@
         <v>143</v>
       </c>
       <c r="D174" s="30">
-        <v>7517945.3410999998</v>
+        <v>7517945.6243000003</v>
       </c>
       <c r="E174" s="30">
-        <v>4692693.0809000004</v>
+        <v>4692693.1765999999</v>
       </c>
       <c r="F174" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G174" s="80"/>
+      <c r="G174" s="88"/>
       <c r="H174" s="30" t="s">
         <v>8</v>
       </c>
@@ -6093,15 +6096,15 @@
         <v>144</v>
       </c>
       <c r="D175" s="30">
-        <v>7517947.9436999997</v>
+        <v>7517948.4293</v>
       </c>
       <c r="E175" s="30">
-        <v>4692685.3624999998</v>
+        <v>4692685.7846999997</v>
       </c>
       <c r="F175" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G175" s="80"/>
+      <c r="G175" s="88"/>
       <c r="H175" s="30" t="s">
         <v>8</v>
       </c>
@@ -6116,15 +6119,15 @@
         <v>145</v>
       </c>
       <c r="D176" s="30">
-        <v>7517949.3491000002</v>
+        <v>7517949.9928000001</v>
       </c>
       <c r="E176" s="30">
-        <v>4692681.1283999998</v>
+        <v>4692681.0932</v>
       </c>
       <c r="F176" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G176" s="80"/>
+      <c r="G176" s="88"/>
       <c r="H176" s="30" t="s">
         <v>8</v>
       </c>
@@ -6139,15 +6142,15 @@
         <v>146</v>
       </c>
       <c r="D177" s="30">
-        <v>7517952.7259999998</v>
+        <v>7517952.7995999996</v>
       </c>
       <c r="E177" s="30">
-        <v>4692682.3354000002</v>
+        <v>4692682.0964000002</v>
       </c>
       <c r="F177" s="19">
         <v>618.84299999999996</v>
       </c>
-      <c r="G177" s="80"/>
+      <c r="G177" s="88"/>
       <c r="H177" s="30" t="s">
         <v>8</v>
       </c>
@@ -6159,20 +6162,20 @@
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="19">
-        <v>101</v>
+        <v>147</v>
       </c>
       <c r="D178" s="30">
-        <v>7517952.4309</v>
+        <v>7517949.4227</v>
       </c>
       <c r="E178" s="30">
-        <v>4692678.5990000004</v>
+        <v>4692680.8893999998</v>
       </c>
       <c r="F178" s="19">
-        <v>616.38300000000004</v>
-      </c>
-      <c r="G178" s="81"/>
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G178" s="88"/>
       <c r="H178" s="30" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I178" s="25"/>
       <c r="J178" s="1"/>
@@ -6181,12 +6184,22 @@
     <row r="179" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-      <c r="C179" s="14"/>
-      <c r="D179" s="17"/>
-      <c r="E179" s="17"/>
-      <c r="F179" s="27"/>
-      <c r="G179" s="27"/>
-      <c r="H179" s="13"/>
+      <c r="C179" s="47">
+        <v>148</v>
+      </c>
+      <c r="D179" s="30">
+        <v>7517951.2527000001</v>
+      </c>
+      <c r="E179" s="30">
+        <v>4692686.7380999997</v>
+      </c>
+      <c r="F179" s="47">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G179" s="88"/>
+      <c r="H179" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I179" s="25"/>
       <c r="J179" s="1"/>
       <c r="K179" s="1"/>
@@ -6194,12 +6207,22 @@
     <row r="180" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
-      <c r="C180" s="14"/>
-      <c r="D180" s="17"/>
-      <c r="E180" s="17"/>
-      <c r="F180" s="27"/>
-      <c r="G180" s="27"/>
-      <c r="H180" s="13"/>
+      <c r="C180" s="47">
+        <v>149</v>
+      </c>
+      <c r="D180" s="30">
+        <v>7517924.9718000004</v>
+      </c>
+      <c r="E180" s="30">
+        <v>4692683.3192999996</v>
+      </c>
+      <c r="F180" s="47">
+        <v>618.84299999999996</v>
+      </c>
+      <c r="G180" s="88"/>
+      <c r="H180" s="30" t="s">
+        <v>8</v>
+      </c>
       <c r="I180" s="25"/>
       <c r="J180" s="1"/>
       <c r="K180" s="1"/>
@@ -6207,12 +6230,22 @@
     <row r="181" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
-      <c r="C181" s="14"/>
-      <c r="D181" s="17"/>
-      <c r="E181" s="17"/>
-      <c r="F181" s="27"/>
-      <c r="G181" s="27"/>
-      <c r="H181" s="13"/>
+      <c r="C181" s="47">
+        <v>101</v>
+      </c>
+      <c r="D181" s="30">
+        <v>7517952.4309</v>
+      </c>
+      <c r="E181" s="30">
+        <v>4692678.5990000004</v>
+      </c>
+      <c r="F181" s="47">
+        <v>616.38300000000004</v>
+      </c>
+      <c r="G181" s="88"/>
+      <c r="H181" s="30" t="s">
+        <v>20</v>
+      </c>
       <c r="I181" s="25"/>
       <c r="J181" s="1"/>
       <c r="K181" s="1"/>
@@ -6220,28 +6253,12 @@
     <row r="182" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
-      <c r="C182" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="D182" s="59"/>
-      <c r="E182" s="59"/>
-      <c r="F182" s="59"/>
-      <c r="G182" s="59"/>
-      <c r="H182" s="59"/>
-      <c r="I182" s="59"/>
       <c r="J182" s="1"/>
       <c r="K182" s="1"/>
     </row>
     <row r="183" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
-      <c r="C183" s="59"/>
-      <c r="D183" s="59"/>
-      <c r="E183" s="59"/>
-      <c r="F183" s="59"/>
-      <c r="G183" s="59"/>
-      <c r="H183" s="59"/>
-      <c r="I183" s="59"/>
       <c r="J183" s="1"/>
       <c r="K183" s="1"/>
     </row>
@@ -6287,26 +6304,28 @@
     <row r="187" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
-      <c r="C187" s="14"/>
-      <c r="D187" s="17"/>
-      <c r="E187" s="17"/>
-      <c r="F187" s="27"/>
-      <c r="G187" s="27"/>
-      <c r="H187" s="13"/>
-      <c r="I187" s="31"/>
+      <c r="C187" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D187" s="62"/>
+      <c r="E187" s="62"/>
+      <c r="F187" s="62"/>
+      <c r="G187" s="62"/>
+      <c r="H187" s="62"/>
+      <c r="I187" s="62"/>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
     </row>
     <row r="188" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
-      <c r="C188" s="14"/>
-      <c r="D188" s="17"/>
-      <c r="E188" s="17"/>
-      <c r="F188" s="27"/>
-      <c r="G188" s="27"/>
-      <c r="H188" s="13"/>
-      <c r="I188" s="31"/>
+      <c r="C188" s="62"/>
+      <c r="D188" s="62"/>
+      <c r="E188" s="62"/>
+      <c r="F188" s="62"/>
+      <c r="G188" s="62"/>
+      <c r="H188" s="62"/>
+      <c r="I188" s="62"/>
       <c r="J188" s="1"/>
       <c r="K188" s="1"/>
     </row>
@@ -6356,148 +6375,148 @@
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
       <c r="D192" s="3"/>
-      <c r="E192" s="60" t="s">
+      <c r="E192" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="F192" s="61"/>
-      <c r="G192" s="62"/>
-      <c r="H192" s="63" t="s">
+      <c r="F192" s="67"/>
+      <c r="G192" s="68"/>
+      <c r="H192" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="I192" s="64"/>
-      <c r="J192" s="67"/>
-      <c r="K192" s="68"/>
+      <c r="I192" s="70"/>
+      <c r="J192" s="73"/>
+      <c r="K192" s="74"/>
     </row>
     <row r="193" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="71" t="s">
+      <c r="A193" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B193" s="72"/>
-      <c r="C193" s="72"/>
-      <c r="D193" s="73"/>
-      <c r="E193" s="74">
+      <c r="B193" s="78"/>
+      <c r="C193" s="78"/>
+      <c r="D193" s="79"/>
+      <c r="E193" s="80">
         <v>140</v>
       </c>
-      <c r="F193" s="75"/>
-      <c r="G193" s="76"/>
-      <c r="H193" s="65"/>
-      <c r="I193" s="66"/>
-      <c r="J193" s="69"/>
-      <c r="K193" s="70"/>
+      <c r="F193" s="81"/>
+      <c r="G193" s="82"/>
+      <c r="H193" s="71"/>
+      <c r="I193" s="72"/>
+      <c r="J193" s="75"/>
+      <c r="K193" s="76"/>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A194" s="48"/>
-      <c r="B194" s="48"/>
-      <c r="C194" s="48"/>
-      <c r="D194" s="48"/>
-      <c r="E194" s="48"/>
-      <c r="F194" s="48"/>
-      <c r="G194" s="48"/>
-      <c r="H194" s="48"/>
-      <c r="I194" s="48"/>
-      <c r="J194" s="48"/>
-      <c r="K194" s="48"/>
+      <c r="A194" s="51"/>
+      <c r="B194" s="51"/>
+      <c r="C194" s="51"/>
+      <c r="D194" s="51"/>
+      <c r="E194" s="51"/>
+      <c r="F194" s="51"/>
+      <c r="G194" s="51"/>
+      <c r="H194" s="51"/>
+      <c r="I194" s="51"/>
+      <c r="J194" s="51"/>
+      <c r="K194" s="51"/>
     </row>
     <row r="195" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="48"/>
-      <c r="B195" s="48"/>
-      <c r="C195" s="48"/>
-      <c r="D195" s="48"/>
-      <c r="E195" s="48"/>
-      <c r="F195" s="48"/>
-      <c r="G195" s="48"/>
-      <c r="H195" s="48"/>
-      <c r="I195" s="48"/>
-      <c r="J195" s="48"/>
-      <c r="K195" s="48"/>
+      <c r="A195" s="51"/>
+      <c r="B195" s="51"/>
+      <c r="C195" s="51"/>
+      <c r="D195" s="51"/>
+      <c r="E195" s="51"/>
+      <c r="F195" s="51"/>
+      <c r="G195" s="51"/>
+      <c r="H195" s="51"/>
+      <c r="I195" s="51"/>
+      <c r="J195" s="51"/>
+      <c r="K195" s="51"/>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A196" s="49" t="s">
+      <c r="A196" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B196" s="49"/>
-      <c r="C196" s="49"/>
-      <c r="D196" s="49"/>
-      <c r="E196" s="49"/>
-      <c r="F196" s="49"/>
-      <c r="G196" s="49"/>
-      <c r="H196" s="49"/>
-      <c r="I196" s="49"/>
-      <c r="J196" s="49"/>
-      <c r="K196" s="49"/>
+      <c r="B196" s="52"/>
+      <c r="C196" s="52"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="52"/>
+      <c r="F196" s="52"/>
+      <c r="G196" s="52"/>
+      <c r="H196" s="52"/>
+      <c r="I196" s="52"/>
+      <c r="J196" s="52"/>
+      <c r="K196" s="52"/>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A197" s="49"/>
-      <c r="B197" s="49"/>
-      <c r="C197" s="49"/>
-      <c r="D197" s="49"/>
-      <c r="E197" s="49"/>
-      <c r="F197" s="49"/>
-      <c r="G197" s="49"/>
-      <c r="H197" s="49"/>
-      <c r="I197" s="49"/>
-      <c r="J197" s="49"/>
-      <c r="K197" s="49"/>
+      <c r="A197" s="52"/>
+      <c r="B197" s="52"/>
+      <c r="C197" s="52"/>
+      <c r="D197" s="52"/>
+      <c r="E197" s="52"/>
+      <c r="F197" s="52"/>
+      <c r="G197" s="52"/>
+      <c r="H197" s="52"/>
+      <c r="I197" s="52"/>
+      <c r="J197" s="52"/>
+      <c r="K197" s="52"/>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A198" s="49"/>
-      <c r="B198" s="49"/>
-      <c r="C198" s="49"/>
-      <c r="D198" s="49"/>
-      <c r="E198" s="49"/>
-      <c r="F198" s="49"/>
-      <c r="G198" s="49"/>
-      <c r="H198" s="49"/>
-      <c r="I198" s="49"/>
-      <c r="J198" s="49"/>
-      <c r="K198" s="49"/>
+      <c r="A198" s="52"/>
+      <c r="B198" s="52"/>
+      <c r="C198" s="52"/>
+      <c r="D198" s="52"/>
+      <c r="E198" s="52"/>
+      <c r="F198" s="52"/>
+      <c r="G198" s="52"/>
+      <c r="H198" s="52"/>
+      <c r="I198" s="52"/>
+      <c r="J198" s="52"/>
+      <c r="K198" s="52"/>
     </row>
     <row r="199" spans="1:11" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="49"/>
-      <c r="B199" s="49"/>
-      <c r="C199" s="49"/>
-      <c r="D199" s="49"/>
-      <c r="E199" s="49"/>
-      <c r="F199" s="49"/>
-      <c r="G199" s="49"/>
-      <c r="H199" s="49"/>
-      <c r="I199" s="49"/>
-      <c r="J199" s="49"/>
-      <c r="K199" s="49"/>
+      <c r="A199" s="52"/>
+      <c r="B199" s="52"/>
+      <c r="C199" s="52"/>
+      <c r="D199" s="52"/>
+      <c r="E199" s="52"/>
+      <c r="F199" s="52"/>
+      <c r="G199" s="52"/>
+      <c r="H199" s="52"/>
+      <c r="I199" s="52"/>
+      <c r="J199" s="52"/>
+      <c r="K199" s="52"/>
     </row>
     <row r="200" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A200" s="1"/>
-      <c r="C200" s="50"/>
-      <c r="D200" s="51"/>
-      <c r="E200" s="51"/>
-      <c r="F200" s="51"/>
-      <c r="G200" s="51"/>
-      <c r="H200" s="51"/>
-      <c r="I200" s="52"/>
+      <c r="C200" s="53"/>
+      <c r="D200" s="54"/>
+      <c r="E200" s="54"/>
+      <c r="F200" s="54"/>
+      <c r="G200" s="54"/>
+      <c r="H200" s="54"/>
+      <c r="I200" s="55"/>
       <c r="J200" s="1"/>
       <c r="K200" s="1"/>
     </row>
     <row r="201" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="1"/>
-      <c r="C201" s="53"/>
-      <c r="D201" s="54"/>
-      <c r="E201" s="54"/>
-      <c r="F201" s="54"/>
-      <c r="G201" s="54"/>
-      <c r="H201" s="54"/>
-      <c r="I201" s="55"/>
+      <c r="C201" s="56"/>
+      <c r="D201" s="57"/>
+      <c r="E201" s="57"/>
+      <c r="F201" s="57"/>
+      <c r="G201" s="57"/>
+      <c r="H201" s="57"/>
+      <c r="I201" s="58"/>
       <c r="J201" s="1"/>
       <c r="K201" s="1"/>
     </row>
     <row r="202" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A202" s="1"/>
-      <c r="C202" s="53"/>
-      <c r="D202" s="54"/>
-      <c r="E202" s="54"/>
-      <c r="F202" s="54"/>
-      <c r="G202" s="54"/>
-      <c r="H202" s="54"/>
-      <c r="I202" s="56"/>
+      <c r="C202" s="56"/>
+      <c r="D202" s="57"/>
+      <c r="E202" s="57"/>
+      <c r="F202" s="57"/>
+      <c r="G202" s="57"/>
+      <c r="H202" s="57"/>
+      <c r="I202" s="61"/>
       <c r="J202" s="1"/>
       <c r="K202" s="1"/>
     </row>
@@ -6538,10 +6557,10 @@
       <c r="E204" s="30">
         <v>4692673.5029999996</v>
       </c>
-      <c r="F204" s="57">
+      <c r="F204" s="88">
         <v>622.86300000000006</v>
       </c>
-      <c r="G204" s="57" t="s">
+      <c r="G204" s="88" t="s">
         <v>24</v>
       </c>
       <c r="H204" s="40" t="s">
@@ -6563,8 +6582,8 @@
       <c r="E205" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F205" s="57"/>
-      <c r="G205" s="57"/>
+      <c r="F205" s="88"/>
+      <c r="G205" s="88"/>
       <c r="H205" s="40" t="s">
         <v>8</v>
       </c>
@@ -6584,8 +6603,8 @@
       <c r="E206" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F206" s="57"/>
-      <c r="G206" s="57"/>
+      <c r="F206" s="88"/>
+      <c r="G206" s="88"/>
       <c r="H206" s="40" t="s">
         <v>8</v>
       </c>
@@ -6605,8 +6624,8 @@
       <c r="E207" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F207" s="57"/>
-      <c r="G207" s="57"/>
+      <c r="F207" s="88"/>
+      <c r="G207" s="88"/>
       <c r="H207" s="40" t="s">
         <v>8</v>
       </c>
@@ -6626,8 +6645,8 @@
       <c r="E208" s="30">
         <v>4692674.3839999996</v>
       </c>
-      <c r="F208" s="57"/>
-      <c r="G208" s="57"/>
+      <c r="F208" s="88"/>
+      <c r="G208" s="88"/>
       <c r="H208" s="40" t="s">
         <v>8</v>
       </c>
@@ -6647,8 +6666,8 @@
       <c r="E209" s="30">
         <v>4692677.5640000002</v>
       </c>
-      <c r="F209" s="57"/>
-      <c r="G209" s="57"/>
+      <c r="F209" s="88"/>
+      <c r="G209" s="88"/>
       <c r="H209" s="40" t="s">
         <v>8</v>
       </c>
@@ -6668,8 +6687,8 @@
       <c r="E210" s="30">
         <v>4692679.0279999999</v>
       </c>
-      <c r="F210" s="57"/>
-      <c r="G210" s="57"/>
+      <c r="F210" s="88"/>
+      <c r="G210" s="88"/>
       <c r="H210" s="40" t="s">
         <v>8</v>
       </c>
@@ -6689,8 +6708,8 @@
       <c r="E211" s="30">
         <v>4692680.25</v>
       </c>
-      <c r="F211" s="57"/>
-      <c r="G211" s="57"/>
+      <c r="F211" s="88"/>
+      <c r="G211" s="88"/>
       <c r="H211" s="40" t="s">
         <v>8</v>
       </c>
@@ -6710,8 +6729,8 @@
       <c r="E212" s="30">
         <v>4692673.0663999999</v>
       </c>
-      <c r="F212" s="57"/>
-      <c r="G212" s="57"/>
+      <c r="F212" s="88"/>
+      <c r="G212" s="88"/>
       <c r="H212" s="40" t="s">
         <v>8</v>
       </c>
@@ -6731,8 +6750,8 @@
       <c r="E213" s="30">
         <v>4692675.5999999996</v>
       </c>
-      <c r="F213" s="57"/>
-      <c r="G213" s="57"/>
+      <c r="F213" s="88"/>
+      <c r="G213" s="88"/>
       <c r="H213" s="40" t="s">
         <v>8</v>
       </c>
@@ -6752,8 +6771,8 @@
       <c r="E214" s="30">
         <v>4692674.3310000002</v>
       </c>
-      <c r="F214" s="57"/>
-      <c r="G214" s="57"/>
+      <c r="F214" s="88"/>
+      <c r="G214" s="88"/>
       <c r="H214" s="40" t="s">
         <v>8</v>
       </c>
@@ -6773,8 +6792,8 @@
       <c r="E215" s="30">
         <v>4692675.5310000004</v>
       </c>
-      <c r="F215" s="57"/>
-      <c r="G215" s="57"/>
+      <c r="F215" s="88"/>
+      <c r="G215" s="88"/>
       <c r="H215" s="40" t="s">
         <v>8</v>
       </c>
@@ -6794,8 +6813,8 @@
       <c r="E216" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F216" s="57"/>
-      <c r="G216" s="57"/>
+      <c r="F216" s="88"/>
+      <c r="G216" s="88"/>
       <c r="H216" s="40" t="s">
         <v>8</v>
       </c>
@@ -6815,8 +6834,8 @@
       <c r="E217" s="30">
         <v>4692677.4869999997</v>
       </c>
-      <c r="F217" s="57"/>
-      <c r="G217" s="57"/>
+      <c r="F217" s="88"/>
+      <c r="G217" s="88"/>
       <c r="H217" s="40" t="s">
         <v>8</v>
       </c>
@@ -6836,8 +6855,8 @@
       <c r="E218" s="30">
         <v>4692678.7819999997</v>
       </c>
-      <c r="F218" s="57"/>
-      <c r="G218" s="57"/>
+      <c r="F218" s="88"/>
+      <c r="G218" s="88"/>
       <c r="H218" s="40" t="s">
         <v>8</v>
       </c>
@@ -6857,8 +6876,8 @@
       <c r="E219" s="30">
         <v>4692681.2970000003</v>
       </c>
-      <c r="F219" s="57"/>
-      <c r="G219" s="57"/>
+      <c r="F219" s="88"/>
+      <c r="G219" s="88"/>
       <c r="H219" s="40" t="s">
         <v>8</v>
       </c>
@@ -6878,8 +6897,8 @@
       <c r="E220" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F220" s="57"/>
-      <c r="G220" s="57"/>
+      <c r="F220" s="88"/>
+      <c r="G220" s="88"/>
       <c r="H220" s="40" t="s">
         <v>8</v>
       </c>
@@ -6899,8 +6918,8 @@
       <c r="E221" s="30">
         <v>4692687.1791000003</v>
       </c>
-      <c r="F221" s="57"/>
-      <c r="G221" s="57"/>
+      <c r="F221" s="88"/>
+      <c r="G221" s="88"/>
       <c r="H221" s="40" t="s">
         <v>8</v>
       </c>
@@ -6920,8 +6939,8 @@
       <c r="E222" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F222" s="57"/>
-      <c r="G222" s="57"/>
+      <c r="F222" s="88"/>
+      <c r="G222" s="88"/>
       <c r="H222" s="40" t="s">
         <v>8</v>
       </c>
@@ -6941,8 +6960,8 @@
       <c r="E223" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F223" s="57"/>
-      <c r="G223" s="57"/>
+      <c r="F223" s="88"/>
+      <c r="G223" s="88"/>
       <c r="H223" s="40" t="s">
         <v>8</v>
       </c>
@@ -6962,8 +6981,8 @@
       <c r="E224" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F224" s="57"/>
-      <c r="G224" s="57"/>
+      <c r="F224" s="88"/>
+      <c r="G224" s="88"/>
       <c r="H224" s="40" t="s">
         <v>8</v>
       </c>
@@ -6983,8 +7002,8 @@
       <c r="E225" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F225" s="57"/>
-      <c r="G225" s="57"/>
+      <c r="F225" s="88"/>
+      <c r="G225" s="88"/>
       <c r="H225" s="40" t="s">
         <v>8</v>
       </c>
@@ -7004,8 +7023,8 @@
       <c r="E226" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F226" s="57"/>
-      <c r="G226" s="57"/>
+      <c r="F226" s="88"/>
+      <c r="G226" s="88"/>
       <c r="H226" s="40" t="s">
         <v>8</v>
       </c>
@@ -7025,8 +7044,8 @@
       <c r="E227" s="30">
         <v>4692683.9784000004</v>
       </c>
-      <c r="F227" s="57"/>
-      <c r="G227" s="57"/>
+      <c r="F227" s="88"/>
+      <c r="G227" s="88"/>
       <c r="H227" s="40" t="s">
         <v>8</v>
       </c>
@@ -7046,8 +7065,8 @@
       <c r="E228" s="30">
         <v>4692680.5674000001</v>
       </c>
-      <c r="F228" s="57"/>
-      <c r="G228" s="57"/>
+      <c r="F228" s="88"/>
+      <c r="G228" s="88"/>
       <c r="H228" s="40" t="s">
         <v>8</v>
       </c>
@@ -7067,8 +7086,8 @@
       <c r="E229" s="30">
         <v>4692679.6714000003</v>
       </c>
-      <c r="F229" s="57"/>
-      <c r="G229" s="57"/>
+      <c r="F229" s="88"/>
+      <c r="G229" s="88"/>
       <c r="H229" s="40" t="s">
         <v>8</v>
       </c>
@@ -7088,8 +7107,8 @@
       <c r="E230" s="30">
         <v>4692687.4755999995</v>
       </c>
-      <c r="F230" s="57"/>
-      <c r="G230" s="57"/>
+      <c r="F230" s="88"/>
+      <c r="G230" s="88"/>
       <c r="H230" s="40" t="s">
         <v>8</v>
       </c>
@@ -7109,8 +7128,8 @@
       <c r="E231" s="30">
         <v>4692681.2410000004</v>
       </c>
-      <c r="F231" s="57"/>
-      <c r="G231" s="57"/>
+      <c r="F231" s="88"/>
+      <c r="G231" s="88"/>
       <c r="H231" s="40" t="s">
         <v>8</v>
       </c>
@@ -7130,8 +7149,8 @@
       <c r="E232" s="30">
         <v>4692682.2426000005</v>
       </c>
-      <c r="F232" s="57"/>
-      <c r="G232" s="57"/>
+      <c r="F232" s="88"/>
+      <c r="G232" s="88"/>
       <c r="H232" s="40" t="s">
         <v>8</v>
       </c>
@@ -7151,8 +7170,8 @@
       <c r="E233" s="30">
         <v>4692688.4773000004</v>
       </c>
-      <c r="F233" s="57"/>
-      <c r="G233" s="57"/>
+      <c r="F233" s="88"/>
+      <c r="G233" s="88"/>
       <c r="H233" s="40" t="s">
         <v>8</v>
       </c>
@@ -7172,8 +7191,8 @@
       <c r="E234" s="30">
         <v>4692689.9908999996</v>
       </c>
-      <c r="F234" s="57"/>
-      <c r="G234" s="57"/>
+      <c r="F234" s="88"/>
+      <c r="G234" s="88"/>
       <c r="H234" s="40" t="s">
         <v>8</v>
       </c>
@@ -7193,8 +7212,8 @@
       <c r="E235" s="30">
         <v>4692683.7561999997</v>
       </c>
-      <c r="F235" s="57"/>
-      <c r="G235" s="57"/>
+      <c r="F235" s="88"/>
+      <c r="G235" s="88"/>
       <c r="H235" s="40" t="s">
         <v>8</v>
       </c>
@@ -7214,8 +7233,8 @@
       <c r="E236" s="30">
         <v>4692685.3595000003</v>
       </c>
-      <c r="F236" s="57"/>
-      <c r="G236" s="57"/>
+      <c r="F236" s="88"/>
+      <c r="G236" s="88"/>
       <c r="H236" s="40" t="s">
         <v>8</v>
       </c>
@@ -7235,8 +7254,8 @@
       <c r="E237" s="30">
         <v>4692691.5941000003</v>
       </c>
-      <c r="F237" s="57"/>
-      <c r="G237" s="57"/>
+      <c r="F237" s="88"/>
+      <c r="G237" s="88"/>
       <c r="H237" s="40" t="s">
         <v>8</v>
       </c>
@@ -7256,8 +7275,8 @@
       <c r="E238" s="30">
         <v>4692693.0789000001</v>
       </c>
-      <c r="F238" s="57"/>
-      <c r="G238" s="57"/>
+      <c r="F238" s="88"/>
+      <c r="G238" s="88"/>
       <c r="H238" s="40" t="s">
         <v>8</v>
       </c>
@@ -7277,8 +7296,8 @@
       <c r="E239" s="30">
         <v>4692686.8443</v>
       </c>
-      <c r="F239" s="57"/>
-      <c r="G239" s="57"/>
+      <c r="F239" s="88"/>
+      <c r="G239" s="88"/>
       <c r="H239" s="40" t="s">
         <v>8</v>
       </c>
@@ -7298,8 +7317,8 @@
       <c r="E240" s="30">
         <v>4692689.7762000002</v>
       </c>
-      <c r="F240" s="57"/>
-      <c r="G240" s="57"/>
+      <c r="F240" s="88"/>
+      <c r="G240" s="88"/>
       <c r="H240" s="40" t="s">
         <v>8</v>
       </c>
@@ -7319,8 +7338,8 @@
       <c r="E241" s="30">
         <v>4692687.6679999996</v>
       </c>
-      <c r="F241" s="57"/>
-      <c r="G241" s="57"/>
+      <c r="F241" s="88"/>
+      <c r="G241" s="88"/>
       <c r="H241" s="40" t="s">
         <v>8</v>
       </c>
@@ -7340,8 +7359,8 @@
       <c r="E242" s="30">
         <v>4692690.4787999997</v>
       </c>
-      <c r="F242" s="57"/>
-      <c r="G242" s="57"/>
+      <c r="F242" s="88"/>
+      <c r="G242" s="88"/>
       <c r="H242" s="40" t="s">
         <v>8</v>
       </c>
@@ -7361,8 +7380,8 @@
       <c r="E243" s="30">
         <v>4692688.38</v>
       </c>
-      <c r="F243" s="57"/>
-      <c r="G243" s="57"/>
+      <c r="F243" s="88"/>
+      <c r="G243" s="88"/>
       <c r="H243" s="40" t="s">
         <v>8</v>
       </c>
@@ -7382,8 +7401,8 @@
       <c r="E244" s="30">
         <v>4692685.5033</v>
       </c>
-      <c r="F244" s="57"/>
-      <c r="G244" s="57"/>
+      <c r="F244" s="88"/>
+      <c r="G244" s="88"/>
       <c r="H244" s="40" t="s">
         <v>8</v>
       </c>
@@ -7403,8 +7422,8 @@
       <c r="E245" s="30">
         <v>4692686.4769000001</v>
       </c>
-      <c r="F245" s="57"/>
-      <c r="G245" s="57"/>
+      <c r="F245" s="88"/>
+      <c r="G245" s="88"/>
       <c r="H245" s="40" t="s">
         <v>8</v>
       </c>
@@ -7424,8 +7443,8 @@
       <c r="E246" s="30">
         <v>4692680.3293000003</v>
       </c>
-      <c r="F246" s="57"/>
-      <c r="G246" s="57"/>
+      <c r="F246" s="88"/>
+      <c r="G246" s="88"/>
       <c r="H246" s="40" t="s">
         <v>8</v>
       </c>
@@ -7445,8 +7464,8 @@
       <c r="E247" s="30">
         <v>4692685.9365999997</v>
       </c>
-      <c r="F247" s="57"/>
-      <c r="G247" s="57"/>
+      <c r="F247" s="88"/>
+      <c r="G247" s="88"/>
       <c r="H247" s="40" t="s">
         <v>8</v>
       </c>
@@ -7466,8 +7485,8 @@
       <c r="E248" s="30">
         <v>4692684.2878</v>
       </c>
-      <c r="F248" s="57"/>
-      <c r="G248" s="57"/>
+      <c r="F248" s="88"/>
+      <c r="G248" s="88"/>
       <c r="H248" s="40" t="s">
         <v>8</v>
       </c>
@@ -7487,8 +7506,8 @@
       <c r="E249" s="30">
         <v>4692677.3678000001</v>
       </c>
-      <c r="F249" s="57"/>
-      <c r="G249" s="57"/>
+      <c r="F249" s="88"/>
+      <c r="G249" s="88"/>
       <c r="H249" s="40" t="s">
         <v>8</v>
       </c>
@@ -7508,8 +7527,8 @@
       <c r="E250" s="30">
         <v>4692675.551</v>
       </c>
-      <c r="F250" s="57"/>
-      <c r="G250" s="57"/>
+      <c r="F250" s="88"/>
+      <c r="G250" s="88"/>
       <c r="H250" s="40" t="s">
         <v>8</v>
       </c>
@@ -7529,8 +7548,8 @@
       <c r="E251" s="30">
         <v>4692682.6838999996</v>
       </c>
-      <c r="F251" s="57"/>
-      <c r="G251" s="57"/>
+      <c r="F251" s="88"/>
+      <c r="G251" s="88"/>
       <c r="H251" s="40" t="s">
         <v>8</v>
       </c>
@@ -7550,8 +7569,8 @@
       <c r="E252" s="30">
         <v>4692681.1698000003</v>
       </c>
-      <c r="F252" s="57"/>
-      <c r="G252" s="57"/>
+      <c r="F252" s="88"/>
+      <c r="G252" s="88"/>
       <c r="H252" s="40" t="s">
         <v>8</v>
       </c>
@@ -7569,8 +7588,8 @@
       <c r="E253" s="30">
         <v>4692679.5367999999</v>
       </c>
-      <c r="F253" s="57"/>
-      <c r="G253" s="57"/>
+      <c r="F253" s="88"/>
+      <c r="G253" s="88"/>
       <c r="H253" s="40" t="s">
         <v>8</v>
       </c>
@@ -7585,8 +7604,8 @@
       <c r="E254" s="30">
         <v>4692678.6008000001</v>
       </c>
-      <c r="F254" s="57"/>
-      <c r="G254" s="57"/>
+      <c r="F254" s="88"/>
+      <c r="G254" s="88"/>
       <c r="H254" s="40" t="s">
         <v>8</v>
       </c>
@@ -7603,8 +7622,8 @@
       <c r="E255" s="30">
         <v>4692673.9884000001</v>
       </c>
-      <c r="F255" s="57"/>
-      <c r="G255" s="57"/>
+      <c r="F255" s="88"/>
+      <c r="G255" s="88"/>
       <c r="H255" s="40" t="s">
         <v>8</v>
       </c>
@@ -7624,8 +7643,8 @@
       <c r="E256" s="42">
         <v>4692673.2940999996</v>
       </c>
-      <c r="F256" s="58"/>
-      <c r="G256" s="58"/>
+      <c r="F256" s="89"/>
+      <c r="G256" s="89"/>
       <c r="H256" s="43" t="s">
         <v>20</v>
       </c>
@@ -7640,34 +7659,34 @@
       <c r="B257" s="3"/>
       <c r="C257" s="35"/>
       <c r="D257" s="35"/>
-      <c r="E257" s="83" t="s">
+      <c r="E257" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="F257" s="84"/>
-      <c r="G257" s="85"/>
-      <c r="H257" s="82" t="s">
+      <c r="F257" s="85"/>
+      <c r="G257" s="86"/>
+      <c r="H257" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="I257" s="64"/>
-      <c r="J257" s="67"/>
-      <c r="K257" s="68"/>
+      <c r="I257" s="70"/>
+      <c r="J257" s="73"/>
+      <c r="K257" s="74"/>
     </row>
     <row r="258" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A258" s="71" t="s">
+      <c r="A258" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B258" s="72"/>
-      <c r="C258" s="72"/>
-      <c r="D258" s="73"/>
-      <c r="E258" s="74">
+      <c r="B258" s="78"/>
+      <c r="C258" s="78"/>
+      <c r="D258" s="79"/>
+      <c r="E258" s="80">
         <v>140</v>
       </c>
-      <c r="F258" s="75"/>
-      <c r="G258" s="76"/>
-      <c r="H258" s="65"/>
-      <c r="I258" s="66"/>
-      <c r="J258" s="69"/>
-      <c r="K258" s="70"/>
+      <c r="F258" s="81"/>
+      <c r="G258" s="82"/>
+      <c r="H258" s="71"/>
+      <c r="I258" s="72"/>
+      <c r="J258" s="75"/>
+      <c r="K258" s="76"/>
     </row>
     <row r="259" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A259" s="1"/>
@@ -7683,118 +7702,118 @@
       <c r="K259" s="1"/>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A260" s="48"/>
-      <c r="B260" s="48"/>
-      <c r="C260" s="48"/>
-      <c r="D260" s="48"/>
-      <c r="E260" s="48"/>
-      <c r="F260" s="48"/>
-      <c r="G260" s="48"/>
-      <c r="H260" s="48"/>
-      <c r="I260" s="48"/>
-      <c r="J260" s="48"/>
-      <c r="K260" s="48"/>
+      <c r="A260" s="51"/>
+      <c r="B260" s="51"/>
+      <c r="C260" s="51"/>
+      <c r="D260" s="51"/>
+      <c r="E260" s="51"/>
+      <c r="F260" s="51"/>
+      <c r="G260" s="51"/>
+      <c r="H260" s="51"/>
+      <c r="I260" s="51"/>
+      <c r="J260" s="51"/>
+      <c r="K260" s="51"/>
     </row>
     <row r="261" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="48"/>
-      <c r="B261" s="48"/>
-      <c r="C261" s="48"/>
-      <c r="D261" s="48"/>
-      <c r="E261" s="48"/>
-      <c r="F261" s="48"/>
-      <c r="G261" s="48"/>
-      <c r="H261" s="48"/>
-      <c r="I261" s="48"/>
-      <c r="J261" s="48"/>
-      <c r="K261" s="48"/>
+      <c r="A261" s="51"/>
+      <c r="B261" s="51"/>
+      <c r="C261" s="51"/>
+      <c r="D261" s="51"/>
+      <c r="E261" s="51"/>
+      <c r="F261" s="51"/>
+      <c r="G261" s="51"/>
+      <c r="H261" s="51"/>
+      <c r="I261" s="51"/>
+      <c r="J261" s="51"/>
+      <c r="K261" s="51"/>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A262" s="49" t="s">
+      <c r="A262" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B262" s="49"/>
-      <c r="C262" s="49"/>
-      <c r="D262" s="49"/>
-      <c r="E262" s="49"/>
-      <c r="F262" s="49"/>
-      <c r="G262" s="49"/>
-      <c r="H262" s="49"/>
-      <c r="I262" s="49"/>
-      <c r="J262" s="49"/>
-      <c r="K262" s="49"/>
+      <c r="B262" s="52"/>
+      <c r="C262" s="52"/>
+      <c r="D262" s="52"/>
+      <c r="E262" s="52"/>
+      <c r="F262" s="52"/>
+      <c r="G262" s="52"/>
+      <c r="H262" s="52"/>
+      <c r="I262" s="52"/>
+      <c r="J262" s="52"/>
+      <c r="K262" s="52"/>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A263" s="49"/>
-      <c r="B263" s="49"/>
-      <c r="C263" s="49"/>
-      <c r="D263" s="49"/>
-      <c r="E263" s="49"/>
-      <c r="F263" s="49"/>
-      <c r="G263" s="49"/>
-      <c r="H263" s="49"/>
-      <c r="I263" s="49"/>
-      <c r="J263" s="49"/>
-      <c r="K263" s="49"/>
+      <c r="A263" s="52"/>
+      <c r="B263" s="52"/>
+      <c r="C263" s="52"/>
+      <c r="D263" s="52"/>
+      <c r="E263" s="52"/>
+      <c r="F263" s="52"/>
+      <c r="G263" s="52"/>
+      <c r="H263" s="52"/>
+      <c r="I263" s="52"/>
+      <c r="J263" s="52"/>
+      <c r="K263" s="52"/>
     </row>
     <row r="264" spans="1:11" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="49"/>
-      <c r="B264" s="49"/>
-      <c r="C264" s="49"/>
-      <c r="D264" s="49"/>
-      <c r="E264" s="49"/>
-      <c r="F264" s="49"/>
-      <c r="G264" s="49"/>
-      <c r="H264" s="49"/>
-      <c r="I264" s="49"/>
-      <c r="J264" s="49"/>
-      <c r="K264" s="49"/>
+      <c r="A264" s="52"/>
+      <c r="B264" s="52"/>
+      <c r="C264" s="52"/>
+      <c r="D264" s="52"/>
+      <c r="E264" s="52"/>
+      <c r="F264" s="52"/>
+      <c r="G264" s="52"/>
+      <c r="H264" s="52"/>
+      <c r="I264" s="52"/>
+      <c r="J264" s="52"/>
+      <c r="K264" s="52"/>
     </row>
     <row r="265" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="49"/>
-      <c r="B265" s="49"/>
-      <c r="C265" s="49"/>
-      <c r="D265" s="49"/>
-      <c r="E265" s="49"/>
-      <c r="F265" s="49"/>
-      <c r="G265" s="49"/>
-      <c r="H265" s="49"/>
-      <c r="I265" s="49"/>
-      <c r="J265" s="49"/>
-      <c r="K265" s="49"/>
+      <c r="A265" s="52"/>
+      <c r="B265" s="52"/>
+      <c r="C265" s="52"/>
+      <c r="D265" s="52"/>
+      <c r="E265" s="52"/>
+      <c r="F265" s="52"/>
+      <c r="G265" s="52"/>
+      <c r="H265" s="52"/>
+      <c r="I265" s="52"/>
+      <c r="J265" s="52"/>
+      <c r="K265" s="52"/>
     </row>
     <row r="266" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A266" s="1"/>
-      <c r="C266" s="50"/>
-      <c r="D266" s="51"/>
-      <c r="E266" s="51"/>
-      <c r="F266" s="51"/>
-      <c r="G266" s="51"/>
-      <c r="H266" s="51"/>
-      <c r="I266" s="52"/>
+      <c r="C266" s="53"/>
+      <c r="D266" s="54"/>
+      <c r="E266" s="54"/>
+      <c r="F266" s="54"/>
+      <c r="G266" s="54"/>
+      <c r="H266" s="54"/>
+      <c r="I266" s="55"/>
       <c r="J266" s="1"/>
       <c r="K266" s="1"/>
     </row>
     <row r="267" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A267" s="1"/>
-      <c r="C267" s="53"/>
-      <c r="D267" s="54"/>
-      <c r="E267" s="54"/>
-      <c r="F267" s="54"/>
-      <c r="G267" s="54"/>
-      <c r="H267" s="54"/>
-      <c r="I267" s="55"/>
+      <c r="C267" s="56"/>
+      <c r="D267" s="57"/>
+      <c r="E267" s="57"/>
+      <c r="F267" s="57"/>
+      <c r="G267" s="57"/>
+      <c r="H267" s="57"/>
+      <c r="I267" s="58"/>
       <c r="J267" s="1"/>
       <c r="K267" s="1"/>
     </row>
     <row r="268" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A268" s="1"/>
-      <c r="C268" s="77"/>
-      <c r="D268" s="78"/>
-      <c r="E268" s="78"/>
-      <c r="F268" s="78"/>
-      <c r="G268" s="78"/>
-      <c r="H268" s="78"/>
-      <c r="I268" s="56"/>
+      <c r="C268" s="59"/>
+      <c r="D268" s="60"/>
+      <c r="E268" s="60"/>
+      <c r="F268" s="60"/>
+      <c r="G268" s="60"/>
+      <c r="H268" s="60"/>
+      <c r="I268" s="61"/>
       <c r="J268" s="1"/>
       <c r="K268" s="1"/>
     </row>
@@ -7848,10 +7867,10 @@
       <c r="E271" s="30">
         <v>4692673.5029999996</v>
       </c>
-      <c r="F271" s="79">
+      <c r="F271" s="48">
         <v>625.72</v>
       </c>
-      <c r="G271" s="86" t="s">
+      <c r="G271" s="63" t="s">
         <v>25</v>
       </c>
       <c r="H271" s="45" t="s">
@@ -7873,8 +7892,8 @@
       <c r="E272" s="30">
         <v>4692672.9689999996</v>
       </c>
-      <c r="F272" s="80"/>
-      <c r="G272" s="87"/>
+      <c r="F272" s="49"/>
+      <c r="G272" s="64"/>
       <c r="H272" s="45" t="s">
         <v>8</v>
       </c>
@@ -7894,8 +7913,8 @@
       <c r="E273" s="30">
         <v>4692672.7319999998</v>
       </c>
-      <c r="F273" s="80"/>
-      <c r="G273" s="87"/>
+      <c r="F273" s="49"/>
+      <c r="G273" s="64"/>
       <c r="H273" s="45" t="s">
         <v>8</v>
       </c>
@@ -7915,8 +7934,8 @@
       <c r="E274" s="30">
         <v>4692672.7970000003</v>
       </c>
-      <c r="F274" s="80"/>
-      <c r="G274" s="87"/>
+      <c r="F274" s="49"/>
+      <c r="G274" s="64"/>
       <c r="H274" s="45" t="s">
         <v>8</v>
       </c>
@@ -7936,8 +7955,8 @@
       <c r="E275" s="30">
         <v>4692674.3839999996</v>
       </c>
-      <c r="F275" s="80"/>
-      <c r="G275" s="87"/>
+      <c r="F275" s="49"/>
+      <c r="G275" s="64"/>
       <c r="H275" s="45" t="s">
         <v>8</v>
       </c>
@@ -7957,8 +7976,8 @@
       <c r="E276" s="30">
         <v>4692677.5640000002</v>
       </c>
-      <c r="F276" s="80"/>
-      <c r="G276" s="87"/>
+      <c r="F276" s="49"/>
+      <c r="G276" s="64"/>
       <c r="H276" s="45" t="s">
         <v>8</v>
       </c>
@@ -7978,8 +7997,8 @@
       <c r="E277" s="30">
         <v>4692679.0279999999</v>
       </c>
-      <c r="F277" s="80"/>
-      <c r="G277" s="87"/>
+      <c r="F277" s="49"/>
+      <c r="G277" s="64"/>
       <c r="H277" s="45" t="s">
         <v>8</v>
       </c>
@@ -7999,8 +8018,8 @@
       <c r="E278" s="30">
         <v>4692680.25</v>
       </c>
-      <c r="F278" s="80"/>
-      <c r="G278" s="87"/>
+      <c r="F278" s="49"/>
+      <c r="G278" s="64"/>
       <c r="H278" s="45" t="s">
         <v>8</v>
       </c>
@@ -8020,8 +8039,8 @@
       <c r="E279" s="30">
         <v>4692673.0663999999</v>
       </c>
-      <c r="F279" s="80"/>
-      <c r="G279" s="87"/>
+      <c r="F279" s="49"/>
+      <c r="G279" s="64"/>
       <c r="H279" s="45" t="s">
         <v>8</v>
       </c>
@@ -8041,8 +8060,8 @@
       <c r="E280" s="30">
         <v>4692675.5999999996</v>
       </c>
-      <c r="F280" s="80"/>
-      <c r="G280" s="87"/>
+      <c r="F280" s="49"/>
+      <c r="G280" s="64"/>
       <c r="H280" s="45" t="s">
         <v>8</v>
       </c>
@@ -8062,8 +8081,8 @@
       <c r="E281" s="30">
         <v>4692674.3310000002</v>
       </c>
-      <c r="F281" s="80"/>
-      <c r="G281" s="87"/>
+      <c r="F281" s="49"/>
+      <c r="G281" s="64"/>
       <c r="H281" s="45" t="s">
         <v>8</v>
       </c>
@@ -8083,8 +8102,8 @@
       <c r="E282" s="30">
         <v>4692675.5310000004</v>
       </c>
-      <c r="F282" s="80"/>
-      <c r="G282" s="87"/>
+      <c r="F282" s="49"/>
+      <c r="G282" s="64"/>
       <c r="H282" s="45" t="s">
         <v>8</v>
       </c>
@@ -8104,8 +8123,8 @@
       <c r="E283" s="30">
         <v>4692685.9060000004</v>
       </c>
-      <c r="F283" s="80"/>
-      <c r="G283" s="87"/>
+      <c r="F283" s="49"/>
+      <c r="G283" s="64"/>
       <c r="H283" s="45" t="s">
         <v>8</v>
       </c>
@@ -8125,8 +8144,8 @@
       <c r="E284" s="30">
         <v>4692677.4869999997</v>
       </c>
-      <c r="F284" s="80"/>
-      <c r="G284" s="87"/>
+      <c r="F284" s="49"/>
+      <c r="G284" s="64"/>
       <c r="H284" s="45" t="s">
         <v>8</v>
       </c>
@@ -8146,8 +8165,8 @@
       <c r="E285" s="30">
         <v>4692678.7819999997</v>
       </c>
-      <c r="F285" s="80"/>
-      <c r="G285" s="87"/>
+      <c r="F285" s="49"/>
+      <c r="G285" s="64"/>
       <c r="H285" s="45" t="s">
         <v>8</v>
       </c>
@@ -8167,8 +8186,8 @@
       <c r="E286" s="30">
         <v>4692681.2970000003</v>
       </c>
-      <c r="F286" s="80"/>
-      <c r="G286" s="87"/>
+      <c r="F286" s="49"/>
+      <c r="G286" s="64"/>
       <c r="H286" s="45" t="s">
         <v>8</v>
       </c>
@@ -8188,8 +8207,8 @@
       <c r="E287" s="30">
         <v>4692686.5060000001</v>
       </c>
-      <c r="F287" s="80"/>
-      <c r="G287" s="87"/>
+      <c r="F287" s="49"/>
+      <c r="G287" s="64"/>
       <c r="H287" s="45" t="s">
         <v>8</v>
       </c>
@@ -8209,8 +8228,8 @@
       <c r="E288" s="30">
         <v>4692687.1791000003</v>
       </c>
-      <c r="F288" s="80"/>
-      <c r="G288" s="87"/>
+      <c r="F288" s="49"/>
+      <c r="G288" s="64"/>
       <c r="H288" s="45" t="s">
         <v>8</v>
       </c>
@@ -8230,8 +8249,8 @@
       <c r="E289" s="30">
         <v>4692688.1239999998</v>
       </c>
-      <c r="F289" s="80"/>
-      <c r="G289" s="87"/>
+      <c r="F289" s="49"/>
+      <c r="G289" s="64"/>
       <c r="H289" s="45" t="s">
         <v>8</v>
       </c>
@@ -8251,8 +8270,8 @@
       <c r="E290" s="30">
         <v>4692694.1169999996</v>
       </c>
-      <c r="F290" s="80"/>
-      <c r="G290" s="87"/>
+      <c r="F290" s="49"/>
+      <c r="G290" s="64"/>
       <c r="H290" s="45" t="s">
         <v>8</v>
       </c>
@@ -8272,8 +8291,8 @@
       <c r="E291" s="30">
         <v>4692693.4919999996</v>
       </c>
-      <c r="F291" s="80"/>
-      <c r="G291" s="87"/>
+      <c r="F291" s="49"/>
+      <c r="G291" s="64"/>
       <c r="H291" s="45" t="s">
         <v>8</v>
       </c>
@@ -8293,8 +8312,8 @@
       <c r="E292" s="30">
         <v>4692694.1579999998</v>
       </c>
-      <c r="F292" s="80"/>
-      <c r="G292" s="87"/>
+      <c r="F292" s="49"/>
+      <c r="G292" s="64"/>
       <c r="H292" s="45" t="s">
         <v>8</v>
       </c>
@@ -8314,8 +8333,8 @@
       <c r="E293" s="30">
         <v>4692689.9910000004</v>
       </c>
-      <c r="F293" s="80"/>
-      <c r="G293" s="87"/>
+      <c r="F293" s="49"/>
+      <c r="G293" s="64"/>
       <c r="H293" s="45" t="s">
         <v>8</v>
       </c>
@@ -8335,8 +8354,8 @@
       <c r="E294" s="30">
         <v>4692691.5941000003</v>
       </c>
-      <c r="F294" s="80"/>
-      <c r="G294" s="87"/>
+      <c r="F294" s="49"/>
+      <c r="G294" s="64"/>
       <c r="H294" s="45" t="s">
         <v>8</v>
       </c>
@@ -8356,8 +8375,8 @@
       <c r="E295" s="30">
         <v>4692685.3595000003</v>
       </c>
-      <c r="F295" s="80"/>
-      <c r="G295" s="87"/>
+      <c r="F295" s="49"/>
+      <c r="G295" s="64"/>
       <c r="H295" s="45" t="s">
         <v>8</v>
       </c>
@@ -8377,8 +8396,8 @@
       <c r="E296" s="30">
         <v>4692683.7562999995</v>
       </c>
-      <c r="F296" s="80"/>
-      <c r="G296" s="87"/>
+      <c r="F296" s="49"/>
+      <c r="G296" s="64"/>
       <c r="H296" s="45" t="s">
         <v>8</v>
       </c>
@@ -8398,8 +8417,8 @@
       <c r="E297" s="30">
         <v>4692680.5674000001</v>
       </c>
-      <c r="F297" s="80"/>
-      <c r="G297" s="87"/>
+      <c r="F297" s="49"/>
+      <c r="G297" s="64"/>
       <c r="H297" s="45" t="s">
         <v>8</v>
       </c>
@@ -8419,8 +8438,8 @@
       <c r="E298" s="30">
         <v>4692683.9784000004</v>
       </c>
-      <c r="F298" s="80"/>
-      <c r="G298" s="87"/>
+      <c r="F298" s="49"/>
+      <c r="G298" s="64"/>
       <c r="H298" s="45" t="s">
         <v>8</v>
       </c>
@@ -8440,8 +8459,8 @@
       <c r="E299" s="30">
         <v>4692683.0823999997</v>
       </c>
-      <c r="F299" s="80"/>
-      <c r="G299" s="87"/>
+      <c r="F299" s="49"/>
+      <c r="G299" s="64"/>
       <c r="H299" s="45" t="s">
         <v>8</v>
       </c>
@@ -8461,8 +8480,8 @@
       <c r="E300" s="30">
         <v>4692679.6714000003</v>
       </c>
-      <c r="F300" s="80"/>
-      <c r="G300" s="87"/>
+      <c r="F300" s="49"/>
+      <c r="G300" s="64"/>
       <c r="H300" s="45" t="s">
         <v>8</v>
       </c>
@@ -8482,8 +8501,8 @@
       <c r="E301" s="30">
         <v>4692678.2399000004</v>
       </c>
-      <c r="F301" s="80"/>
-      <c r="G301" s="87"/>
+      <c r="F301" s="49"/>
+      <c r="G301" s="64"/>
       <c r="H301" s="45" t="s">
         <v>8</v>
       </c>
@@ -8503,8 +8522,8 @@
       <c r="E302" s="30">
         <v>4692682.3244000003</v>
       </c>
-      <c r="F302" s="80"/>
-      <c r="G302" s="87"/>
+      <c r="F302" s="49"/>
+      <c r="G302" s="64"/>
       <c r="H302" s="45" t="s">
         <v>8</v>
       </c>
@@ -8524,8 +8543,8 @@
       <c r="E303" s="30">
         <v>4692683.8091000002</v>
       </c>
-      <c r="F303" s="80"/>
-      <c r="G303" s="87"/>
+      <c r="F303" s="49"/>
+      <c r="G303" s="64"/>
       <c r="H303" s="45" t="s">
         <v>8</v>
       </c>
@@ -8545,8 +8564,8 @@
       <c r="E304" s="30">
         <v>4692683.9275000002</v>
       </c>
-      <c r="F304" s="80"/>
-      <c r="G304" s="87"/>
+      <c r="F304" s="49"/>
+      <c r="G304" s="64"/>
       <c r="H304" s="45" t="s">
         <v>8</v>
       </c>
@@ -8566,8 +8585,8 @@
       <c r="E305" s="30">
         <v>4692686.4386999998</v>
       </c>
-      <c r="F305" s="80"/>
-      <c r="G305" s="87"/>
+      <c r="F305" s="49"/>
+      <c r="G305" s="64"/>
       <c r="H305" s="45" t="s">
         <v>8</v>
       </c>
@@ -8587,8 +8606,8 @@
       <c r="E306" s="30">
         <v>4692675.5519000003</v>
       </c>
-      <c r="F306" s="81"/>
-      <c r="G306" s="87"/>
+      <c r="F306" s="50"/>
+      <c r="G306" s="64"/>
       <c r="H306" s="45" t="s">
         <v>8</v>
       </c>
@@ -8611,7 +8630,7 @@
       <c r="F307" s="34">
         <v>616.38300000000004</v>
       </c>
-      <c r="G307" s="88"/>
+      <c r="G307" s="65"/>
       <c r="H307" s="45" t="s">
         <v>20</v>
       </c>
@@ -8635,28 +8654,28 @@
     <row r="309" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A309" s="1"/>
       <c r="B309" s="33"/>
-      <c r="C309" s="59" t="s">
+      <c r="C309" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D309" s="59"/>
-      <c r="E309" s="59"/>
-      <c r="F309" s="59"/>
-      <c r="G309" s="59"/>
-      <c r="H309" s="59"/>
-      <c r="I309" s="59"/>
+      <c r="D309" s="62"/>
+      <c r="E309" s="62"/>
+      <c r="F309" s="62"/>
+      <c r="G309" s="62"/>
+      <c r="H309" s="62"/>
+      <c r="I309" s="62"/>
       <c r="J309" s="1"/>
       <c r="K309" s="1"/>
     </row>
     <row r="310" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A310" s="1"/>
       <c r="B310" s="33"/>
-      <c r="C310" s="59"/>
-      <c r="D310" s="59"/>
-      <c r="E310" s="59"/>
-      <c r="F310" s="59"/>
-      <c r="G310" s="59"/>
-      <c r="H310" s="59"/>
-      <c r="I310" s="59"/>
+      <c r="C310" s="62"/>
+      <c r="D310" s="62"/>
+      <c r="E310" s="62"/>
+      <c r="F310" s="62"/>
+      <c r="G310" s="62"/>
+      <c r="H310" s="62"/>
+      <c r="I310" s="62"/>
       <c r="J310" s="1"/>
       <c r="K310" s="1"/>
     </row>
@@ -8732,47 +8751,53 @@
       <c r="B316" s="3"/>
       <c r="C316" s="3"/>
       <c r="D316" s="3"/>
-      <c r="E316" s="60" t="s">
+      <c r="E316" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="F316" s="61"/>
-      <c r="G316" s="62"/>
-      <c r="H316" s="63" t="s">
+      <c r="F316" s="67"/>
+      <c r="G316" s="68"/>
+      <c r="H316" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="I316" s="64"/>
-      <c r="J316" s="67"/>
-      <c r="K316" s="68"/>
+      <c r="I316" s="70"/>
+      <c r="J316" s="73"/>
+      <c r="K316" s="74"/>
     </row>
     <row r="317" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A317" s="71" t="s">
+      <c r="A317" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B317" s="72"/>
-      <c r="C317" s="72"/>
-      <c r="D317" s="73"/>
-      <c r="E317" s="74">
+      <c r="B317" s="78"/>
+      <c r="C317" s="78"/>
+      <c r="D317" s="79"/>
+      <c r="E317" s="80">
         <v>140</v>
       </c>
-      <c r="F317" s="75"/>
-      <c r="G317" s="76"/>
-      <c r="H317" s="65"/>
-      <c r="I317" s="66"/>
-      <c r="J317" s="69"/>
-      <c r="K317" s="70"/>
+      <c r="F317" s="81"/>
+      <c r="G317" s="82"/>
+      <c r="H317" s="71"/>
+      <c r="I317" s="72"/>
+      <c r="J317" s="75"/>
+      <c r="K317" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G77:G112"/>
-    <mergeCell ref="F77:F112"/>
-    <mergeCell ref="A260:K261"/>
-    <mergeCell ref="A262:K265"/>
-    <mergeCell ref="C266:I268"/>
-    <mergeCell ref="C309:I310"/>
-    <mergeCell ref="G271:G307"/>
-    <mergeCell ref="F271:F306"/>
-    <mergeCell ref="E316:G316"/>
-    <mergeCell ref="H316:I317"/>
+    <mergeCell ref="J192:K193"/>
+    <mergeCell ref="A193:D193"/>
+    <mergeCell ref="E193:G193"/>
+    <mergeCell ref="C120:I121"/>
+    <mergeCell ref="A66:K67"/>
+    <mergeCell ref="G144:G181"/>
+    <mergeCell ref="C7:I9"/>
+    <mergeCell ref="A3:K6"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="B61:H62"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:I65"/>
+    <mergeCell ref="J64:K65"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="G36:G55"/>
     <mergeCell ref="J316:K317"/>
     <mergeCell ref="A317:D317"/>
     <mergeCell ref="E317:G317"/>
@@ -8784,37 +8809,31 @@
     <mergeCell ref="E258:G258"/>
     <mergeCell ref="J257:K258"/>
     <mergeCell ref="A134:K137"/>
-    <mergeCell ref="G144:G178"/>
     <mergeCell ref="H128:I129"/>
     <mergeCell ref="J128:K129"/>
     <mergeCell ref="A129:D129"/>
     <mergeCell ref="E129:G129"/>
+    <mergeCell ref="C309:I310"/>
+    <mergeCell ref="G271:G307"/>
+    <mergeCell ref="F271:F306"/>
+    <mergeCell ref="E316:G316"/>
+    <mergeCell ref="H316:I317"/>
+    <mergeCell ref="G77:G112"/>
+    <mergeCell ref="F77:F112"/>
+    <mergeCell ref="A260:K261"/>
+    <mergeCell ref="A262:K265"/>
+    <mergeCell ref="C266:I268"/>
     <mergeCell ref="A132:K133"/>
     <mergeCell ref="E128:G128"/>
     <mergeCell ref="C139:I141"/>
-    <mergeCell ref="C7:I9"/>
-    <mergeCell ref="A3:K6"/>
-    <mergeCell ref="A1:K2"/>
-    <mergeCell ref="B61:H62"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:I65"/>
-    <mergeCell ref="J64:K65"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="G36:G55"/>
     <mergeCell ref="A194:K195"/>
     <mergeCell ref="A196:K199"/>
     <mergeCell ref="C200:I202"/>
     <mergeCell ref="G204:G256"/>
     <mergeCell ref="F204:F256"/>
-    <mergeCell ref="C182:I183"/>
+    <mergeCell ref="C187:I188"/>
     <mergeCell ref="E192:G192"/>
     <mergeCell ref="H192:I193"/>
-    <mergeCell ref="J192:K193"/>
-    <mergeCell ref="A193:D193"/>
-    <mergeCell ref="E193:G193"/>
-    <mergeCell ref="C120:I121"/>
-    <mergeCell ref="A66:K67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>